<commit_message>
added ifo gdp component analysis preprocessing
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
@@ -369,13 +369,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ES224"/>
+  <dimension ref="A1:ET225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:149">
+    <row r="1" spans="1:150">
       <c r="B1" s="1">
         <v>32508</v>
       </c>
@@ -820,8 +820,11 @@
       <c r="ES1" s="1">
         <v>45891</v>
       </c>
+      <c r="ET1" s="1">
+        <v>45986</v>
+      </c>
     </row>
-    <row r="2" spans="1:149">
+    <row r="2" spans="1:150">
       <c r="A2" s="1">
         <v>25569</v>
       </c>
@@ -1269,8 +1272,11 @@
       <c r="ES2">
         <v>38.50631393048884</v>
       </c>
+      <c r="ET2">
+        <v>38.50631393048884</v>
+      </c>
     </row>
-    <row r="3" spans="1:149">
+    <row r="3" spans="1:150">
       <c r="A3" s="1">
         <v>25659</v>
       </c>
@@ -1718,8 +1724,11 @@
       <c r="ES3">
         <v>40.02695818027691</v>
       </c>
+      <c r="ET3">
+        <v>40.02695818027691</v>
+      </c>
     </row>
-    <row r="4" spans="1:149">
+    <row r="4" spans="1:150">
       <c r="A4" s="1">
         <v>25750</v>
       </c>
@@ -2167,8 +2176,11 @@
       <c r="ES4">
         <v>40.7772760666855</v>
       </c>
+      <c r="ET4">
+        <v>40.7772760666855</v>
+      </c>
     </row>
-    <row r="5" spans="1:149">
+    <row r="5" spans="1:150">
       <c r="A5" s="1">
         <v>25842</v>
       </c>
@@ -2616,8 +2628,11 @@
       <c r="ES5">
         <v>41.12742441367618</v>
       </c>
+      <c r="ET5">
+        <v>41.12742441367618</v>
+      </c>
     </row>
-    <row r="6" spans="1:149">
+    <row r="6" spans="1:150">
       <c r="A6" s="1">
         <v>25934</v>
       </c>
@@ -3065,8 +3080,11 @@
       <c r="ES6">
         <v>40.32708533484035</v>
       </c>
+      <c r="ET6">
+        <v>40.32708533484035</v>
+      </c>
     </row>
-    <row r="7" spans="1:149">
+    <row r="7" spans="1:150">
       <c r="A7" s="1">
         <v>26024</v>
       </c>
@@ -3514,8 +3532,11 @@
       <c r="ES7">
         <v>41.18744984458887</v>
       </c>
+      <c r="ET7">
+        <v>41.18744984458887</v>
+      </c>
     </row>
-    <row r="8" spans="1:149">
+    <row r="8" spans="1:150">
       <c r="A8" s="1">
         <v>26115</v>
       </c>
@@ -3963,8 +3984,11 @@
       <c r="ES8">
         <v>41.88774653857022</v>
       </c>
+      <c r="ET8">
+        <v>41.88774653857022</v>
+      </c>
     </row>
-    <row r="9" spans="1:149">
+    <row r="9" spans="1:150">
       <c r="A9" s="1">
         <v>26207</v>
       </c>
@@ -4412,8 +4436,11 @@
       <c r="ES9">
         <v>41.84772958462842</v>
       </c>
+      <c r="ET9">
+        <v>41.84772958462842</v>
+      </c>
     </row>
-    <row r="10" spans="1:149">
+    <row r="10" spans="1:150">
       <c r="A10" s="1">
         <v>26299</v>
       </c>
@@ -4861,8 +4888,11 @@
       <c r="ES10">
         <v>41.88774653857022</v>
       </c>
+      <c r="ET10">
+        <v>41.88774653857022</v>
+      </c>
     </row>
-    <row r="11" spans="1:149">
+    <row r="11" spans="1:150">
       <c r="A11" s="1">
         <v>26390</v>
       </c>
@@ -5310,8 +5340,11 @@
       <c r="ES11">
         <v>42.57803899406613</v>
       </c>
+      <c r="ET11">
+        <v>42.57803899406613</v>
+      </c>
     </row>
-    <row r="12" spans="1:149">
+    <row r="12" spans="1:150">
       <c r="A12" s="1">
         <v>26481</v>
       </c>
@@ -5759,8 +5792,11 @@
       <c r="ES12">
         <v>43.56845860412546</v>
       </c>
+      <c r="ET12">
+        <v>43.56845860412546</v>
+      </c>
     </row>
-    <row r="13" spans="1:149">
+    <row r="13" spans="1:150">
       <c r="A13" s="1">
         <v>26573</v>
       </c>
@@ -6208,8 +6244,11 @@
       <c r="ES13">
         <v>44.23874258265047</v>
       </c>
+      <c r="ET13">
+        <v>44.23874258265047</v>
+      </c>
     </row>
-    <row r="14" spans="1:149">
+    <row r="14" spans="1:150">
       <c r="A14" s="1">
         <v>26665</v>
       </c>
@@ -6657,8 +6696,11 @@
       <c r="ES14">
         <v>44.87901384571913</v>
       </c>
+      <c r="ET14">
+        <v>44.87901384571913</v>
+      </c>
     </row>
-    <row r="15" spans="1:149">
+    <row r="15" spans="1:150">
       <c r="A15" s="1">
         <v>26755</v>
       </c>
@@ -7106,8 +7148,11 @@
       <c r="ES15">
         <v>45.18914523876802</v>
       </c>
+      <c r="ET15">
+        <v>45.18914523876802</v>
+      </c>
     </row>
-    <row r="16" spans="1:149">
+    <row r="16" spans="1:150">
       <c r="A16" s="1">
         <v>26846</v>
       </c>
@@ -7555,8 +7600,11 @@
       <c r="ES16">
         <v>45.34921305453518</v>
       </c>
+      <c r="ET16">
+        <v>45.34921305453518</v>
+      </c>
     </row>
-    <row r="17" spans="1:149">
+    <row r="17" spans="1:150">
       <c r="A17" s="1">
         <v>26938</v>
       </c>
@@ -8004,8 +8052,11 @@
       <c r="ES17">
         <v>45.44925543938966</v>
       </c>
+      <c r="ET17">
+        <v>45.44925543938966</v>
+      </c>
     </row>
-    <row r="18" spans="1:149">
+    <row r="18" spans="1:150">
       <c r="A18" s="1">
         <v>27030</v>
       </c>
@@ -8453,8 +8504,11 @@
       <c r="ES18">
         <v>45.82941650183668</v>
       </c>
+      <c r="ET18">
+        <v>45.82941650183668</v>
+      </c>
     </row>
-    <row r="19" spans="1:149">
+    <row r="19" spans="1:150">
       <c r="A19" s="1">
         <v>27120</v>
       </c>
@@ -8902,8 +8956,11 @@
       <c r="ES19">
         <v>45.78939954789489</v>
       </c>
+      <c r="ET19">
+        <v>45.78939954789489</v>
+      </c>
     </row>
-    <row r="20" spans="1:149">
+    <row r="20" spans="1:150">
       <c r="A20" s="1">
         <v>27211</v>
       </c>
@@ -9351,8 +9408,11 @@
       <c r="ES20">
         <v>45.79940378638034</v>
       </c>
+      <c r="ET20">
+        <v>45.79940378638034</v>
+      </c>
     </row>
-    <row r="21" spans="1:149">
+    <row r="21" spans="1:150">
       <c r="A21" s="1">
         <v>27303</v>
       </c>
@@ -9800,8 +9860,11 @@
       <c r="ES21">
         <v>45.22916219270981</v>
       </c>
+      <c r="ET21">
+        <v>45.22916219270981</v>
+      </c>
     </row>
-    <row r="22" spans="1:149">
+    <row r="22" spans="1:150">
       <c r="A22" s="1">
         <v>27395</v>
       </c>
@@ -10249,8 +10312,11 @@
       <c r="ES22">
         <v>44.96905199208817</v>
       </c>
+      <c r="ET22">
+        <v>44.96905199208817</v>
+      </c>
     </row>
-    <row r="23" spans="1:149">
+    <row r="23" spans="1:150">
       <c r="A23" s="1">
         <v>27485</v>
       </c>
@@ -10698,8 +10764,11 @@
       <c r="ES23">
         <v>44.73895450692286</v>
       </c>
+      <c r="ET23">
+        <v>44.73895450692286</v>
+      </c>
     </row>
-    <row r="24" spans="1:149">
+    <row r="24" spans="1:150">
       <c r="A24" s="1">
         <v>27576</v>
       </c>
@@ -11147,8 +11216,11 @@
       <c r="ES24">
         <v>45.22916219270981</v>
       </c>
+      <c r="ET24">
+        <v>45.22916219270981</v>
+      </c>
     </row>
-    <row r="25" spans="1:149">
+    <row r="25" spans="1:150">
       <c r="A25" s="1">
         <v>27668</v>
       </c>
@@ -11596,8 +11668,11 @@
       <c r="ES25">
         <v>46.11953941791467</v>
       </c>
+      <c r="ET25">
+        <v>46.11953941791467</v>
+      </c>
     </row>
-    <row r="26" spans="1:149">
+    <row r="26" spans="1:150">
       <c r="A26" s="1">
         <v>27760</v>
       </c>
@@ -12045,8 +12120,11 @@
       <c r="ES26">
         <v>46.51970895733258</v>
       </c>
+      <c r="ET26">
+        <v>46.51970895733258</v>
+      </c>
     </row>
-    <row r="27" spans="1:149">
+    <row r="27" spans="1:150">
       <c r="A27" s="1">
         <v>27851</v>
       </c>
@@ -12494,8 +12572,11 @@
       <c r="ES27">
         <v>47.22000565131393</v>
       </c>
+      <c r="ET27">
+        <v>47.22000565131393</v>
+      </c>
     </row>
-    <row r="28" spans="1:149">
+    <row r="28" spans="1:150">
       <c r="A28" s="1">
         <v>27942</v>
       </c>
@@ -12943,8 +13024,11 @@
       <c r="ES28">
         <v>47.23000988979938</v>
       </c>
+      <c r="ET28">
+        <v>47.23000988979938</v>
+      </c>
     </row>
-    <row r="29" spans="1:149">
+    <row r="29" spans="1:150">
       <c r="A29" s="1">
         <v>28034</v>
       </c>
@@ -13392,8 +13476,11 @@
       <c r="ES29">
         <v>48.1103828765188</v>
       </c>
+      <c r="ET29">
+        <v>48.1103828765188</v>
+      </c>
     </row>
-    <row r="30" spans="1:149">
+    <row r="30" spans="1:150">
       <c r="A30" s="1">
         <v>28126</v>
       </c>
@@ -13841,8 +13928,11 @@
       <c r="ES30">
         <v>48.5305608929076</v>
       </c>
+      <c r="ET30">
+        <v>48.5305608929076</v>
+      </c>
     </row>
-    <row r="31" spans="1:149">
+    <row r="31" spans="1:150">
       <c r="A31" s="1">
         <v>28216</v>
       </c>
@@ -14290,8 +14380,11 @@
       <c r="ES31">
         <v>48.8006753320147</v>
       </c>
+      <c r="ET31">
+        <v>48.8006753320147</v>
+      </c>
     </row>
-    <row r="32" spans="1:149">
+    <row r="32" spans="1:150">
       <c r="A32" s="1">
         <v>28307</v>
       </c>
@@ -14739,8 +14832,11 @@
       <c r="ES32">
         <v>48.7806668550438</v>
       </c>
+      <c r="ET32">
+        <v>48.7806668550438</v>
+      </c>
     </row>
-    <row r="33" spans="1:149">
+    <row r="33" spans="1:150">
       <c r="A33" s="1">
         <v>28399</v>
       </c>
@@ -15188,8 +15284,11 @@
       <c r="ES33">
         <v>49.62102288782143</v>
       </c>
+      <c r="ET33">
+        <v>49.62102288782143</v>
+      </c>
     </row>
-    <row r="34" spans="1:149">
+    <row r="34" spans="1:150">
       <c r="A34" s="1">
         <v>28491</v>
       </c>
@@ -15637,8 +15736,11 @@
       <c r="ES34">
         <v>49.82110765753038</v>
       </c>
+      <c r="ET34">
+        <v>49.82110765753038</v>
+      </c>
     </row>
-    <row r="35" spans="1:149">
+    <row r="35" spans="1:150">
       <c r="A35" s="1">
         <v>28581</v>
       </c>
@@ -16086,8 +16188,11 @@
       <c r="ES35">
         <v>50.03119666572479</v>
       </c>
+      <c r="ET35">
+        <v>50.03119666572479</v>
+      </c>
     </row>
-    <row r="36" spans="1:149">
+    <row r="36" spans="1:150">
       <c r="A36" s="1">
         <v>28672</v>
       </c>
@@ -16535,8 +16640,11 @@
       <c r="ES36">
         <v>50.68147216727889</v>
       </c>
+      <c r="ET36">
+        <v>50.68147216727889</v>
+      </c>
     </row>
-    <row r="37" spans="1:149">
+    <row r="37" spans="1:150">
       <c r="A37" s="1">
         <v>28764</v>
       </c>
@@ -16984,8 +17092,11 @@
       <c r="ES37">
         <v>51.27172223792032</v>
       </c>
+      <c r="ET37">
+        <v>51.27172223792032</v>
+      </c>
     </row>
-    <row r="38" spans="1:149">
+    <row r="38" spans="1:150">
       <c r="A38" s="1">
         <v>28856</v>
       </c>
@@ -17433,8 +17544,11 @@
       <c r="ES38">
         <v>51.34175190731845</v>
       </c>
+      <c r="ET38">
+        <v>51.34175190731845</v>
+      </c>
     </row>
-    <row r="39" spans="1:149">
+    <row r="39" spans="1:150">
       <c r="A39" s="1">
         <v>28946</v>
       </c>
@@ -17882,8 +17996,11 @@
       <c r="ES39">
         <v>52.93242582650466</v>
       </c>
+      <c r="ET39">
+        <v>52.93242582650466</v>
+      </c>
     </row>
-    <row r="40" spans="1:149">
+    <row r="40" spans="1:150">
       <c r="A40" s="1">
         <v>29037</v>
       </c>
@@ -18331,8 +18448,11 @@
       <c r="ES40">
         <v>52.93242582650466</v>
       </c>
+      <c r="ET40">
+        <v>52.93242582650466</v>
+      </c>
     </row>
-    <row r="41" spans="1:149">
+    <row r="41" spans="1:150">
       <c r="A41" s="1">
         <v>29129</v>
       </c>
@@ -18780,8 +18900,11 @@
       <c r="ES41">
         <v>53.26256569652445</v>
       </c>
+      <c r="ET41">
+        <v>53.26256569652445</v>
+      </c>
     </row>
-    <row r="42" spans="1:149">
+    <row r="42" spans="1:150">
       <c r="A42" s="1">
         <v>29221</v>
       </c>
@@ -19229,8 +19352,11 @@
       <c r="ES42">
         <v>53.68274371291325</v>
       </c>
+      <c r="ET42">
+        <v>53.68274371291325</v>
+      </c>
     </row>
-    <row r="43" spans="1:149">
+    <row r="43" spans="1:150">
       <c r="A43" s="1">
         <v>29312</v>
       </c>
@@ -19678,8 +19804,11 @@
       <c r="ES43">
         <v>53.33259536592258</v>
       </c>
+      <c r="ET43">
+        <v>53.33259536592258</v>
+      </c>
     </row>
-    <row r="44" spans="1:149">
+    <row r="44" spans="1:150">
       <c r="A44" s="1">
         <v>29403</v>
       </c>
@@ -20127,8 +20256,11 @@
       <c r="ES44">
         <v>53.11250211924273</v>
       </c>
+      <c r="ET44">
+        <v>53.11250211924273</v>
+      </c>
     </row>
-    <row r="45" spans="1:149">
+    <row r="45" spans="1:150">
       <c r="A45" s="1">
         <v>29495</v>
       </c>
@@ -20576,8 +20708,11 @@
       <c r="ES45">
         <v>53.0424724498446</v>
       </c>
+      <c r="ET45">
+        <v>53.0424724498446</v>
+      </c>
     </row>
-    <row r="46" spans="1:149">
+    <row r="46" spans="1:150">
       <c r="A46" s="1">
         <v>29587</v>
       </c>
@@ -21025,8 +21160,11 @@
       <c r="ES46">
         <v>53.68274371291325</v>
       </c>
+      <c r="ET46">
+        <v>53.68274371291325</v>
+      </c>
     </row>
-    <row r="47" spans="1:149">
+    <row r="47" spans="1:150">
       <c r="A47" s="1">
         <v>29677</v>
       </c>
@@ -21474,8 +21612,11 @@
       <c r="ES47">
         <v>53.54268437411699</v>
       </c>
+      <c r="ET47">
+        <v>53.54268437411699</v>
+      </c>
     </row>
-    <row r="48" spans="1:149">
+    <row r="48" spans="1:150">
       <c r="A48" s="1">
         <v>29768</v>
       </c>
@@ -21923,8 +22064,11 @@
       <c r="ES48">
         <v>53.69274795139871</v>
       </c>
+      <c r="ET48">
+        <v>53.69274795139871</v>
+      </c>
     </row>
-    <row r="49" spans="1:149">
+    <row r="49" spans="1:150">
       <c r="A49" s="1">
         <v>29860</v>
       </c>
@@ -22372,8 +22516,11 @@
       <c r="ES49">
         <v>53.63272252048601</v>
       </c>
+      <c r="ET49">
+        <v>53.63272252048601</v>
+      </c>
     </row>
-    <row r="50" spans="1:149">
+    <row r="50" spans="1:150">
       <c r="A50" s="1">
         <v>29952</v>
       </c>
@@ -22821,8 +22968,11 @@
       <c r="ES50">
         <v>53.85281576716586</v>
       </c>
+      <c r="ET50">
+        <v>53.85281576716586</v>
+      </c>
     </row>
-    <row r="51" spans="1:149">
+    <row r="51" spans="1:150">
       <c r="A51" s="1">
         <v>30042</v>
       </c>
@@ -23270,8 +23420,11 @@
       <c r="ES51">
         <v>53.51267165866064</v>
       </c>
+      <c r="ET51">
+        <v>53.51267165866064</v>
+      </c>
     </row>
-    <row r="52" spans="1:149">
+    <row r="52" spans="1:150">
       <c r="A52" s="1">
         <v>30133</v>
       </c>
@@ -23719,8 +23872,11 @@
       <c r="ES52">
         <v>53.00245549590279</v>
       </c>
+      <c r="ET52">
+        <v>53.00245549590279</v>
+      </c>
     </row>
-    <row r="53" spans="1:149">
+    <row r="53" spans="1:150">
       <c r="A53" s="1">
         <v>30225</v>
       </c>
@@ -24168,8 +24324,11 @@
       <c r="ES53">
         <v>53.11250211924273</v>
       </c>
+      <c r="ET53">
+        <v>53.11250211924273</v>
+      </c>
     </row>
-    <row r="54" spans="1:149">
+    <row r="54" spans="1:150">
       <c r="A54" s="1">
         <v>30317</v>
       </c>
@@ -24617,8 +24776,11 @@
       <c r="ES54">
         <v>53.60270980502967</v>
       </c>
+      <c r="ET54">
+        <v>53.60270980502967</v>
+      </c>
     </row>
-    <row r="55" spans="1:149">
+    <row r="55" spans="1:150">
       <c r="A55" s="1">
         <v>30407</v>
       </c>
@@ -25066,8 +25228,11 @@
       <c r="ES55">
         <v>54.1729513987002</v>
       </c>
+      <c r="ET55">
+        <v>54.1729513987002</v>
+      </c>
     </row>
-    <row r="56" spans="1:149">
+    <row r="56" spans="1:150">
       <c r="A56" s="1">
         <v>30498</v>
       </c>
@@ -25515,8 +25680,11 @@
       <c r="ES56">
         <v>54.04289629838938</v>
       </c>
+      <c r="ET56">
+        <v>54.04289629838938</v>
+      </c>
     </row>
-    <row r="57" spans="1:149">
+    <row r="57" spans="1:150">
       <c r="A57" s="1">
         <v>30590</v>
       </c>
@@ -25964,8 +26132,11 @@
       <c r="ES57">
         <v>54.79321418479798</v>
       </c>
+      <c r="ET57">
+        <v>54.79321418479798</v>
+      </c>
     </row>
-    <row r="58" spans="1:149">
+    <row r="58" spans="1:150">
       <c r="A58" s="1">
         <v>30682</v>
       </c>
@@ -26413,8 +26584,11 @@
       <c r="ES58">
         <v>55.51351935575022</v>
       </c>
+      <c r="ET58">
+        <v>55.51351935575022</v>
+      </c>
     </row>
-    <row r="59" spans="1:149">
+    <row r="59" spans="1:150">
       <c r="A59" s="1">
         <v>30773</v>
       </c>
@@ -26862,8 +27036,11 @@
       <c r="ES59">
         <v>54.64315060751625</v>
       </c>
+      <c r="ET59">
+        <v>54.64315060751625</v>
+      </c>
     </row>
-    <row r="60" spans="1:149">
+    <row r="60" spans="1:150">
       <c r="A60" s="1">
         <v>30864</v>
       </c>
@@ -27311,8 +27488,11 @@
       <c r="ES60">
         <v>56.13378214184798</v>
       </c>
+      <c r="ET60">
+        <v>56.13378214184798</v>
+      </c>
     </row>
-    <row r="61" spans="1:149">
+    <row r="61" spans="1:150">
       <c r="A61" s="1">
         <v>30956</v>
       </c>
@@ -27760,8 +27940,11 @@
       <c r="ES61">
         <v>56.60398135066403</v>
       </c>
+      <c r="ET61">
+        <v>56.60398135066403</v>
+      </c>
     </row>
-    <row r="62" spans="1:149">
+    <row r="62" spans="1:150">
       <c r="A62" s="1">
         <v>31048</v>
       </c>
@@ -28209,8 +28392,11 @@
       <c r="ES62">
         <v>56.30385419610059</v>
       </c>
+      <c r="ET62">
+        <v>56.30385419610059</v>
+      </c>
     </row>
-    <row r="63" spans="1:149">
+    <row r="63" spans="1:150">
       <c r="A63" s="1">
         <v>31138</v>
       </c>
@@ -28658,8 +28844,11 @@
       <c r="ES63">
         <v>56.85408731280022</v>
       </c>
+      <c r="ET63">
+        <v>56.85408731280022</v>
+      </c>
     </row>
-    <row r="64" spans="1:149">
+    <row r="64" spans="1:150">
       <c r="A64" s="1">
         <v>31229</v>
       </c>
@@ -29107,8 +29296,11 @@
       <c r="ES64">
         <v>57.59440096072337</v>
       </c>
+      <c r="ET64">
+        <v>57.59440096072337</v>
+      </c>
     </row>
-    <row r="65" spans="1:149">
+    <row r="65" spans="1:150">
       <c r="A65" s="1">
         <v>31321</v>
       </c>
@@ -29556,8 +29748,11 @@
       <c r="ES65">
         <v>57.94454930771405</v>
       </c>
+      <c r="ET65">
+        <v>57.94454930771405</v>
+      </c>
     </row>
-    <row r="66" spans="1:149">
+    <row r="66" spans="1:150">
       <c r="A66" s="1">
         <v>31413</v>
       </c>
@@ -30005,8 +30200,11 @@
       <c r="ES66">
         <v>57.61440943769427</v>
       </c>
+      <c r="ET66">
+        <v>57.61440943769427</v>
+      </c>
     </row>
-    <row r="67" spans="1:149">
+    <row r="67" spans="1:150">
       <c r="A67" s="1">
         <v>31503</v>
       </c>
@@ -30454,8 +30652,11 @@
       <c r="ES67">
         <v>58.28469341621927</v>
       </c>
+      <c r="ET67">
+        <v>58.28469341621927</v>
+      </c>
     </row>
-    <row r="68" spans="1:149">
+    <row r="68" spans="1:150">
       <c r="A68" s="1">
         <v>31594</v>
       </c>
@@ -30903,8 +31104,11 @@
       <c r="ES68">
         <v>58.71487567109353</v>
       </c>
+      <c r="ET68">
+        <v>58.71487567109353</v>
+      </c>
     </row>
-    <row r="69" spans="1:149">
+    <row r="69" spans="1:150">
       <c r="A69" s="1">
         <v>31686</v>
       </c>
@@ -31352,8 +31556,11 @@
       <c r="ES69">
         <v>59.29512150324951</v>
       </c>
+      <c r="ET69">
+        <v>59.29512150324951</v>
+      </c>
     </row>
-    <row r="70" spans="1:149">
+    <row r="70" spans="1:150">
       <c r="A70" s="1">
         <v>31778</v>
       </c>
@@ -31801,8 +32008,11 @@
       <c r="ES70">
         <v>57.80448996891778</v>
       </c>
+      <c r="ET70">
+        <v>57.80448996891778</v>
+      </c>
     </row>
-    <row r="71" spans="1:149">
+    <row r="71" spans="1:150">
       <c r="A71" s="1">
         <v>31868</v>
       </c>
@@ -32250,8 +32460,11 @@
       <c r="ES71">
         <v>59.105040972026</v>
       </c>
+      <c r="ET71">
+        <v>59.105040972026</v>
+      </c>
     </row>
-    <row r="72" spans="1:149">
+    <row r="72" spans="1:150">
       <c r="A72" s="1">
         <v>31959</v>
       </c>
@@ -32699,8 +32912,11 @@
       <c r="ES72">
         <v>59.52521898841481</v>
       </c>
+      <c r="ET72">
+        <v>59.52521898841481</v>
+      </c>
     </row>
-    <row r="73" spans="1:149">
+    <row r="73" spans="1:150">
       <c r="A73" s="1">
         <v>32051</v>
       </c>
@@ -33148,8 +33364,11 @@
       <c r="ES73">
         <v>60.46561740604691</v>
       </c>
+      <c r="ET73">
+        <v>60.46561740604691</v>
+      </c>
     </row>
-    <row r="74" spans="1:149">
+    <row r="74" spans="1:150">
       <c r="A74" s="1">
         <v>32143</v>
       </c>
@@ -33597,8 +33816,11 @@
       <c r="ES74">
         <v>59.92538852783272</v>
       </c>
+      <c r="ET74">
+        <v>59.92538852783272</v>
+      </c>
     </row>
-    <row r="75" spans="1:149">
+    <row r="75" spans="1:150">
       <c r="A75" s="1">
         <v>32234</v>
       </c>
@@ -34046,8 +34268,11 @@
       <c r="ES75">
         <v>61.01585052274655</v>
       </c>
+      <c r="ET75">
+        <v>61.01585052274655</v>
+      </c>
     </row>
-    <row r="76" spans="1:149">
+    <row r="76" spans="1:150">
       <c r="A76" s="1">
         <v>32325</v>
       </c>
@@ -34495,8 +34720,11 @@
       <c r="ES76">
         <v>61.68613450127155</v>
       </c>
+      <c r="ET76">
+        <v>61.68613450127155</v>
+      </c>
     </row>
-    <row r="77" spans="1:149">
+    <row r="77" spans="1:150">
       <c r="A77" s="1">
         <v>32417</v>
       </c>
@@ -34941,8 +35169,11 @@
       <c r="ES77">
         <v>62.42644814919469</v>
       </c>
+      <c r="ET77">
+        <v>62.42644814919469</v>
+      </c>
     </row>
-    <row r="78" spans="1:149">
+    <row r="78" spans="1:150">
       <c r="A78" s="1">
         <v>32509</v>
       </c>
@@ -35384,8 +35615,11 @@
       <c r="ES78">
         <v>63.06671941226335</v>
       </c>
+      <c r="ET78">
+        <v>63.06671941226335</v>
+      </c>
     </row>
-    <row r="79" spans="1:149">
+    <row r="79" spans="1:150">
       <c r="A79" s="1">
         <v>32599</v>
       </c>
@@ -35824,8 +36058,11 @@
       <c r="ES79">
         <v>63.326829612885</v>
       </c>
+      <c r="ET79">
+        <v>63.326829612885</v>
+      </c>
     </row>
-    <row r="80" spans="1:149">
+    <row r="80" spans="1:150">
       <c r="A80" s="1">
         <v>32690</v>
       </c>
@@ -36261,8 +36498,11 @@
       <c r="ES80">
         <v>63.89707120655552</v>
       </c>
+      <c r="ET80">
+        <v>63.89707120655552</v>
+      </c>
     </row>
-    <row r="81" spans="1:149">
+    <row r="81" spans="1:150">
       <c r="A81" s="1">
         <v>32782</v>
       </c>
@@ -36695,8 +36935,11 @@
       <c r="ES81">
         <v>64.64738909296412</v>
       </c>
+      <c r="ET81">
+        <v>64.64738909296412</v>
+      </c>
     </row>
-    <row r="82" spans="1:149">
+    <row r="82" spans="1:150">
       <c r="A82" s="1">
         <v>32874</v>
       </c>
@@ -37126,8 +37369,11 @@
       <c r="ES82">
         <v>65.98795705001413</v>
       </c>
+      <c r="ET82">
+        <v>65.98795705001413</v>
+      </c>
     </row>
-    <row r="83" spans="1:149">
+    <row r="83" spans="1:150">
       <c r="A83" s="1">
         <v>32964</v>
       </c>
@@ -37554,8 +37800,11 @@
       <c r="ES83">
         <v>66.30809268154846</v>
       </c>
+      <c r="ET83">
+        <v>66.30809268154846</v>
+      </c>
     </row>
-    <row r="84" spans="1:149">
+    <row r="84" spans="1:150">
       <c r="A84" s="1">
         <v>33055</v>
       </c>
@@ -37979,8 +38228,11 @@
       <c r="ES84">
         <v>67.70868606951117</v>
       </c>
+      <c r="ET84">
+        <v>67.70868606951117</v>
+      </c>
     </row>
-    <row r="85" spans="1:149">
+    <row r="85" spans="1:150">
       <c r="A85" s="1">
         <v>33147</v>
       </c>
@@ -38401,8 +38653,11 @@
       <c r="ES85">
         <v>68.90919468776491</v>
       </c>
+      <c r="ET85">
+        <v>68.90919468776491</v>
+      </c>
     </row>
-    <row r="86" spans="1:149">
+    <row r="86" spans="1:150">
       <c r="A86" s="1">
         <v>33239</v>
       </c>
@@ -38820,8 +39075,11 @@
       <c r="ES86">
         <v>70.81</v>
       </c>
+      <c r="ET86">
+        <v>70.81</v>
+      </c>
     </row>
-    <row r="87" spans="1:149">
+    <row r="87" spans="1:150">
       <c r="A87" s="1">
         <v>33329</v>
       </c>
@@ -39236,8 +39494,11 @@
       <c r="ES87">
         <v>70.47</v>
       </c>
+      <c r="ET87">
+        <v>70.47</v>
+      </c>
     </row>
-    <row r="88" spans="1:149">
+    <row r="88" spans="1:150">
       <c r="A88" s="1">
         <v>33420</v>
       </c>
@@ -39649,8 +39910,11 @@
       <c r="ES88">
         <v>70.36</v>
       </c>
+      <c r="ET88">
+        <v>70.36</v>
+      </c>
     </row>
-    <row r="89" spans="1:149">
+    <row r="89" spans="1:150">
       <c r="A89" s="1">
         <v>33512</v>
       </c>
@@ -40059,8 +40323,11 @@
       <c r="ES89">
         <v>71.37</v>
       </c>
+      <c r="ET89">
+        <v>71.37</v>
+      </c>
     </row>
-    <row r="90" spans="1:149">
+    <row r="90" spans="1:150">
       <c r="A90" s="1">
         <v>33604</v>
       </c>
@@ -40466,8 +40733,11 @@
       <c r="ES90">
         <v>72.34999999999999</v>
       </c>
+      <c r="ET90">
+        <v>72.34999999999999</v>
+      </c>
     </row>
-    <row r="91" spans="1:149">
+    <row r="91" spans="1:150">
       <c r="A91" s="1">
         <v>33695</v>
       </c>
@@ -40870,8 +41140,11 @@
       <c r="ES91">
         <v>71.90000000000001</v>
       </c>
+      <c r="ET91">
+        <v>71.90000000000001</v>
+      </c>
     </row>
-    <row r="92" spans="1:149">
+    <row r="92" spans="1:150">
       <c r="A92" s="1">
         <v>33786</v>
       </c>
@@ -41271,8 +41544,11 @@
       <c r="ES92">
         <v>71.73</v>
       </c>
+      <c r="ET92">
+        <v>71.73</v>
+      </c>
     </row>
-    <row r="93" spans="1:149">
+    <row r="93" spans="1:150">
       <c r="A93" s="1">
         <v>33878</v>
       </c>
@@ -41669,8 +41945,11 @@
       <c r="ES93">
         <v>71.53</v>
       </c>
+      <c r="ET93">
+        <v>71.53</v>
+      </c>
     </row>
-    <row r="94" spans="1:149">
+    <row r="94" spans="1:150">
       <c r="A94" s="1">
         <v>33970</v>
       </c>
@@ -42064,8 +42343,11 @@
       <c r="ES94">
         <v>70.95999999999999</v>
       </c>
+      <c r="ET94">
+        <v>70.95999999999999</v>
+      </c>
     </row>
-    <row r="95" spans="1:149">
+    <row r="95" spans="1:150">
       <c r="A95" s="1">
         <v>34060</v>
       </c>
@@ -42456,8 +42738,11 @@
       <c r="ES95">
         <v>70.97</v>
       </c>
+      <c r="ET95">
+        <v>70.97</v>
+      </c>
     </row>
-    <row r="96" spans="1:149">
+    <row r="96" spans="1:150">
       <c r="A96" s="1">
         <v>34151</v>
       </c>
@@ -42845,8 +43130,11 @@
       <c r="ES96">
         <v>71.39</v>
       </c>
+      <c r="ET96">
+        <v>71.39</v>
+      </c>
     </row>
-    <row r="97" spans="1:149">
+    <row r="97" spans="1:150">
       <c r="A97" s="1">
         <v>34243</v>
       </c>
@@ -43231,8 +43519,11 @@
       <c r="ES97">
         <v>71.33</v>
       </c>
+      <c r="ET97">
+        <v>71.33</v>
+      </c>
     </row>
-    <row r="98" spans="1:149">
+    <row r="98" spans="1:150">
       <c r="A98" s="1">
         <v>34335</v>
       </c>
@@ -43614,8 +43905,11 @@
       <c r="ES98">
         <v>72.34</v>
       </c>
+      <c r="ET98">
+        <v>72.34</v>
+      </c>
     </row>
-    <row r="99" spans="1:149">
+    <row r="99" spans="1:150">
       <c r="A99" s="1">
         <v>34425</v>
       </c>
@@ -43994,8 +44288,11 @@
       <c r="ES99">
         <v>72.73999999999999</v>
       </c>
+      <c r="ET99">
+        <v>72.73999999999999</v>
+      </c>
     </row>
-    <row r="100" spans="1:149">
+    <row r="100" spans="1:150">
       <c r="A100" s="1">
         <v>34516</v>
       </c>
@@ -44371,8 +44668,11 @@
       <c r="ES100">
         <v>73.17</v>
       </c>
+      <c r="ET100">
+        <v>73.17</v>
+      </c>
     </row>
-    <row r="101" spans="1:149">
+    <row r="101" spans="1:150">
       <c r="A101" s="1">
         <v>34608</v>
       </c>
@@ -44745,8 +45045,11 @@
       <c r="ES101">
         <v>73.98</v>
       </c>
+      <c r="ET101">
+        <v>73.98</v>
+      </c>
     </row>
-    <row r="102" spans="1:149">
+    <row r="102" spans="1:150">
       <c r="A102" s="1">
         <v>34700</v>
       </c>
@@ -45116,8 +45419,11 @@
       <c r="ES102">
         <v>73.69</v>
       </c>
+      <c r="ET102">
+        <v>73.69</v>
+      </c>
     </row>
-    <row r="103" spans="1:149">
+    <row r="103" spans="1:150">
       <c r="A103" s="1">
         <v>34790</v>
       </c>
@@ -45484,8 +45790,11 @@
       <c r="ES103">
         <v>74.28</v>
       </c>
+      <c r="ET103">
+        <v>74.28</v>
+      </c>
     </row>
-    <row r="104" spans="1:149">
+    <row r="104" spans="1:150">
       <c r="A104" s="1">
         <v>34881</v>
       </c>
@@ -45849,8 +46158,11 @@
       <c r="ES104">
         <v>74.43000000000001</v>
       </c>
+      <c r="ET104">
+        <v>74.43000000000001</v>
+      </c>
     </row>
-    <row r="105" spans="1:149">
+    <row r="105" spans="1:150">
       <c r="A105" s="1">
         <v>34973</v>
       </c>
@@ -46211,8 +46523,11 @@
       <c r="ES105">
         <v>74.45999999999999</v>
       </c>
+      <c r="ET105">
+        <v>74.45999999999999</v>
+      </c>
     </row>
-    <row r="106" spans="1:149">
+    <row r="106" spans="1:150">
       <c r="A106" s="1">
         <v>35065</v>
       </c>
@@ -46570,8 +46885,11 @@
       <c r="ES106">
         <v>73.93000000000001</v>
       </c>
+      <c r="ET106">
+        <v>73.93000000000001</v>
+      </c>
     </row>
-    <row r="107" spans="1:149">
+    <row r="107" spans="1:150">
       <c r="A107" s="1">
         <v>35156</v>
       </c>
@@ -46926,8 +47244,11 @@
       <c r="ES107">
         <v>74.94</v>
       </c>
+      <c r="ET107">
+        <v>74.94</v>
+      </c>
     </row>
-    <row r="108" spans="1:149">
+    <row r="108" spans="1:150">
       <c r="A108" s="1">
         <v>35247</v>
       </c>
@@ -47279,8 +47600,11 @@
       <c r="ES108">
         <v>75.23</v>
       </c>
+      <c r="ET108">
+        <v>75.23</v>
+      </c>
     </row>
-    <row r="109" spans="1:149">
+    <row r="109" spans="1:150">
       <c r="A109" s="1">
         <v>35339</v>
       </c>
@@ -47629,8 +47953,11 @@
       <c r="ES109">
         <v>75.92</v>
       </c>
+      <c r="ET109">
+        <v>75.92</v>
+      </c>
     </row>
-    <row r="110" spans="1:149">
+    <row r="110" spans="1:150">
       <c r="A110" s="1">
         <v>35431</v>
       </c>
@@ -47976,8 +48303,11 @@
       <c r="ES110">
         <v>75.53</v>
       </c>
+      <c r="ET110">
+        <v>75.53</v>
+      </c>
     </row>
-    <row r="111" spans="1:149">
+    <row r="111" spans="1:150">
       <c r="A111" s="1">
         <v>35521</v>
       </c>
@@ -48320,8 +48650,11 @@
       <c r="ES111">
         <v>76.37</v>
       </c>
+      <c r="ET111">
+        <v>76.37</v>
+      </c>
     </row>
-    <row r="112" spans="1:149">
+    <row r="112" spans="1:150">
       <c r="A112" s="1">
         <v>35612</v>
       </c>
@@ -48661,8 +48994,11 @@
       <c r="ES112">
         <v>76.67</v>
       </c>
+      <c r="ET112">
+        <v>76.67</v>
+      </c>
     </row>
-    <row r="113" spans="1:149">
+    <row r="113" spans="1:150">
       <c r="A113" s="1">
         <v>35704</v>
       </c>
@@ -48999,8 +49335,11 @@
       <c r="ES113">
         <v>77.23999999999999</v>
       </c>
+      <c r="ET113">
+        <v>77.23999999999999</v>
+      </c>
     </row>
-    <row r="114" spans="1:149">
+    <row r="114" spans="1:150">
       <c r="A114" s="1">
         <v>35796</v>
       </c>
@@ -49334,8 +49673,11 @@
       <c r="ES114">
         <v>77.98</v>
       </c>
+      <c r="ET114">
+        <v>77.98</v>
+      </c>
     </row>
-    <row r="115" spans="1:149">
+    <row r="115" spans="1:150">
       <c r="A115" s="1">
         <v>35886</v>
       </c>
@@ -49666,8 +50008,11 @@
       <c r="ES115">
         <v>77.62</v>
       </c>
+      <c r="ET115">
+        <v>77.62</v>
+      </c>
     </row>
-    <row r="116" spans="1:149">
+    <row r="116" spans="1:150">
       <c r="A116" s="1">
         <v>35977</v>
       </c>
@@ -49995,8 +50340,11 @@
       <c r="ES116">
         <v>78</v>
       </c>
+      <c r="ET116">
+        <v>78</v>
+      </c>
     </row>
-    <row r="117" spans="1:149">
+    <row r="117" spans="1:150">
       <c r="A117" s="1">
         <v>36069</v>
       </c>
@@ -50321,8 +50669,11 @@
       <c r="ES117">
         <v>77.98</v>
       </c>
+      <c r="ET117">
+        <v>77.98</v>
+      </c>
     </row>
-    <row r="118" spans="1:149">
+    <row r="118" spans="1:150">
       <c r="A118" s="1">
         <v>36161</v>
       </c>
@@ -50644,8 +50995,11 @@
       <c r="ES118">
         <v>78.88</v>
       </c>
+      <c r="ET118">
+        <v>78.88</v>
+      </c>
     </row>
-    <row r="119" spans="1:149">
+    <row r="119" spans="1:150">
       <c r="A119" s="1">
         <v>36251</v>
       </c>
@@ -50964,8 +51318,11 @@
       <c r="ES119">
         <v>78.78</v>
       </c>
+      <c r="ET119">
+        <v>78.78</v>
+      </c>
     </row>
-    <row r="120" spans="1:149">
+    <row r="120" spans="1:150">
       <c r="A120" s="1">
         <v>36342</v>
       </c>
@@ -51281,8 +51638,11 @@
       <c r="ES120">
         <v>79.86</v>
       </c>
+      <c r="ET120">
+        <v>79.86</v>
+      </c>
     </row>
-    <row r="121" spans="1:149">
+    <row r="121" spans="1:150">
       <c r="A121" s="1">
         <v>36434</v>
       </c>
@@ -51595,8 +51955,11 @@
       <c r="ES121">
         <v>80.23999999999999</v>
       </c>
+      <c r="ET121">
+        <v>80.23999999999999</v>
+      </c>
     </row>
-    <row r="122" spans="1:149">
+    <row r="122" spans="1:150">
       <c r="A122" s="1">
         <v>36526</v>
       </c>
@@ -51906,8 +52269,11 @@
       <c r="ES122">
         <v>81.48</v>
       </c>
+      <c r="ET122">
+        <v>81.48</v>
+      </c>
     </row>
-    <row r="123" spans="1:149">
+    <row r="123" spans="1:150">
       <c r="A123" s="1">
         <v>36617</v>
       </c>
@@ -52214,8 +52580,11 @@
       <c r="ES123">
         <v>82.13</v>
       </c>
+      <c r="ET123">
+        <v>82.13</v>
+      </c>
     </row>
-    <row r="124" spans="1:149">
+    <row r="124" spans="1:150">
       <c r="A124" s="1">
         <v>36708</v>
       </c>
@@ -52519,8 +52888,11 @@
       <c r="ES124">
         <v>82.19</v>
       </c>
+      <c r="ET124">
+        <v>82.19</v>
+      </c>
     </row>
-    <row r="125" spans="1:149">
+    <row r="125" spans="1:150">
       <c r="A125" s="1">
         <v>36800</v>
       </c>
@@ -52821,8 +53193,11 @@
       <c r="ES125">
         <v>81.84</v>
       </c>
+      <c r="ET125">
+        <v>81.84</v>
+      </c>
     </row>
-    <row r="126" spans="1:149">
+    <row r="126" spans="1:150">
       <c r="A126" s="1">
         <v>36892</v>
       </c>
@@ -53120,8 +53495,11 @@
       <c r="ES126">
         <v>83.58</v>
       </c>
+      <c r="ET126">
+        <v>83.58</v>
+      </c>
     </row>
-    <row r="127" spans="1:149">
+    <row r="127" spans="1:150">
       <c r="A127" s="1">
         <v>36982</v>
       </c>
@@ -53416,8 +53794,11 @@
       <c r="ES127">
         <v>83.37</v>
       </c>
+      <c r="ET127">
+        <v>83.37</v>
+      </c>
     </row>
-    <row r="128" spans="1:149">
+    <row r="128" spans="1:150">
       <c r="A128" s="1">
         <v>37073</v>
       </c>
@@ -53709,8 +54090,11 @@
       <c r="ES128">
         <v>83.37</v>
       </c>
+      <c r="ET128">
+        <v>83.37</v>
+      </c>
     </row>
-    <row r="129" spans="1:149">
+    <row r="129" spans="1:150">
       <c r="A129" s="1">
         <v>37165</v>
       </c>
@@ -53999,8 +54383,11 @@
       <c r="ES129">
         <v>83.11</v>
       </c>
+      <c r="ET129">
+        <v>83.11</v>
+      </c>
     </row>
-    <row r="130" spans="1:149">
+    <row r="130" spans="1:150">
       <c r="A130" s="1">
         <v>37257</v>
       </c>
@@ -54286,8 +54673,11 @@
       <c r="ES130">
         <v>82.72</v>
       </c>
+      <c r="ET130">
+        <v>82.72</v>
+      </c>
     </row>
-    <row r="131" spans="1:149">
+    <row r="131" spans="1:150">
       <c r="A131" s="1">
         <v>37347</v>
       </c>
@@ -54570,8 +54960,11 @@
       <c r="ES131">
         <v>83.04000000000001</v>
       </c>
+      <c r="ET131">
+        <v>83.04000000000001</v>
+      </c>
     </row>
-    <row r="132" spans="1:149">
+    <row r="132" spans="1:150">
       <c r="A132" s="1">
         <v>37438</v>
       </c>
@@ -54851,8 +55244,11 @@
       <c r="ES132">
         <v>83.61</v>
       </c>
+      <c r="ET132">
+        <v>83.61</v>
+      </c>
     </row>
-    <row r="133" spans="1:149">
+    <row r="133" spans="1:150">
       <c r="A133" s="1">
         <v>37530</v>
       </c>
@@ -55129,8 +55525,11 @@
       <c r="ES133">
         <v>83.38</v>
       </c>
+      <c r="ET133">
+        <v>83.38</v>
+      </c>
     </row>
-    <row r="134" spans="1:149">
+    <row r="134" spans="1:150">
       <c r="A134" s="1">
         <v>37622</v>
       </c>
@@ -55404,8 +55803,11 @@
       <c r="ES134">
         <v>82.25</v>
       </c>
+      <c r="ET134">
+        <v>82.25</v>
+      </c>
     </row>
-    <row r="135" spans="1:149">
+    <row r="135" spans="1:150">
       <c r="A135" s="1">
         <v>37712</v>
       </c>
@@ -55676,8 +56078,11 @@
       <c r="ES135">
         <v>82.37</v>
       </c>
+      <c r="ET135">
+        <v>82.37</v>
+      </c>
     </row>
-    <row r="136" spans="1:149">
+    <row r="136" spans="1:150">
       <c r="A136" s="1">
         <v>37803</v>
       </c>
@@ -55945,8 +56350,11 @@
       <c r="ES136">
         <v>83.12</v>
       </c>
+      <c r="ET136">
+        <v>83.12</v>
+      </c>
     </row>
-    <row r="137" spans="1:149">
+    <row r="137" spans="1:150">
       <c r="A137" s="1">
         <v>37895</v>
       </c>
@@ -56211,8 +56619,11 @@
       <c r="ES137">
         <v>83.22</v>
       </c>
+      <c r="ET137">
+        <v>83.22</v>
+      </c>
     </row>
-    <row r="138" spans="1:149">
+    <row r="138" spans="1:150">
       <c r="A138" s="1">
         <v>37987</v>
       </c>
@@ -56474,8 +56885,11 @@
       <c r="ES138">
         <v>83.09</v>
       </c>
+      <c r="ET138">
+        <v>83.09</v>
+      </c>
     </row>
-    <row r="139" spans="1:149">
+    <row r="139" spans="1:150">
       <c r="A139" s="1">
         <v>38078</v>
       </c>
@@ -56734,8 +57148,11 @@
       <c r="ES139">
         <v>83.58</v>
       </c>
+      <c r="ET139">
+        <v>83.58</v>
+      </c>
     </row>
-    <row r="140" spans="1:149">
+    <row r="140" spans="1:150">
       <c r="A140" s="1">
         <v>38169</v>
       </c>
@@ -56991,8 +57408,11 @@
       <c r="ES140">
         <v>83.31</v>
       </c>
+      <c r="ET140">
+        <v>83.31</v>
+      </c>
     </row>
-    <row r="141" spans="1:149">
+    <row r="141" spans="1:150">
       <c r="A141" s="1">
         <v>38261</v>
       </c>
@@ -57245,8 +57665,11 @@
       <c r="ES141">
         <v>83.28</v>
       </c>
+      <c r="ET141">
+        <v>83.28</v>
+      </c>
     </row>
-    <row r="142" spans="1:149">
+    <row r="142" spans="1:150">
       <c r="A142" s="1">
         <v>38353</v>
       </c>
@@ -57496,8 +57919,11 @@
       <c r="ES142">
         <v>83.41</v>
       </c>
+      <c r="ET142">
+        <v>83.41</v>
+      </c>
     </row>
-    <row r="143" spans="1:149">
+    <row r="143" spans="1:150">
       <c r="A143" s="1">
         <v>38443</v>
       </c>
@@ -57744,8 +58170,11 @@
       <c r="ES143">
         <v>83.91</v>
       </c>
+      <c r="ET143">
+        <v>83.91</v>
+      </c>
     </row>
-    <row r="144" spans="1:149">
+    <row r="144" spans="1:150">
       <c r="A144" s="1">
         <v>38534</v>
       </c>
@@ -57989,8 +58418,11 @@
       <c r="ES144">
         <v>84.56999999999999</v>
       </c>
+      <c r="ET144">
+        <v>84.56999999999999</v>
+      </c>
     </row>
-    <row r="145" spans="1:149">
+    <row r="145" spans="1:150">
       <c r="A145" s="1">
         <v>38626</v>
       </c>
@@ -58231,8 +58663,11 @@
       <c r="ES145">
         <v>84.89</v>
       </c>
+      <c r="ET145">
+        <v>84.89</v>
+      </c>
     </row>
-    <row r="146" spans="1:149">
+    <row r="146" spans="1:150">
       <c r="A146" s="1">
         <v>38718</v>
       </c>
@@ -58470,8 +58905,11 @@
       <c r="ES146">
         <v>85.84</v>
       </c>
+      <c r="ET146">
+        <v>85.84</v>
+      </c>
     </row>
-    <row r="147" spans="1:149">
+    <row r="147" spans="1:150">
       <c r="A147" s="1">
         <v>38808</v>
       </c>
@@ -58706,8 +59144,11 @@
       <c r="ES147">
         <v>87.31</v>
       </c>
+      <c r="ET147">
+        <v>87.31</v>
+      </c>
     </row>
-    <row r="148" spans="1:149">
+    <row r="148" spans="1:150">
       <c r="A148" s="1">
         <v>38899</v>
       </c>
@@ -58939,8 +59380,11 @@
       <c r="ES148">
         <v>87.97</v>
       </c>
+      <c r="ET148">
+        <v>87.97</v>
+      </c>
     </row>
-    <row r="149" spans="1:149">
+    <row r="149" spans="1:150">
       <c r="A149" s="1">
         <v>38991</v>
       </c>
@@ -59169,8 +59613,11 @@
       <c r="ES149">
         <v>89.26000000000001</v>
       </c>
+      <c r="ET149">
+        <v>89.26000000000001</v>
+      </c>
     </row>
-    <row r="150" spans="1:149">
+    <row r="150" spans="1:150">
       <c r="A150" s="1">
         <v>39083</v>
       </c>
@@ -59396,8 +59843,11 @@
       <c r="ES150">
         <v>89.38</v>
       </c>
+      <c r="ET150">
+        <v>89.38</v>
+      </c>
     </row>
-    <row r="151" spans="1:149">
+    <row r="151" spans="1:150">
       <c r="A151" s="1">
         <v>39173</v>
       </c>
@@ -59620,8 +60070,11 @@
       <c r="ES151">
         <v>89.97</v>
       </c>
+      <c r="ET151">
+        <v>89.97</v>
+      </c>
     </row>
-    <row r="152" spans="1:149">
+    <row r="152" spans="1:150">
       <c r="A152" s="1">
         <v>39264</v>
       </c>
@@ -59841,8 +60294,11 @@
       <c r="ES152">
         <v>90.43000000000001</v>
       </c>
+      <c r="ET152">
+        <v>90.43000000000001</v>
+      </c>
     </row>
-    <row r="153" spans="1:149">
+    <row r="153" spans="1:150">
       <c r="A153" s="1">
         <v>39356</v>
       </c>
@@ -60059,8 +60515,11 @@
       <c r="ES153">
         <v>91.09999999999999</v>
       </c>
+      <c r="ET153">
+        <v>91.09999999999999</v>
+      </c>
     </row>
-    <row r="154" spans="1:149">
+    <row r="154" spans="1:150">
       <c r="A154" s="1">
         <v>39448</v>
       </c>
@@ -60274,8 +60733,11 @@
       <c r="ES154">
         <v>91.63</v>
       </c>
+      <c r="ET154">
+        <v>91.63</v>
+      </c>
     </row>
-    <row r="155" spans="1:149">
+    <row r="155" spans="1:150">
       <c r="A155" s="1">
         <v>39539</v>
       </c>
@@ -60486,8 +60948,11 @@
       <c r="ES155">
         <v>91.3</v>
       </c>
+      <c r="ET155">
+        <v>91.3</v>
+      </c>
     </row>
-    <row r="156" spans="1:149">
+    <row r="156" spans="1:150">
       <c r="A156" s="1">
         <v>39630</v>
       </c>
@@ -60695,8 +61160,11 @@
       <c r="ES156">
         <v>90.8</v>
       </c>
+      <c r="ET156">
+        <v>90.8</v>
+      </c>
     </row>
-    <row r="157" spans="1:149">
+    <row r="157" spans="1:150">
       <c r="A157" s="1">
         <v>39722</v>
       </c>
@@ -60901,8 +61369,11 @@
       <c r="ES157">
         <v>89.39</v>
       </c>
+      <c r="ET157">
+        <v>89.39</v>
+      </c>
     </row>
-    <row r="158" spans="1:149">
+    <row r="158" spans="1:150">
       <c r="A158" s="1">
         <v>39814</v>
       </c>
@@ -61104,8 +61575,11 @@
       <c r="ES158">
         <v>85.2</v>
       </c>
+      <c r="ET158">
+        <v>85.2</v>
+      </c>
     </row>
-    <row r="159" spans="1:149">
+    <row r="159" spans="1:150">
       <c r="A159" s="1">
         <v>39904</v>
       </c>
@@ -61304,8 +61778,11 @@
       <c r="ES159">
         <v>85.41</v>
       </c>
+      <c r="ET159">
+        <v>85.41</v>
+      </c>
     </row>
-    <row r="160" spans="1:149">
+    <row r="160" spans="1:150">
       <c r="A160" s="1">
         <v>39995</v>
       </c>
@@ -61501,8 +61978,11 @@
       <c r="ES160">
         <v>85.94</v>
       </c>
+      <c r="ET160">
+        <v>85.94</v>
+      </c>
     </row>
-    <row r="161" spans="1:149">
+    <row r="161" spans="1:150">
       <c r="A161" s="1">
         <v>40087</v>
       </c>
@@ -61695,8 +62175,11 @@
       <c r="ES161">
         <v>86.59999999999999</v>
       </c>
+      <c r="ET161">
+        <v>86.59999999999999</v>
+      </c>
     </row>
-    <row r="162" spans="1:149">
+    <row r="162" spans="1:150">
       <c r="A162" s="1">
         <v>40179</v>
       </c>
@@ -61886,8 +62369,11 @@
       <c r="ES162">
         <v>87.23</v>
       </c>
+      <c r="ET162">
+        <v>87.23</v>
+      </c>
     </row>
-    <row r="163" spans="1:149">
+    <row r="163" spans="1:150">
       <c r="A163" s="1">
         <v>40269</v>
       </c>
@@ -62074,8 +62560,11 @@
       <c r="ES163">
         <v>89.12</v>
       </c>
+      <c r="ET163">
+        <v>89.12</v>
+      </c>
     </row>
-    <row r="164" spans="1:149">
+    <row r="164" spans="1:150">
       <c r="A164" s="1">
         <v>40360</v>
       </c>
@@ -62259,8 +62748,11 @@
       <c r="ES164">
         <v>89.98</v>
       </c>
+      <c r="ET164">
+        <v>89.98</v>
+      </c>
     </row>
-    <row r="165" spans="1:149">
+    <row r="165" spans="1:150">
       <c r="A165" s="1">
         <v>40452</v>
       </c>
@@ -62441,8 +62933,11 @@
       <c r="ES165">
         <v>90.56999999999999</v>
       </c>
+      <c r="ET165">
+        <v>90.56999999999999</v>
+      </c>
     </row>
-    <row r="166" spans="1:149">
+    <row r="166" spans="1:150">
       <c r="A166" s="1">
         <v>40544</v>
       </c>
@@ -62620,8 +63115,11 @@
       <c r="ES166">
         <v>92.20999999999999</v>
       </c>
+      <c r="ET166">
+        <v>92.20999999999999</v>
+      </c>
     </row>
-    <row r="167" spans="1:149">
+    <row r="167" spans="1:150">
       <c r="A167" s="1">
         <v>40634</v>
       </c>
@@ -62796,8 +63294,11 @@
       <c r="ES167">
         <v>92.45999999999999</v>
       </c>
+      <c r="ET167">
+        <v>92.45999999999999</v>
+      </c>
     </row>
-    <row r="168" spans="1:149">
+    <row r="168" spans="1:150">
       <c r="A168" s="1">
         <v>40725</v>
       </c>
@@ -62969,8 +63470,11 @@
       <c r="ES168">
         <v>92.95999999999999</v>
       </c>
+      <c r="ET168">
+        <v>92.95999999999999</v>
+      </c>
     </row>
-    <row r="169" spans="1:149">
+    <row r="169" spans="1:150">
       <c r="A169" s="1">
         <v>40817</v>
       </c>
@@ -63139,8 +63643,11 @@
       <c r="ES169">
         <v>92.95</v>
       </c>
+      <c r="ET169">
+        <v>92.95</v>
+      </c>
     </row>
-    <row r="170" spans="1:149">
+    <row r="170" spans="1:150">
       <c r="A170" s="1">
         <v>40909</v>
       </c>
@@ -63306,8 +63813,11 @@
       <c r="ES170">
         <v>93.15000000000001</v>
       </c>
+      <c r="ET170">
+        <v>93.15000000000001</v>
+      </c>
     </row>
-    <row r="171" spans="1:149">
+    <row r="171" spans="1:150">
       <c r="A171" s="1">
         <v>41000</v>
       </c>
@@ -63470,8 +63980,11 @@
       <c r="ES171">
         <v>93.25</v>
       </c>
+      <c r="ET171">
+        <v>93.25</v>
+      </c>
     </row>
-    <row r="172" spans="1:149">
+    <row r="172" spans="1:150">
       <c r="A172" s="1">
         <v>41091</v>
       </c>
@@ -63631,8 +64144,11 @@
       <c r="ES172">
         <v>93.44</v>
       </c>
+      <c r="ET172">
+        <v>93.44</v>
+      </c>
     </row>
-    <row r="173" spans="1:149">
+    <row r="173" spans="1:150">
       <c r="A173" s="1">
         <v>41183</v>
       </c>
@@ -63789,8 +64305,11 @@
       <c r="ES173">
         <v>93.16</v>
       </c>
+      <c r="ET173">
+        <v>93.16</v>
+      </c>
     </row>
-    <row r="174" spans="1:149">
+    <row r="174" spans="1:150">
       <c r="A174" s="1">
         <v>41275</v>
       </c>
@@ -63944,8 +64463,11 @@
       <c r="ES174">
         <v>92.64</v>
       </c>
+      <c r="ET174">
+        <v>92.64</v>
+      </c>
     </row>
-    <row r="175" spans="1:149">
+    <row r="175" spans="1:150">
       <c r="A175" s="1">
         <v>41365</v>
       </c>
@@ -64096,8 +64618,11 @@
       <c r="ES175">
         <v>93.72</v>
       </c>
+      <c r="ET175">
+        <v>93.72</v>
+      </c>
     </row>
-    <row r="176" spans="1:149">
+    <row r="176" spans="1:150">
       <c r="A176" s="1">
         <v>41456</v>
       </c>
@@ -64245,8 +64770,11 @@
       <c r="ES176">
         <v>94.2</v>
       </c>
+      <c r="ET176">
+        <v>94.2</v>
+      </c>
     </row>
-    <row r="177" spans="1:149">
+    <row r="177" spans="1:150">
       <c r="A177" s="1">
         <v>41548</v>
       </c>
@@ -64391,8 +64919,11 @@
       <c r="ES177">
         <v>94.34</v>
       </c>
+      <c r="ET177">
+        <v>94.34</v>
+      </c>
     </row>
-    <row r="178" spans="1:149">
+    <row r="178" spans="1:150">
       <c r="A178" s="1">
         <v>41640</v>
       </c>
@@ -64534,8 +65065,11 @@
       <c r="ES178">
         <v>95.33</v>
       </c>
+      <c r="ET178">
+        <v>95.33</v>
+      </c>
     </row>
-    <row r="179" spans="1:149">
+    <row r="179" spans="1:150">
       <c r="A179" s="1">
         <v>41730</v>
       </c>
@@ -64674,8 +65208,11 @@
       <c r="ES179">
         <v>95.31</v>
       </c>
+      <c r="ET179">
+        <v>95.31</v>
+      </c>
     </row>
-    <row r="180" spans="1:149">
+    <row r="180" spans="1:150">
       <c r="A180" s="1">
         <v>41821</v>
       </c>
@@ -64811,8 +65348,11 @@
       <c r="ES180">
         <v>95.84</v>
       </c>
+      <c r="ET180">
+        <v>95.84</v>
+      </c>
     </row>
-    <row r="181" spans="1:149">
+    <row r="181" spans="1:150">
       <c r="A181" s="1">
         <v>41913</v>
       </c>
@@ -64945,8 +65485,11 @@
       <c r="ES181">
         <v>96.56999999999999</v>
       </c>
+      <c r="ET181">
+        <v>96.56999999999999</v>
+      </c>
     </row>
-    <row r="182" spans="1:149">
+    <row r="182" spans="1:150">
       <c r="A182" s="1">
         <v>42005</v>
       </c>
@@ -65076,8 +65619,11 @@
       <c r="ES182">
         <v>96.36</v>
       </c>
+      <c r="ET182">
+        <v>96.36</v>
+      </c>
     </row>
-    <row r="183" spans="1:149">
+    <row r="183" spans="1:150">
       <c r="A183" s="1">
         <v>42095</v>
       </c>
@@ -65204,8 +65750,11 @@
       <c r="ES183">
         <v>96.86</v>
       </c>
+      <c r="ET183">
+        <v>96.86</v>
+      </c>
     </row>
-    <row r="184" spans="1:149">
+    <row r="184" spans="1:150">
       <c r="A184" s="1">
         <v>42186</v>
       </c>
@@ -65329,8 +65878,11 @@
       <c r="ES184">
         <v>97.38</v>
       </c>
+      <c r="ET184">
+        <v>97.38</v>
+      </c>
     </row>
-    <row r="185" spans="1:149">
+    <row r="185" spans="1:150">
       <c r="A185" s="1">
         <v>42278</v>
       </c>
@@ -65451,8 +66003,11 @@
       <c r="ES185">
         <v>97.88</v>
       </c>
+      <c r="ET185">
+        <v>97.88</v>
+      </c>
     </row>
-    <row r="186" spans="1:149">
+    <row r="186" spans="1:150">
       <c r="A186" s="1">
         <v>42370</v>
       </c>
@@ -65570,8 +66125,11 @@
       <c r="ES186">
         <v>98.73999999999999</v>
       </c>
+      <c r="ET186">
+        <v>98.73999999999999</v>
+      </c>
     </row>
-    <row r="187" spans="1:149">
+    <row r="187" spans="1:150">
       <c r="A187" s="1">
         <v>42461</v>
       </c>
@@ -65686,8 +66244,11 @@
       <c r="ES187">
         <v>98.95999999999999</v>
       </c>
+      <c r="ET187">
+        <v>98.95999999999999</v>
+      </c>
     </row>
-    <row r="188" spans="1:149">
+    <row r="188" spans="1:150">
       <c r="A188" s="1">
         <v>42552</v>
       </c>
@@ -65799,8 +66360,11 @@
       <c r="ES188">
         <v>99.31</v>
       </c>
+      <c r="ET188">
+        <v>99.31</v>
+      </c>
     </row>
-    <row r="189" spans="1:149">
+    <row r="189" spans="1:150">
       <c r="A189" s="1">
         <v>42644</v>
       </c>
@@ -65909,8 +66473,11 @@
       <c r="ES189">
         <v>99.77</v>
       </c>
+      <c r="ET189">
+        <v>99.77</v>
+      </c>
     </row>
-    <row r="190" spans="1:149">
+    <row r="190" spans="1:150">
       <c r="A190" s="1">
         <v>42736</v>
       </c>
@@ -66016,8 +66583,11 @@
       <c r="ES190">
         <v>101.06</v>
       </c>
+      <c r="ET190">
+        <v>101.06</v>
+      </c>
     </row>
-    <row r="191" spans="1:149">
+    <row r="191" spans="1:150">
       <c r="A191" s="1">
         <v>42826</v>
       </c>
@@ -66120,8 +66690,11 @@
       <c r="ES191">
         <v>101.78</v>
       </c>
+      <c r="ET191">
+        <v>101.78</v>
+      </c>
     </row>
-    <row r="192" spans="1:149">
+    <row r="192" spans="1:150">
       <c r="A192" s="1">
         <v>42917</v>
       </c>
@@ -66221,8 +66794,11 @@
       <c r="ES192">
         <v>102.59</v>
       </c>
+      <c r="ET192">
+        <v>102.59</v>
+      </c>
     </row>
-    <row r="193" spans="1:149">
+    <row r="193" spans="1:150">
       <c r="A193" s="1">
         <v>43009</v>
       </c>
@@ -66319,8 +66895,11 @@
       <c r="ES193">
         <v>103.63</v>
       </c>
+      <c r="ET193">
+        <v>103.63</v>
+      </c>
     </row>
-    <row r="194" spans="1:149">
+    <row r="194" spans="1:150">
       <c r="A194" s="1">
         <v>43101</v>
       </c>
@@ -66414,8 +66993,11 @@
       <c r="ES194">
         <v>103.06</v>
       </c>
+      <c r="ET194">
+        <v>103.06</v>
+      </c>
     </row>
-    <row r="195" spans="1:149">
+    <row r="195" spans="1:150">
       <c r="A195" s="1">
         <v>43191</v>
       </c>
@@ -66506,8 +67088,11 @@
       <c r="ES195">
         <v>103.87</v>
       </c>
+      <c r="ET195">
+        <v>103.87</v>
+      </c>
     </row>
-    <row r="196" spans="1:149">
+    <row r="196" spans="1:150">
       <c r="A196" s="1">
         <v>43282</v>
       </c>
@@ -66595,8 +67180,11 @@
       <c r="ES196">
         <v>103.19</v>
       </c>
+      <c r="ET196">
+        <v>103.19</v>
+      </c>
     </row>
-    <row r="197" spans="1:149">
+    <row r="197" spans="1:150">
       <c r="A197" s="1">
         <v>43374</v>
       </c>
@@ -66681,8 +67269,11 @@
       <c r="ES197">
         <v>103.65</v>
       </c>
+      <c r="ET197">
+        <v>103.65</v>
+      </c>
     </row>
-    <row r="198" spans="1:149">
+    <row r="198" spans="1:150">
       <c r="A198" s="1">
         <v>43466</v>
       </c>
@@ -66764,8 +67355,11 @@
       <c r="ES198">
         <v>104.33</v>
       </c>
+      <c r="ET198">
+        <v>104.33</v>
+      </c>
     </row>
-    <row r="199" spans="1:149">
+    <row r="199" spans="1:150">
       <c r="A199" s="1">
         <v>43556</v>
       </c>
@@ -66844,8 +67438,11 @@
       <c r="ES199">
         <v>104.39</v>
       </c>
+      <c r="ET199">
+        <v>104.39</v>
+      </c>
     </row>
-    <row r="200" spans="1:149">
+    <row r="200" spans="1:150">
       <c r="A200" s="1">
         <v>43647</v>
       </c>
@@ -66921,8 +67518,11 @@
       <c r="ES200">
         <v>104.79</v>
       </c>
+      <c r="ET200">
+        <v>104.79</v>
+      </c>
     </row>
-    <row r="201" spans="1:149">
+    <row r="201" spans="1:150">
       <c r="A201" s="1">
         <v>43739</v>
       </c>
@@ -66995,8 +67595,11 @@
       <c r="ES201">
         <v>104.44</v>
       </c>
+      <c r="ET201">
+        <v>104.44</v>
+      </c>
     </row>
-    <row r="202" spans="1:149">
+    <row r="202" spans="1:150">
       <c r="A202" s="1">
         <v>43831</v>
       </c>
@@ -67066,8 +67669,11 @@
       <c r="ES202">
         <v>102.32</v>
       </c>
+      <c r="ET202">
+        <v>102.32</v>
+      </c>
     </row>
-    <row r="203" spans="1:149">
+    <row r="203" spans="1:150">
       <c r="A203" s="1">
         <v>43922</v>
       </c>
@@ -67134,8 +67740,11 @@
       <c r="ES203">
         <v>93.23999999999999</v>
       </c>
+      <c r="ET203">
+        <v>93.23999999999999</v>
+      </c>
     </row>
-    <row r="204" spans="1:149">
+    <row r="204" spans="1:150">
       <c r="A204" s="1">
         <v>44013</v>
       </c>
@@ -67199,8 +67808,11 @@
       <c r="ES204">
         <v>101.33</v>
       </c>
+      <c r="ET204">
+        <v>101.33</v>
+      </c>
     </row>
-    <row r="205" spans="1:149">
+    <row r="205" spans="1:150">
       <c r="A205" s="1">
         <v>44105</v>
       </c>
@@ -67261,8 +67873,11 @@
       <c r="ES205">
         <v>102.31</v>
       </c>
+      <c r="ET205">
+        <v>102.31</v>
+      </c>
     </row>
-    <row r="206" spans="1:149">
+    <row r="206" spans="1:150">
       <c r="A206" s="1">
         <v>44197</v>
       </c>
@@ -67320,8 +67935,11 @@
       <c r="ES206">
         <v>101.68</v>
       </c>
+      <c r="ET206">
+        <v>101.68</v>
+      </c>
     </row>
-    <row r="207" spans="1:149">
+    <row r="207" spans="1:150">
       <c r="A207" s="1">
         <v>44287</v>
       </c>
@@ -67376,8 +67994,11 @@
       <c r="ES207">
         <v>104.07</v>
       </c>
+      <c r="ET207">
+        <v>104.07</v>
+      </c>
     </row>
-    <row r="208" spans="1:149">
+    <row r="208" spans="1:150">
       <c r="A208" s="1">
         <v>44378</v>
       </c>
@@ -67429,8 +68050,11 @@
       <c r="ES208">
         <v>104.16</v>
       </c>
+      <c r="ET208">
+        <v>104.16</v>
+      </c>
     </row>
-    <row r="209" spans="1:149">
+    <row r="209" spans="1:150">
       <c r="A209" s="1">
         <v>44470</v>
       </c>
@@ -67479,8 +68103,11 @@
       <c r="ES209">
         <v>104.72</v>
       </c>
+      <c r="ET209">
+        <v>104.72</v>
+      </c>
     </row>
-    <row r="210" spans="1:149">
+    <row r="210" spans="1:150">
       <c r="A210" s="1">
         <v>44562</v>
       </c>
@@ -67526,8 +68153,11 @@
       <c r="ES210">
         <v>105.43</v>
       </c>
+      <c r="ET210">
+        <v>105.43</v>
+      </c>
     </row>
-    <row r="211" spans="1:149">
+    <row r="211" spans="1:150">
       <c r="A211" s="1">
         <v>44652</v>
       </c>
@@ -67570,8 +68200,11 @@
       <c r="ES211">
         <v>105.59</v>
       </c>
+      <c r="ET211">
+        <v>105.59</v>
+      </c>
     </row>
-    <row r="212" spans="1:149">
+    <row r="212" spans="1:150">
       <c r="A212" s="1">
         <v>44743</v>
       </c>
@@ -67611,8 +68244,11 @@
       <c r="ES212">
         <v>105.9</v>
       </c>
+      <c r="ET212">
+        <v>105.9</v>
+      </c>
     </row>
-    <row r="213" spans="1:149">
+    <row r="213" spans="1:150">
       <c r="A213" s="1">
         <v>44835</v>
       </c>
@@ -67649,8 +68285,11 @@
       <c r="ES213">
         <v>105.53</v>
       </c>
+      <c r="ET213">
+        <v>105.53</v>
+      </c>
     </row>
-    <row r="214" spans="1:149">
+    <row r="214" spans="1:150">
       <c r="A214" s="1">
         <v>44927</v>
       </c>
@@ -67684,8 +68323,11 @@
       <c r="ES214">
         <v>105.03</v>
       </c>
+      <c r="ET214">
+        <v>105.03</v>
+      </c>
     </row>
-    <row r="215" spans="1:149">
+    <row r="215" spans="1:150">
       <c r="A215" s="1">
         <v>45017</v>
       </c>
@@ -67716,8 +68358,11 @@
       <c r="ES215">
         <v>104.95</v>
       </c>
+      <c r="ET215">
+        <v>104.95</v>
+      </c>
     </row>
-    <row r="216" spans="1:149">
+    <row r="216" spans="1:150">
       <c r="A216" s="1">
         <v>45108</v>
       </c>
@@ -67745,8 +68390,11 @@
       <c r="ES216">
         <v>104.95</v>
       </c>
+      <c r="ET216">
+        <v>104.95</v>
+      </c>
     </row>
-    <row r="217" spans="1:149">
+    <row r="217" spans="1:150">
       <c r="A217" s="1">
         <v>45200</v>
       </c>
@@ -67771,8 +68419,11 @@
       <c r="ES217">
         <v>104.66</v>
       </c>
+      <c r="ET217">
+        <v>104.66</v>
+      </c>
     </row>
-    <row r="218" spans="1:149">
+    <row r="218" spans="1:150">
       <c r="A218" s="1">
         <v>45292</v>
       </c>
@@ -67794,8 +68445,11 @@
       <c r="ES218">
         <v>104.55</v>
       </c>
+      <c r="ET218">
+        <v>104.55</v>
+      </c>
     </row>
-    <row r="219" spans="1:149">
+    <row r="219" spans="1:150">
       <c r="A219" s="1">
         <v>45383</v>
       </c>
@@ -67814,8 +68468,11 @@
       <c r="ES219">
         <v>104.28</v>
       </c>
+      <c r="ET219">
+        <v>104.28</v>
+      </c>
     </row>
-    <row r="220" spans="1:149">
+    <row r="220" spans="1:150">
       <c r="A220" s="1">
         <v>45474</v>
       </c>
@@ -67831,8 +68488,11 @@
       <c r="ES220">
         <v>104.3</v>
       </c>
+      <c r="ET220">
+        <v>104.3</v>
+      </c>
     </row>
-    <row r="221" spans="1:149">
+    <row r="221" spans="1:150">
       <c r="A221" s="1">
         <v>45566</v>
       </c>
@@ -67845,8 +68505,11 @@
       <c r="ES221">
         <v>104.49</v>
       </c>
+      <c r="ET221">
+        <v>104.49</v>
+      </c>
     </row>
-    <row r="222" spans="1:149">
+    <row r="222" spans="1:150">
       <c r="A222" s="1">
         <v>45658</v>
       </c>
@@ -67856,18 +68519,32 @@
       <c r="ES222">
         <v>104.81</v>
       </c>
+      <c r="ET222">
+        <v>104.81</v>
+      </c>
     </row>
-    <row r="223" spans="1:149">
+    <row r="223" spans="1:150">
       <c r="A223" s="1">
         <v>45748</v>
       </c>
       <c r="ES223">
         <v>104.52</v>
       </c>
+      <c r="ET223">
+        <v>104.59</v>
+      </c>
     </row>
-    <row r="224" spans="1:149">
+    <row r="224" spans="1:150">
       <c r="A224" s="1">
         <v>45839</v>
+      </c>
+      <c r="ET224">
+        <v>104.59</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="1">
+        <v>45931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixed the naive forecaster component module
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
@@ -11,6 +11,683 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
+  <si>
+    <t>1970Q1</t>
+  </si>
+  <si>
+    <t>1970Q2</t>
+  </si>
+  <si>
+    <t>1970Q3</t>
+  </si>
+  <si>
+    <t>1970Q4</t>
+  </si>
+  <si>
+    <t>1971Q1</t>
+  </si>
+  <si>
+    <t>1971Q2</t>
+  </si>
+  <si>
+    <t>1971Q3</t>
+  </si>
+  <si>
+    <t>1971Q4</t>
+  </si>
+  <si>
+    <t>1972Q1</t>
+  </si>
+  <si>
+    <t>1972Q2</t>
+  </si>
+  <si>
+    <t>1972Q3</t>
+  </si>
+  <si>
+    <t>1972Q4</t>
+  </si>
+  <si>
+    <t>1973Q1</t>
+  </si>
+  <si>
+    <t>1973Q2</t>
+  </si>
+  <si>
+    <t>1973Q3</t>
+  </si>
+  <si>
+    <t>1973Q4</t>
+  </si>
+  <si>
+    <t>1974Q1</t>
+  </si>
+  <si>
+    <t>1974Q2</t>
+  </si>
+  <si>
+    <t>1974Q3</t>
+  </si>
+  <si>
+    <t>1974Q4</t>
+  </si>
+  <si>
+    <t>1975Q1</t>
+  </si>
+  <si>
+    <t>1975Q2</t>
+  </si>
+  <si>
+    <t>1975Q3</t>
+  </si>
+  <si>
+    <t>1975Q4</t>
+  </si>
+  <si>
+    <t>1976Q1</t>
+  </si>
+  <si>
+    <t>1976Q2</t>
+  </si>
+  <si>
+    <t>1976Q3</t>
+  </si>
+  <si>
+    <t>1976Q4</t>
+  </si>
+  <si>
+    <t>1977Q1</t>
+  </si>
+  <si>
+    <t>1977Q2</t>
+  </si>
+  <si>
+    <t>1977Q3</t>
+  </si>
+  <si>
+    <t>1977Q4</t>
+  </si>
+  <si>
+    <t>1978Q1</t>
+  </si>
+  <si>
+    <t>1978Q2</t>
+  </si>
+  <si>
+    <t>1978Q3</t>
+  </si>
+  <si>
+    <t>1978Q4</t>
+  </si>
+  <si>
+    <t>1979Q1</t>
+  </si>
+  <si>
+    <t>1979Q2</t>
+  </si>
+  <si>
+    <t>1979Q3</t>
+  </si>
+  <si>
+    <t>1979Q4</t>
+  </si>
+  <si>
+    <t>1980Q1</t>
+  </si>
+  <si>
+    <t>1980Q2</t>
+  </si>
+  <si>
+    <t>1980Q3</t>
+  </si>
+  <si>
+    <t>1980Q4</t>
+  </si>
+  <si>
+    <t>1981Q1</t>
+  </si>
+  <si>
+    <t>1981Q2</t>
+  </si>
+  <si>
+    <t>1981Q3</t>
+  </si>
+  <si>
+    <t>1981Q4</t>
+  </si>
+  <si>
+    <t>1982Q1</t>
+  </si>
+  <si>
+    <t>1982Q2</t>
+  </si>
+  <si>
+    <t>1982Q3</t>
+  </si>
+  <si>
+    <t>1982Q4</t>
+  </si>
+  <si>
+    <t>1983Q1</t>
+  </si>
+  <si>
+    <t>1983Q2</t>
+  </si>
+  <si>
+    <t>1983Q3</t>
+  </si>
+  <si>
+    <t>1983Q4</t>
+  </si>
+  <si>
+    <t>1984Q1</t>
+  </si>
+  <si>
+    <t>1984Q2</t>
+  </si>
+  <si>
+    <t>1984Q3</t>
+  </si>
+  <si>
+    <t>1984Q4</t>
+  </si>
+  <si>
+    <t>1985Q1</t>
+  </si>
+  <si>
+    <t>1985Q2</t>
+  </si>
+  <si>
+    <t>1985Q3</t>
+  </si>
+  <si>
+    <t>1985Q4</t>
+  </si>
+  <si>
+    <t>1986Q1</t>
+  </si>
+  <si>
+    <t>1986Q2</t>
+  </si>
+  <si>
+    <t>1986Q3</t>
+  </si>
+  <si>
+    <t>1986Q4</t>
+  </si>
+  <si>
+    <t>1987Q1</t>
+  </si>
+  <si>
+    <t>1987Q2</t>
+  </si>
+  <si>
+    <t>1987Q3</t>
+  </si>
+  <si>
+    <t>1987Q4</t>
+  </si>
+  <si>
+    <t>1988Q1</t>
+  </si>
+  <si>
+    <t>1988Q2</t>
+  </si>
+  <si>
+    <t>1988Q3</t>
+  </si>
+  <si>
+    <t>1988Q4</t>
+  </si>
+  <si>
+    <t>1989Q1</t>
+  </si>
+  <si>
+    <t>1989Q2</t>
+  </si>
+  <si>
+    <t>1989Q3</t>
+  </si>
+  <si>
+    <t>1989Q4</t>
+  </si>
+  <si>
+    <t>1990Q1</t>
+  </si>
+  <si>
+    <t>1990Q2</t>
+  </si>
+  <si>
+    <t>1990Q3</t>
+  </si>
+  <si>
+    <t>1990Q4</t>
+  </si>
+  <si>
+    <t>1991Q1</t>
+  </si>
+  <si>
+    <t>1991Q2</t>
+  </si>
+  <si>
+    <t>1991Q3</t>
+  </si>
+  <si>
+    <t>1991Q4</t>
+  </si>
+  <si>
+    <t>1992Q1</t>
+  </si>
+  <si>
+    <t>1992Q2</t>
+  </si>
+  <si>
+    <t>1992Q3</t>
+  </si>
+  <si>
+    <t>1992Q4</t>
+  </si>
+  <si>
+    <t>1993Q1</t>
+  </si>
+  <si>
+    <t>1993Q2</t>
+  </si>
+  <si>
+    <t>1993Q3</t>
+  </si>
+  <si>
+    <t>1993Q4</t>
+  </si>
+  <si>
+    <t>1994Q1</t>
+  </si>
+  <si>
+    <t>1994Q2</t>
+  </si>
+  <si>
+    <t>1994Q3</t>
+  </si>
+  <si>
+    <t>1994Q4</t>
+  </si>
+  <si>
+    <t>1995Q1</t>
+  </si>
+  <si>
+    <t>1995Q2</t>
+  </si>
+  <si>
+    <t>1995Q3</t>
+  </si>
+  <si>
+    <t>1995Q4</t>
+  </si>
+  <si>
+    <t>1996Q1</t>
+  </si>
+  <si>
+    <t>1996Q2</t>
+  </si>
+  <si>
+    <t>1996Q3</t>
+  </si>
+  <si>
+    <t>1996Q4</t>
+  </si>
+  <si>
+    <t>1997Q1</t>
+  </si>
+  <si>
+    <t>1997Q2</t>
+  </si>
+  <si>
+    <t>1997Q3</t>
+  </si>
+  <si>
+    <t>1997Q4</t>
+  </si>
+  <si>
+    <t>1998Q1</t>
+  </si>
+  <si>
+    <t>1998Q2</t>
+  </si>
+  <si>
+    <t>1998Q3</t>
+  </si>
+  <si>
+    <t>1998Q4</t>
+  </si>
+  <si>
+    <t>1999Q1</t>
+  </si>
+  <si>
+    <t>1999Q2</t>
+  </si>
+  <si>
+    <t>1999Q3</t>
+  </si>
+  <si>
+    <t>1999Q4</t>
+  </si>
+  <si>
+    <t>2000Q1</t>
+  </si>
+  <si>
+    <t>2000Q2</t>
+  </si>
+  <si>
+    <t>2000Q3</t>
+  </si>
+  <si>
+    <t>2000Q4</t>
+  </si>
+  <si>
+    <t>2001Q1</t>
+  </si>
+  <si>
+    <t>2001Q2</t>
+  </si>
+  <si>
+    <t>2001Q3</t>
+  </si>
+  <si>
+    <t>2001Q4</t>
+  </si>
+  <si>
+    <t>2002Q1</t>
+  </si>
+  <si>
+    <t>2002Q2</t>
+  </si>
+  <si>
+    <t>2002Q3</t>
+  </si>
+  <si>
+    <t>2002Q4</t>
+  </si>
+  <si>
+    <t>2003Q1</t>
+  </si>
+  <si>
+    <t>2003Q2</t>
+  </si>
+  <si>
+    <t>2003Q3</t>
+  </si>
+  <si>
+    <t>2003Q4</t>
+  </si>
+  <si>
+    <t>2004Q1</t>
+  </si>
+  <si>
+    <t>2004Q2</t>
+  </si>
+  <si>
+    <t>2004Q3</t>
+  </si>
+  <si>
+    <t>2004Q4</t>
+  </si>
+  <si>
+    <t>2005Q1</t>
+  </si>
+  <si>
+    <t>2005Q2</t>
+  </si>
+  <si>
+    <t>2005Q3</t>
+  </si>
+  <si>
+    <t>2005Q4</t>
+  </si>
+  <si>
+    <t>2006Q1</t>
+  </si>
+  <si>
+    <t>2006Q2</t>
+  </si>
+  <si>
+    <t>2006Q3</t>
+  </si>
+  <si>
+    <t>2006Q4</t>
+  </si>
+  <si>
+    <t>2007Q1</t>
+  </si>
+  <si>
+    <t>2007Q2</t>
+  </si>
+  <si>
+    <t>2007Q3</t>
+  </si>
+  <si>
+    <t>2007Q4</t>
+  </si>
+  <si>
+    <t>2008Q1</t>
+  </si>
+  <si>
+    <t>2008Q2</t>
+  </si>
+  <si>
+    <t>2008Q3</t>
+  </si>
+  <si>
+    <t>2008Q4</t>
+  </si>
+  <si>
+    <t>2009Q1</t>
+  </si>
+  <si>
+    <t>2009Q2</t>
+  </si>
+  <si>
+    <t>2009Q3</t>
+  </si>
+  <si>
+    <t>2009Q4</t>
+  </si>
+  <si>
+    <t>2010Q1</t>
+  </si>
+  <si>
+    <t>2010Q2</t>
+  </si>
+  <si>
+    <t>2010Q3</t>
+  </si>
+  <si>
+    <t>2010Q4</t>
+  </si>
+  <si>
+    <t>2011Q1</t>
+  </si>
+  <si>
+    <t>2011Q2</t>
+  </si>
+  <si>
+    <t>2011Q3</t>
+  </si>
+  <si>
+    <t>2011Q4</t>
+  </si>
+  <si>
+    <t>2012Q1</t>
+  </si>
+  <si>
+    <t>2012Q2</t>
+  </si>
+  <si>
+    <t>2012Q3</t>
+  </si>
+  <si>
+    <t>2012Q4</t>
+  </si>
+  <si>
+    <t>2013Q1</t>
+  </si>
+  <si>
+    <t>2013Q2</t>
+  </si>
+  <si>
+    <t>2013Q3</t>
+  </si>
+  <si>
+    <t>2013Q4</t>
+  </si>
+  <si>
+    <t>2014Q1</t>
+  </si>
+  <si>
+    <t>2014Q2</t>
+  </si>
+  <si>
+    <t>2014Q3</t>
+  </si>
+  <si>
+    <t>2014Q4</t>
+  </si>
+  <si>
+    <t>2015Q1</t>
+  </si>
+  <si>
+    <t>2015Q2</t>
+  </si>
+  <si>
+    <t>2015Q3</t>
+  </si>
+  <si>
+    <t>2015Q4</t>
+  </si>
+  <si>
+    <t>2016Q1</t>
+  </si>
+  <si>
+    <t>2016Q2</t>
+  </si>
+  <si>
+    <t>2016Q3</t>
+  </si>
+  <si>
+    <t>2016Q4</t>
+  </si>
+  <si>
+    <t>2017Q1</t>
+  </si>
+  <si>
+    <t>2017Q2</t>
+  </si>
+  <si>
+    <t>2017Q3</t>
+  </si>
+  <si>
+    <t>2017Q4</t>
+  </si>
+  <si>
+    <t>2018Q1</t>
+  </si>
+  <si>
+    <t>2018Q2</t>
+  </si>
+  <si>
+    <t>2018Q3</t>
+  </si>
+  <si>
+    <t>2018Q4</t>
+  </si>
+  <si>
+    <t>2019Q1</t>
+  </si>
+  <si>
+    <t>2019Q2</t>
+  </si>
+  <si>
+    <t>2019Q3</t>
+  </si>
+  <si>
+    <t>2019Q4</t>
+  </si>
+  <si>
+    <t>2020Q1</t>
+  </si>
+  <si>
+    <t>2020Q2</t>
+  </si>
+  <si>
+    <t>2020Q3</t>
+  </si>
+  <si>
+    <t>2020Q4</t>
+  </si>
+  <si>
+    <t>2021Q1</t>
+  </si>
+  <si>
+    <t>2021Q2</t>
+  </si>
+  <si>
+    <t>2021Q3</t>
+  </si>
+  <si>
+    <t>2021Q4</t>
+  </si>
+  <si>
+    <t>2022Q1</t>
+  </si>
+  <si>
+    <t>2022Q2</t>
+  </si>
+  <si>
+    <t>2022Q3</t>
+  </si>
+  <si>
+    <t>2022Q4</t>
+  </si>
+  <si>
+    <t>2023Q1</t>
+  </si>
+  <si>
+    <t>2023Q2</t>
+  </si>
+  <si>
+    <t>2023Q3</t>
+  </si>
+  <si>
+    <t>2023Q4</t>
+  </si>
+  <si>
+    <t>2024Q1</t>
+  </si>
+  <si>
+    <t>2024Q2</t>
+  </si>
+  <si>
+    <t>2024Q3</t>
+  </si>
+  <si>
+    <t>2024Q4</t>
+  </si>
+  <si>
+    <t>2025Q1</t>
+  </si>
+  <si>
+    <t>2025Q2</t>
+  </si>
+  <si>
+    <t>2025Q3</t>
+  </si>
+  <si>
+    <t>2025Q4</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70,9 +747,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -825,8 +1505,8 @@
       </c>
     </row>
     <row r="2" spans="1:150">
-      <c r="A2" s="1">
-        <v>25569</v>
+      <c r="A2" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>78.38903449704861</v>
@@ -1277,8 +1957,8 @@
       </c>
     </row>
     <row r="3" spans="1:150">
-      <c r="A3" s="1">
-        <v>25659</v>
+      <c r="A3" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>81.48467836391049</v>
@@ -1729,8 +2409,8 @@
       </c>
     </row>
     <row r="4" spans="1:150">
-      <c r="A4" s="1">
-        <v>25750</v>
+      <c r="A4" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>83.01213421926997</v>
@@ -2181,8 +2861,8 @@
       </c>
     </row>
     <row r="5" spans="1:150">
-      <c r="A5" s="1">
-        <v>25842</v>
+      <c r="A5" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>83.72494695177107</v>
@@ -2633,8 +3313,8 @@
       </c>
     </row>
     <row r="6" spans="1:150">
-      <c r="A6" s="1">
-        <v>25934</v>
+      <c r="A6" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B6">
         <v>82.09566070605429</v>
@@ -3085,8 +3765,8 @@
       </c>
     </row>
     <row r="7" spans="1:150">
-      <c r="A7" s="1">
-        <v>26024</v>
+      <c r="A7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B7">
         <v>83.84714342019983</v>
@@ -3537,8 +4217,8 @@
       </c>
     </row>
     <row r="8" spans="1:150">
-      <c r="A8" s="1">
-        <v>26115</v>
+      <c r="A8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="B8">
         <v>85.27276888520201</v>
@@ -3989,8 +4669,8 @@
       </c>
     </row>
     <row r="9" spans="1:150">
-      <c r="A9" s="1">
-        <v>26207</v>
+      <c r="A9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="B9">
         <v>85.19130457291617</v>
@@ -4441,8 +5121,8 @@
       </c>
     </row>
     <row r="10" spans="1:150">
-      <c r="A10" s="1">
-        <v>26299</v>
+      <c r="A10" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="B10">
         <v>85.27276888520201</v>
@@ -4893,8 +5573,8 @@
       </c>
     </row>
     <row r="11" spans="1:150">
-      <c r="A11" s="1">
-        <v>26390</v>
+      <c r="A11" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B11">
         <v>86.67802827213274</v>
@@ -5345,8 +6025,8 @@
       </c>
     </row>
     <row r="12" spans="1:150">
-      <c r="A12" s="1">
-        <v>26481</v>
+      <c r="A12" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>88.69427000120724</v>
@@ -5797,8 +6477,8 @@
       </c>
     </row>
     <row r="13" spans="1:150">
-      <c r="A13" s="1">
-        <v>26573</v>
+      <c r="A13" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B13">
         <v>90.05879723199506</v>
@@ -6249,8 +6929,8 @@
       </c>
     </row>
     <row r="14" spans="1:150">
-      <c r="A14" s="1">
-        <v>26665</v>
+      <c r="A14" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B14">
         <v>91.36222622856847</v>
@@ -6701,8 +7381,8 @@
       </c>
     </row>
     <row r="15" spans="1:150">
-      <c r="A15" s="1">
-        <v>26755</v>
+      <c r="A15" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B15">
         <v>91.99357464878373</v>
@@ -7153,8 +7833,8 @@
       </c>
     </row>
     <row r="16" spans="1:150">
-      <c r="A16" s="1">
-        <v>26846</v>
+      <c r="A16" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="B16">
         <v>92.31943189792709</v>
@@ -7605,8 +8285,8 @@
       </c>
     </row>
     <row r="17" spans="1:150">
-      <c r="A17" s="1">
-        <v>26938</v>
+      <c r="A17" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B17">
         <v>92.52309267864169</v>
@@ -8057,8 +8737,8 @@
       </c>
     </row>
     <row r="18" spans="1:150">
-      <c r="A18" s="1">
-        <v>27030</v>
+      <c r="A18" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B18">
         <v>93.29700364535717</v>
@@ -8509,8 +9189,8 @@
       </c>
     </row>
     <row r="19" spans="1:150">
-      <c r="A19" s="1">
-        <v>27120</v>
+      <c r="A19" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="B19">
         <v>93.21553933307132</v>
@@ -8961,8 +9641,8 @@
       </c>
     </row>
     <row r="20" spans="1:150">
-      <c r="A20" s="1">
-        <v>27211</v>
+      <c r="A20" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="B20">
         <v>93.23590541114278</v>
@@ -9413,8 +10093,8 @@
       </c>
     </row>
     <row r="21" spans="1:150">
-      <c r="A21" s="1">
-        <v>27303</v>
+      <c r="A21" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="B21">
         <v>92.07503896106957</v>
@@ -9865,8 +10545,8 @@
       </c>
     </row>
     <row r="22" spans="1:150">
-      <c r="A22" s="1">
-        <v>27395</v>
+      <c r="A22" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="B22">
         <v>91.54552093121163</v>
@@ -10317,8 +10997,8 @@
       </c>
     </row>
     <row r="23" spans="1:150">
-      <c r="A23" s="1">
-        <v>27485</v>
+      <c r="A23" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="B23">
         <v>91.07710113556804</v>
@@ -10769,8 +11449,8 @@
       </c>
     </row>
     <row r="24" spans="1:150">
-      <c r="A24" s="1">
-        <v>27576</v>
+      <c r="A24" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B24">
         <v>92.07503896106957</v>
@@ -11221,8 +11901,8 @@
       </c>
     </row>
     <row r="25" spans="1:150">
-      <c r="A25" s="1">
-        <v>27668</v>
+      <c r="A25" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B25">
         <v>93.88761990942949</v>
@@ -11673,8 +12353,8 @@
       </c>
     </row>
     <row r="26" spans="1:150">
-      <c r="A26" s="1">
-        <v>27760</v>
+      <c r="A26" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B26">
         <v>94.70226303228787</v>
@@ -12125,8 +12805,8 @@
       </c>
     </row>
     <row r="27" spans="1:150">
-      <c r="A27" s="1">
-        <v>27851</v>
+      <c r="A27" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B27">
         <v>96.12788849729007</v>
@@ -12577,8 +13257,8 @@
       </c>
     </row>
     <row r="28" spans="1:150">
-      <c r="A28" s="1">
-        <v>27942</v>
+      <c r="A28" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B28">
         <v>96.14825457536152</v>
@@ -13029,8 +13709,8 @@
       </c>
     </row>
     <row r="29" spans="1:150">
-      <c r="A29" s="1">
-        <v>28034</v>
+      <c r="A29" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B29">
         <v>97.94046944564998</v>
@@ -13481,8 +14161,8 @@
       </c>
     </row>
     <row r="30" spans="1:150">
-      <c r="A30" s="1">
-        <v>28126</v>
+      <c r="A30" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B30">
         <v>98.79584472465129</v>
@@ -13933,8 +14613,8 @@
       </c>
     </row>
     <row r="31" spans="1:150">
-      <c r="A31" s="1">
-        <v>28216</v>
+      <c r="A31" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B31">
         <v>99.3457288325807</v>
@@ -14385,8 +15065,8 @@
       </c>
     </row>
     <row r="32" spans="1:150">
-      <c r="A32" s="1">
-        <v>28307</v>
+      <c r="A32" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B32">
         <v>99.30499667643778</v>
@@ -14837,8 +15517,8 @@
       </c>
     </row>
     <row r="33" spans="1:150">
-      <c r="A33" s="1">
-        <v>28399</v>
+      <c r="A33" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B33">
         <v>101.0157472344404</v>
@@ -15289,8 +15969,8 @@
       </c>
     </row>
     <row r="34" spans="1:150">
-      <c r="A34" s="1">
-        <v>28491</v>
+      <c r="A34" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B34">
         <v>101.4230687958696</v>
@@ -15741,8 +16421,8 @@
       </c>
     </row>
     <row r="35" spans="1:150">
-      <c r="A35" s="1">
-        <v>28581</v>
+      <c r="A35" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B35">
         <v>101.8507564353702</v>
@@ -16193,8 +16873,8 @@
       </c>
     </row>
     <row r="36" spans="1:150">
-      <c r="A36" s="1">
-        <v>28672</v>
+      <c r="A36" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B36">
         <v>103.1745515100151</v>
@@ -16645,8 +17325,8 @@
       </c>
     </row>
     <row r="37" spans="1:150">
-      <c r="A37" s="1">
-        <v>28764</v>
+      <c r="A37" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B37">
         <v>104.3761501162313</v>
@@ -17097,8 +17777,8 @@
       </c>
     </row>
     <row r="38" spans="1:150">
-      <c r="A38" s="1">
-        <v>28856</v>
+      <c r="A38" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B38">
         <v>104.5187126627315</v>
@@ -17549,8 +18229,8 @@
       </c>
     </row>
     <row r="39" spans="1:150">
-      <c r="A39" s="1">
-        <v>28946</v>
+      <c r="A39" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B39">
         <v>107.7569190760936</v>
@@ -18001,8 +18681,8 @@
       </c>
     </row>
     <row r="40" spans="1:150">
-      <c r="A40" s="1">
-        <v>29037</v>
+      <c r="A40" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B40">
         <v>107.7569190760936</v>
@@ -18453,8 +19133,8 @@
       </c>
     </row>
     <row r="41" spans="1:150">
-      <c r="A41" s="1">
-        <v>29129</v>
+      <c r="A41" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B41">
         <v>108.4289996524518</v>
@@ -18905,8 +19585,8 @@
       </c>
     </row>
     <row r="42" spans="1:150">
-      <c r="A42" s="1">
-        <v>29221</v>
+      <c r="A42" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="B42">
         <v>109.2843749314531</v>
@@ -19357,8 +20037,8 @@
       </c>
     </row>
     <row r="43" spans="1:150">
-      <c r="A43" s="1">
-        <v>29312</v>
+      <c r="A43" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B43">
         <v>108.571562198952</v>
@@ -19809,8 +20489,8 @@
       </c>
     </row>
     <row r="44" spans="1:150">
-      <c r="A44" s="1">
-        <v>29403</v>
+      <c r="A44" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="B44">
         <v>108.1235084813799</v>
@@ -20261,8 +20941,8 @@
       </c>
     </row>
     <row r="45" spans="1:150">
-      <c r="A45" s="1">
-        <v>29495</v>
+      <c r="A45" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B45">
         <v>107.9809459348796</v>
@@ -20713,8 +21393,8 @@
       </c>
     </row>
     <row r="46" spans="1:150">
-      <c r="A46" s="1">
-        <v>29587</v>
+      <c r="A46" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B46">
         <v>109.2843749314531</v>
@@ -21165,8 +21845,8 @@
       </c>
     </row>
     <row r="47" spans="1:150">
-      <c r="A47" s="1">
-        <v>29677</v>
+      <c r="A47" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="B47">
         <v>108.9992498384526</v>
@@ -21617,8 +22297,8 @@
       </c>
     </row>
     <row r="48" spans="1:150">
-      <c r="A48" s="1">
-        <v>29768</v>
+      <c r="A48" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B48">
         <v>109.3047410095245</v>
@@ -22069,8 +22749,8 @@
       </c>
     </row>
     <row r="49" spans="1:150">
-      <c r="A49" s="1">
-        <v>29860</v>
+      <c r="A49" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="B49">
         <v>109.1825445410958</v>
@@ -22521,8 +23201,8 @@
       </c>
     </row>
     <row r="50" spans="1:150">
-      <c r="A50" s="1">
-        <v>29952</v>
+      <c r="A50" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B50">
         <v>109.6305982586679</v>
@@ -22973,8 +23653,8 @@
       </c>
     </row>
     <row r="51" spans="1:150">
-      <c r="A51" s="1">
-        <v>30042</v>
+      <c r="A51" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B51">
         <v>108.9381516042383</v>
@@ -23425,8 +24105,8 @@
       </c>
     </row>
     <row r="52" spans="1:150">
-      <c r="A52" s="1">
-        <v>30133</v>
+      <c r="A52" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B52">
         <v>107.8994816225938</v>
@@ -23877,8 +24557,8 @@
       </c>
     </row>
     <row r="53" spans="1:150">
-      <c r="A53" s="1">
-        <v>30225</v>
+      <c r="A53" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B53">
         <v>108.1235084813799</v>
@@ -24329,8 +25009,8 @@
       </c>
     </row>
     <row r="54" spans="1:150">
-      <c r="A54" s="1">
-        <v>30317</v>
+      <c r="A54" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="B54">
         <v>109.1214463068814</v>
@@ -24781,8 +25461,8 @@
       </c>
     </row>
     <row r="55" spans="1:150">
-      <c r="A55" s="1">
-        <v>30407</v>
+      <c r="A55" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="B55">
         <v>110.2823127569546</v>
@@ -25233,8 +25913,8 @@
       </c>
     </row>
     <row r="56" spans="1:150">
-      <c r="A56" s="1">
-        <v>30498</v>
+      <c r="A56" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B56">
         <v>110.0175537420256</v>
@@ -25685,8 +26365,8 @@
       </c>
     </row>
     <row r="57" spans="1:150">
-      <c r="A57" s="1">
-        <v>30590</v>
+      <c r="A57" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="B57">
         <v>111.5450095973851</v>
@@ -26137,8 +26817,8 @@
       </c>
     </row>
     <row r="58" spans="1:150">
-      <c r="A58" s="1">
-        <v>30682</v>
+      <c r="A58" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B58">
         <v>113.0113672185302</v>
@@ -26589,8 +27269,8 @@
       </c>
     </row>
     <row r="59" spans="1:150">
-      <c r="A59" s="1">
-        <v>30773</v>
+      <c r="A59" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="B59">
         <v>111.2395184263132</v>
@@ -27041,8 +27721,8 @@
       </c>
     </row>
     <row r="60" spans="1:150">
-      <c r="A60" s="1">
-        <v>30864</v>
+      <c r="A60" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B60">
         <v>114.2740640589607</v>
@@ -27493,8 +28173,8 @@
       </c>
     </row>
     <row r="61" spans="1:150">
-      <c r="A61" s="1">
-        <v>30956</v>
+      <c r="A61" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B61">
         <v>115.2312697283193</v>
@@ -27945,8 +28625,8 @@
       </c>
     </row>
     <row r="62" spans="1:150">
-      <c r="A62" s="1">
-        <v>31048</v>
+      <c r="A62" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="B62">
         <v>114.6202873861755</v>
@@ -28397,8 +29077,8 @@
       </c>
     </row>
     <row r="63" spans="1:150">
-      <c r="A63" s="1">
-        <v>31138</v>
+      <c r="A63" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="B63">
         <v>115.7404216801058</v>
@@ -28849,8 +29529,8 @@
       </c>
     </row>
     <row r="64" spans="1:150">
-      <c r="A64" s="1">
-        <v>31229</v>
+      <c r="A64" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="B64">
         <v>117.2475114573938</v>
@@ -29301,8 +29981,8 @@
       </c>
     </row>
     <row r="65" spans="1:150">
-      <c r="A65" s="1">
-        <v>31321</v>
+      <c r="A65" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="B65">
         <v>117.9603241898949</v>
@@ -29753,8 +30433,8 @@
       </c>
     </row>
     <row r="66" spans="1:150">
-      <c r="A66" s="1">
-        <v>31413</v>
+      <c r="A66" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="B66">
         <v>117.2882436135368</v>
@@ -30205,8 +30885,8 @@
       </c>
     </row>
     <row r="67" spans="1:150">
-      <c r="A67" s="1">
-        <v>31503</v>
+      <c r="A67" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="B67">
         <v>118.6527708443246</v>
@@ -30657,8 +31337,8 @@
       </c>
     </row>
     <row r="68" spans="1:150">
-      <c r="A68" s="1">
-        <v>31594</v>
+      <c r="A68" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B68">
         <v>119.5285122013973</v>
@@ -31109,8 +31789,8 @@
       </c>
     </row>
     <row r="69" spans="1:150">
-      <c r="A69" s="1">
-        <v>31686</v>
+      <c r="A69" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B69">
         <v>120.709744729542</v>
@@ -31561,8 +32241,8 @@
       </c>
     </row>
     <row r="70" spans="1:150">
-      <c r="A70" s="1">
-        <v>31778</v>
+      <c r="A70" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B70">
         <v>117.6751990968945</v>
@@ -32013,8 +32693,8 @@
       </c>
     </row>
     <row r="71" spans="1:150">
-      <c r="A71" s="1">
-        <v>31868</v>
+      <c r="A71" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B71">
         <v>120.3227892461843</v>
@@ -32465,8 +33145,8 @@
       </c>
     </row>
     <row r="72" spans="1:150">
-      <c r="A72" s="1">
-        <v>31959</v>
+      <c r="A72" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B72">
         <v>121.1781645251856</v>
@@ -32917,8 +33597,8 @@
       </c>
     </row>
     <row r="73" spans="1:150">
-      <c r="A73" s="1">
-        <v>32051</v>
+      <c r="A73" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B73">
         <v>123.0925758639028</v>
@@ -33369,8 +34049,8 @@
       </c>
     </row>
     <row r="74" spans="1:150">
-      <c r="A74" s="1">
-        <v>32143</v>
+      <c r="A74" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B74">
         <v>121.992807648044</v>
@@ -33821,8 +34501,8 @@
       </c>
     </row>
     <row r="75" spans="1:150">
-      <c r="A75" s="1">
-        <v>32234</v>
+      <c r="A75" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B75">
         <v>124.2127101578331</v>
@@ -34273,8 +34953,8 @@
       </c>
     </row>
     <row r="76" spans="1:150">
-      <c r="A76" s="1">
-        <v>32325</v>
+      <c r="A76" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="B76">
         <v>125.5772373886209</v>
@@ -34725,8 +35405,8 @@
       </c>
     </row>
     <row r="77" spans="1:150">
-      <c r="A77" s="1">
-        <v>32417</v>
+      <c r="A77" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C77">
         <v>127.0843271659089</v>
@@ -35174,8 +35854,8 @@
       </c>
     </row>
     <row r="78" spans="1:150">
-      <c r="A78" s="1">
-        <v>32509</v>
+      <c r="A78" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="D78">
         <v>128.3877561624823</v>
@@ -35620,8 +36300,8 @@
       </c>
     </row>
     <row r="79" spans="1:150">
-      <c r="A79" s="1">
-        <v>32599</v>
+      <c r="A79" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="E79">
         <v>128.9172741923403</v>
@@ -36063,8 +36743,8 @@
       </c>
     </row>
     <row r="80" spans="1:150">
-      <c r="A80" s="1">
-        <v>32690</v>
+      <c r="A80" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="F80">
         <v>130.0781406424135</v>
@@ -36503,8 +37183,8 @@
       </c>
     </row>
     <row r="81" spans="1:150">
-      <c r="A81" s="1">
-        <v>32782</v>
+      <c r="A81" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="G81">
         <v>131.605596497773</v>
@@ -36940,8 +37620,8 @@
       </c>
     </row>
     <row r="82" spans="1:150">
-      <c r="A82" s="1">
-        <v>32874</v>
+      <c r="A82" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="H82">
         <v>134.3346509593486</v>
@@ -37374,8 +38054,8 @@
       </c>
     </row>
     <row r="83" spans="1:150">
-      <c r="A83" s="1">
-        <v>32964</v>
+      <c r="A83" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="I83">
         <v>134.9863654576353</v>
@@ -37805,8 +38485,8 @@
       </c>
     </row>
     <row r="84" spans="1:150">
-      <c r="A84" s="1">
-        <v>33055</v>
+      <c r="A84" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="J84">
         <v>137.8376163876397</v>
@@ -38233,8 +38913,8 @@
       </c>
     </row>
     <row r="85" spans="1:150">
-      <c r="A85" s="1">
-        <v>33147</v>
+      <c r="A85" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="K85">
         <v>140.2815457562148</v>
@@ -38658,8 +39338,8 @@
       </c>
     </row>
     <row r="86" spans="1:150">
-      <c r="A86" s="1">
-        <v>33239</v>
+      <c r="A86" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="L86">
         <v>144.1511005897922</v>
@@ -39080,8 +39760,8 @@
       </c>
     </row>
     <row r="87" spans="1:150">
-      <c r="A87" s="1">
-        <v>33329</v>
+      <c r="A87" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="M87">
         <v>145.7563919552551</v>
@@ -39499,8 +40179,8 @@
       </c>
     </row>
     <row r="88" spans="1:150">
-      <c r="A88" s="1">
-        <v>33420</v>
+      <c r="A88" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="N88">
         <v>144.8826257689904</v>
@@ -39915,8 +40595,8 @@
       </c>
     </row>
     <row r="89" spans="1:150">
-      <c r="A89" s="1">
-        <v>33512</v>
+      <c r="A89" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="O89">
         <v>146.1424746887208</v>
@@ -40328,8 +41008,8 @@
       </c>
     </row>
     <row r="90" spans="1:150">
-      <c r="A90" s="1">
-        <v>33604</v>
+      <c r="A90" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="P90">
         <v>148.1135286437828</v>
@@ -40738,8 +41418,8 @@
       </c>
     </row>
     <row r="91" spans="1:150">
-      <c r="A91" s="1">
-        <v>33695</v>
+      <c r="A91" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="Q91">
         <v>148.0525682121829</v>
@@ -41145,8 +41825,8 @@
       </c>
     </row>
     <row r="92" spans="1:150">
-      <c r="A92" s="1">
-        <v>33786</v>
+      <c r="A92" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="R92">
         <v>147.8290466296502</v>
@@ -41549,8 +42229,8 @@
       </c>
     </row>
     <row r="93" spans="1:150">
-      <c r="A93" s="1">
-        <v>33878</v>
+      <c r="A93" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="S93">
         <v>147.6258451909839</v>
@@ -41950,8 +42630,8 @@
       </c>
     </row>
     <row r="94" spans="1:150">
-      <c r="A94" s="1">
-        <v>33970</v>
+      <c r="A94" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="T94">
         <v>144.9842264883235</v>
@@ -42348,8 +43028,8 @@
       </c>
     </row>
     <row r="95" spans="1:150">
-      <c r="A95" s="1">
-        <v>34060</v>
+      <c r="A95" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="U95">
         <v>145.8986329623214</v>
@@ -42743,8 +43423,8 @@
       </c>
     </row>
     <row r="96" spans="1:150">
-      <c r="A96" s="1">
-        <v>34151</v>
+      <c r="A96" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="V96">
         <v>146.9552804433855</v>
@@ -43135,8 +43815,8 @@
       </c>
     </row>
     <row r="97" spans="1:150">
-      <c r="A97" s="1">
-        <v>34243</v>
+      <c r="A97" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="W97">
         <v>146.6707984292529</v>
@@ -43524,8 +44204,8 @@
       </c>
     </row>
     <row r="98" spans="1:150">
-      <c r="A98" s="1">
-        <v>34335</v>
+      <c r="A98" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="X98">
         <v>148.3980106579154</v>
@@ -43910,8 +44590,8 @@
       </c>
     </row>
     <row r="99" spans="1:150">
-      <c r="A99" s="1">
-        <v>34425</v>
+      <c r="A99" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="Y99">
         <v>150.2268236059111</v>
@@ -44293,8 +44973,8 @@
       </c>
     </row>
     <row r="100" spans="1:150">
-      <c r="A100" s="1">
-        <v>34516</v>
+      <c r="A100" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="Z100">
         <v>151.1615502237756</v>
@@ -44673,8 +45353,8 @@
       </c>
     </row>
     <row r="101" spans="1:150">
-      <c r="A101" s="1">
-        <v>34608</v>
+      <c r="A101" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="AA101">
         <v>152.09627684164</v>
@@ -45050,8 +45730,8 @@
       </c>
     </row>
     <row r="102" spans="1:150">
-      <c r="A102" s="1">
-        <v>34700</v>
+      <c r="A102" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="AB102">
         <v>152.4213991435059</v>
@@ -45424,8 +46104,8 @@
       </c>
     </row>
     <row r="103" spans="1:150">
-      <c r="A103" s="1">
-        <v>34790</v>
+      <c r="A103" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="AC103">
         <v>154.0470106528354</v>
@@ -45795,8 +46475,8 @@
       </c>
     </row>
     <row r="104" spans="1:150">
-      <c r="A104" s="1">
-        <v>34881</v>
+      <c r="A104" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="AD104">
         <v>154.0266905089688</v>
@@ -46163,8 +46843,8 @@
       </c>
     </row>
     <row r="105" spans="1:150">
-      <c r="A105" s="1">
-        <v>34973</v>
+      <c r="A105" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="AE105">
         <v>153.6609279193697</v>
@@ -46528,8 +47208,8 @@
       </c>
     </row>
     <row r="106" spans="1:150">
-      <c r="A106" s="1">
-        <v>35065</v>
+      <c r="A106" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="AF106">
         <v>153.2545250420373</v>
@@ -46890,8 +47570,8 @@
       </c>
     </row>
     <row r="107" spans="1:150">
-      <c r="A107" s="1">
-        <v>35156</v>
+      <c r="A107" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="AG107">
         <v>155.5710214428318</v>
@@ -47249,8 +47929,8 @@
       </c>
     </row>
     <row r="108" spans="1:150">
-      <c r="A108" s="1">
-        <v>35247</v>
+      <c r="A108" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="AH108">
         <v>156.8715106502954</v>
@@ -47605,8 +48285,8 @@
       </c>
     </row>
     <row r="109" spans="1:150">
-      <c r="A109" s="1">
-        <v>35339</v>
+      <c r="A109" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="AI109">
         <v>156.9121509380286</v>
@@ -47958,8 +48638,8 @@
       </c>
     </row>
     <row r="110" spans="1:150">
-      <c r="A110" s="1">
-        <v>35431</v>
+      <c r="A110" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="AJ110">
         <v>157.6030358294937</v>
@@ -48308,8 +48988,8 @@
       </c>
     </row>
     <row r="111" spans="1:150">
-      <c r="A111" s="1">
-        <v>35521</v>
+      <c r="A111" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="AK111">
         <v>158.436161728025</v>
@@ -48655,8 +49335,8 @@
       </c>
     </row>
     <row r="112" spans="1:150">
-      <c r="A112" s="1">
-        <v>35612</v>
+      <c r="A112" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="AL112">
         <v>159.6960106477554</v>
@@ -48999,8 +49679,8 @@
       </c>
     </row>
     <row r="113" spans="1:150">
-      <c r="A113" s="1">
-        <v>35704</v>
+      <c r="A113" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="AM113">
         <v>160.0008128057547</v>
@@ -49340,8 +50020,8 @@
       </c>
     </row>
     <row r="114" spans="1:150">
-      <c r="A114" s="1">
-        <v>35796</v>
+      <c r="A114" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="AN114">
         <v>161.5654638834843</v>
@@ -49678,8 +50358,8 @@
       </c>
     </row>
     <row r="115" spans="1:150">
-      <c r="A115" s="1">
-        <v>35886</v>
+      <c r="A115" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="AO115">
         <v>161.4029027325514</v>
@@ -50013,8 +50693,8 @@
       </c>
     </row>
     <row r="116" spans="1:150">
-      <c r="A116" s="1">
-        <v>35977</v>
+      <c r="A116" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="AP116">
         <v>162.7033919400149</v>
@@ -50345,8 +51025,8 @@
       </c>
     </row>
     <row r="117" spans="1:150">
-      <c r="A117" s="1">
-        <v>36069</v>
+      <c r="A117" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="AQ117">
         <v>161.9921869046833</v>
@@ -50674,8 +51354,8 @@
       </c>
     </row>
     <row r="118" spans="1:150">
-      <c r="A118" s="1">
-        <v>36161</v>
+      <c r="A118" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="AR118">
         <v>96.39876250323853</v>
@@ -51000,8 +51680,8 @@
       </c>
     </row>
     <row r="119" spans="1:150">
-      <c r="A119" s="1">
-        <v>36251</v>
+      <c r="A119" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="AS119">
         <v>95.93139919430629</v>
@@ -51323,8 +52003,8 @@
       </c>
     </row>
     <row r="120" spans="1:150">
-      <c r="A120" s="1">
-        <v>36342</v>
+      <c r="A120" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="AT120">
         <v>96.86612581217075</v>
@@ -51643,8 +52323,8 @@
       </c>
     </row>
     <row r="121" spans="1:150">
-      <c r="A121" s="1">
-        <v>36434</v>
+      <c r="A121" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="AU121">
         <v>97.69925171070211</v>
@@ -51960,8 +52640,8 @@
       </c>
     </row>
     <row r="122" spans="1:150">
-      <c r="A122" s="1">
-        <v>36526</v>
+      <c r="A122" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="AV122">
         <v>98.29869595476735</v>
@@ -52274,8 +52954,8 @@
       </c>
     </row>
     <row r="123" spans="1:150">
-      <c r="A123" s="1">
-        <v>36617</v>
+      <c r="A123" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="AW123">
         <v>99.51993660115113</v>
@@ -52585,8 +53265,8 @@
       </c>
     </row>
     <row r="124" spans="1:150">
-      <c r="A124" s="1">
-        <v>36708</v>
+      <c r="A124" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="AX124">
         <v>100.2108214926162</v>
@@ -52893,8 +53573,8 @@
       </c>
     </row>
     <row r="125" spans="1:150">
-      <c r="A125" s="1">
-        <v>36800</v>
+      <c r="A125" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="AY125">
         <v>100.302262140016</v>
@@ -53198,8 +53878,8 @@
       </c>
     </row>
     <row r="126" spans="1:150">
-      <c r="A126" s="1">
-        <v>36892</v>
+      <c r="A126" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="AZ126">
         <v>100.6741207727751</v>
@@ -53500,8 +54180,8 @@
       </c>
     </row>
     <row r="127" spans="1:150">
-      <c r="A127" s="1">
-        <v>36982</v>
+      <c r="A127" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="BA127">
         <v>100.8082337222948</v>
@@ -53799,8 +54479,8 @@
       </c>
     </row>
     <row r="128" spans="1:150">
-      <c r="A128" s="1">
-        <v>37073</v>
+      <c r="A128" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="BB128">
         <v>100.6659927152284</v>
@@ -54095,8 +54775,8 @@
       </c>
     </row>
     <row r="129" spans="1:150">
-      <c r="A129" s="1">
-        <v>37165</v>
+      <c r="A129" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="BC129">
         <v>100.4505991902423</v>
@@ -54388,8 +55068,8 @@
       </c>
     </row>
     <row r="130" spans="1:150">
-      <c r="A130" s="1">
-        <v>37257</v>
+      <c r="A130" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="BD130">
         <v>100.6212883987219</v>
@@ -54678,8 +55358,8 @@
       </c>
     </row>
     <row r="131" spans="1:150">
-      <c r="A131" s="1">
-        <v>37347</v>
+      <c r="A131" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="BE131">
         <v>100.9850189739343</v>
@@ -54965,8 +55645,8 @@
       </c>
     </row>
     <row r="132" spans="1:150">
-      <c r="A132" s="1">
-        <v>37438</v>
+      <c r="A132" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="BF132">
         <v>101.1333560241606</v>
@@ -55249,8 +55929,8 @@
       </c>
     </row>
     <row r="133" spans="1:150">
-      <c r="A133" s="1">
-        <v>37530</v>
+      <c r="A133" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="BG133">
         <v>101.1516441536406</v>
@@ -55530,8 +56210,8 @@
       </c>
     </row>
     <row r="134" spans="1:150">
-      <c r="A134" s="1">
-        <v>37622</v>
+      <c r="A134" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="BH134">
         <v>100.9220265279478</v>
@@ -55808,8 +56488,8 @@
       </c>
     </row>
     <row r="135" spans="1:150">
-      <c r="A135" s="1">
-        <v>37712</v>
+      <c r="A135" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="BI135">
         <v>101.0195632185076</v>
@@ -56083,8 +56763,8 @@
       </c>
     </row>
     <row r="136" spans="1:150">
-      <c r="A136" s="1">
-        <v>37803</v>
+      <c r="A136" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="BJ136">
         <v>101.1394520673206</v>
@@ -56355,8 +57035,8 @@
       </c>
     </row>
     <row r="137" spans="1:150">
-      <c r="A137" s="1">
-        <v>37895</v>
+      <c r="A137" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="BK137">
         <v>101.3365574628268</v>
@@ -56624,8 +57304,8 @@
       </c>
     </row>
     <row r="138" spans="1:150">
-      <c r="A138" s="1">
-        <v>37987</v>
+      <c r="A138" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="BL138">
         <v>101.8140808436924</v>
@@ -56890,8 +57570,8 @@
       </c>
     </row>
     <row r="139" spans="1:150">
-      <c r="A139" s="1">
-        <v>38078</v>
+      <c r="A139" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="BM139">
         <v>102.2021955915448</v>
@@ -57153,8 +57833,8 @@
       </c>
     </row>
     <row r="140" spans="1:150">
-      <c r="A140" s="1">
-        <v>38169</v>
+      <c r="A140" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="BN140">
         <v>102.2408038648914</v>
@@ -57413,8 +58093,8 @@
       </c>
     </row>
     <row r="141" spans="1:150">
-      <c r="A141" s="1">
-        <v>38261</v>
+      <c r="A141" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="BO141">
         <v>101.9258416349588</v>
@@ -57670,8 +58350,8 @@
       </c>
     </row>
     <row r="142" spans="1:150">
-      <c r="A142" s="1">
-        <v>38353</v>
+      <c r="A142" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="BP142">
         <v>103.55</v>
@@ -57924,8 +58604,8 @@
       </c>
     </row>
     <row r="143" spans="1:150">
-      <c r="A143" s="1">
-        <v>38443</v>
+      <c r="A143" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="BQ143">
         <v>103.09</v>
@@ -58175,8 +58855,8 @@
       </c>
     </row>
     <row r="144" spans="1:150">
-      <c r="A144" s="1">
-        <v>38534</v>
+      <c r="A144" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="BR144">
         <v>103.79</v>
@@ -58423,8 +59103,8 @@
       </c>
     </row>
     <row r="145" spans="1:150">
-      <c r="A145" s="1">
-        <v>38626</v>
+      <c r="A145" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="BS145">
         <v>103.9</v>
@@ -58668,8 +59348,8 @@
       </c>
     </row>
     <row r="146" spans="1:150">
-      <c r="A146" s="1">
-        <v>38718</v>
+      <c r="A146" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="BT146">
         <v>104.39</v>
@@ -58910,8 +59590,8 @@
       </c>
     </row>
     <row r="147" spans="1:150">
-      <c r="A147" s="1">
-        <v>38808</v>
+      <c r="A147" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="BU147">
         <v>105.26</v>
@@ -59149,8 +59829,8 @@
       </c>
     </row>
     <row r="148" spans="1:150">
-      <c r="A148" s="1">
-        <v>38899</v>
+      <c r="A148" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="BV148">
         <v>106.24</v>
@@ -59385,8 +60065,8 @@
       </c>
     </row>
     <row r="149" spans="1:150">
-      <c r="A149" s="1">
-        <v>38991</v>
+      <c r="A149" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="BW149">
         <v>107.48</v>
@@ -59618,8 +60298,8 @@
       </c>
     </row>
     <row r="150" spans="1:150">
-      <c r="A150" s="1">
-        <v>39083</v>
+      <c r="A150" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="BX150">
         <v>108.25</v>
@@ -59848,8 +60528,8 @@
       </c>
     </row>
     <row r="151" spans="1:150">
-      <c r="A151" s="1">
-        <v>39173</v>
+      <c r="A151" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="BY151">
         <v>108.27</v>
@@ -60075,8 +60755,8 @@
       </c>
     </row>
     <row r="152" spans="1:150">
-      <c r="A152" s="1">
-        <v>39264</v>
+      <c r="A152" s="2" t="s">
+        <v>150</v>
       </c>
       <c r="BZ152">
         <v>109.01</v>
@@ -60299,8 +60979,8 @@
       </c>
     </row>
     <row r="153" spans="1:150">
-      <c r="A153" s="1">
-        <v>39356</v>
+      <c r="A153" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="CA153">
         <v>109.29</v>
@@ -60520,8 +61200,8 @@
       </c>
     </row>
     <row r="154" spans="1:150">
-      <c r="A154" s="1">
-        <v>39448</v>
+      <c r="A154" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="CB154">
         <v>110.96</v>
@@ -60738,8 +61418,8 @@
       </c>
     </row>
     <row r="155" spans="1:150">
-      <c r="A155" s="1">
-        <v>39539</v>
+      <c r="A155" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="CC155">
         <v>110.39</v>
@@ -60953,8 +61633,8 @@
       </c>
     </row>
     <row r="156" spans="1:150">
-      <c r="A156" s="1">
-        <v>39630</v>
+      <c r="A156" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="CD156">
         <v>110.02</v>
@@ -61165,8 +61845,8 @@
       </c>
     </row>
     <row r="157" spans="1:150">
-      <c r="A157" s="1">
-        <v>39722</v>
+      <c r="A157" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="CE157">
         <v>107.74</v>
@@ -61374,8 +62054,8 @@
       </c>
     </row>
     <row r="158" spans="1:150">
-      <c r="A158" s="1">
-        <v>39814</v>
+      <c r="A158" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="CF158">
         <v>103.52</v>
@@ -61580,8 +62260,8 @@
       </c>
     </row>
     <row r="159" spans="1:150">
-      <c r="A159" s="1">
-        <v>39904</v>
+      <c r="A159" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="CG159">
         <v>104.26</v>
@@ -61783,8 +62463,8 @@
       </c>
     </row>
     <row r="160" spans="1:150">
-      <c r="A160" s="1">
-        <v>39995</v>
+      <c r="A160" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="CH160">
         <v>105.15</v>
@@ -61983,8 +62663,8 @@
       </c>
     </row>
     <row r="161" spans="1:150">
-      <c r="A161" s="1">
-        <v>40087</v>
+      <c r="A161" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="CI161">
         <v>105.18</v>
@@ -62180,8 +62860,8 @@
       </c>
     </row>
     <row r="162" spans="1:150">
-      <c r="A162" s="1">
-        <v>40179</v>
+      <c r="A162" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="CJ162">
         <v>105.53</v>
@@ -62374,8 +63054,8 @@
       </c>
     </row>
     <row r="163" spans="1:150">
-      <c r="A163" s="1">
-        <v>40269</v>
+      <c r="A163" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="CK163">
         <v>108.64</v>
@@ -62565,8 +63245,8 @@
       </c>
     </row>
     <row r="164" spans="1:150">
-      <c r="A164" s="1">
-        <v>40360</v>
+      <c r="A164" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="CL164">
         <v>109.64</v>
@@ -62753,8 +63433,8 @@
       </c>
     </row>
     <row r="165" spans="1:150">
-      <c r="A165" s="1">
-        <v>40452</v>
+      <c r="A165" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="CM165">
         <v>110.05</v>
@@ -62938,8 +63618,8 @@
       </c>
     </row>
     <row r="166" spans="1:150">
-      <c r="A166" s="1">
-        <v>40544</v>
+      <c r="A166" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="CN166">
         <v>111.71</v>
@@ -63120,8 +63800,8 @@
       </c>
     </row>
     <row r="167" spans="1:150">
-      <c r="A167" s="1">
-        <v>40634</v>
+      <c r="A167" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="CO167">
         <v>109.17</v>
@@ -63299,8 +63979,8 @@
       </c>
     </row>
     <row r="168" spans="1:150">
-      <c r="A168" s="1">
-        <v>40725</v>
+      <c r="A168" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="CP168">
         <v>109.89</v>
@@ -63475,8 +64155,8 @@
       </c>
     </row>
     <row r="169" spans="1:150">
-      <c r="A169" s="1">
-        <v>40817</v>
+      <c r="A169" s="2" t="s">
+        <v>167</v>
       </c>
       <c r="CQ169">
         <v>109.77</v>
@@ -63648,8 +64328,8 @@
       </c>
     </row>
     <row r="170" spans="1:150">
-      <c r="A170" s="1">
-        <v>40909</v>
+      <c r="A170" s="2" t="s">
+        <v>168</v>
       </c>
       <c r="CR170">
         <v>110.33</v>
@@ -63818,8 +64498,8 @@
       </c>
     </row>
     <row r="171" spans="1:150">
-      <c r="A171" s="1">
-        <v>41000</v>
+      <c r="A171" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="CS171">
         <v>111.12</v>
@@ -63985,8 +64665,8 @@
       </c>
     </row>
     <row r="172" spans="1:150">
-      <c r="A172" s="1">
-        <v>41091</v>
+      <c r="A172" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="CT172">
         <v>111.38</v>
@@ -64149,8 +64829,8 @@
       </c>
     </row>
     <row r="173" spans="1:150">
-      <c r="A173" s="1">
-        <v>41183</v>
+      <c r="A173" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="CU173">
         <v>110.73</v>
@@ -64310,8 +64990,8 @@
       </c>
     </row>
     <row r="174" spans="1:150">
-      <c r="A174" s="1">
-        <v>41275</v>
+      <c r="A174" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="CV174">
         <v>110.68</v>
@@ -64468,8 +65148,8 @@
       </c>
     </row>
     <row r="175" spans="1:150">
-      <c r="A175" s="1">
-        <v>41365</v>
+      <c r="A175" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="CW175">
         <v>111.69</v>
@@ -64623,8 +65303,8 @@
       </c>
     </row>
     <row r="176" spans="1:150">
-      <c r="A176" s="1">
-        <v>41456</v>
+      <c r="A176" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="CX176">
         <v>112.05</v>
@@ -64775,8 +65455,8 @@
       </c>
     </row>
     <row r="177" spans="1:150">
-      <c r="A177" s="1">
-        <v>41548</v>
+      <c r="A177" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="CY177">
         <v>112.48</v>
@@ -64924,8 +65604,8 @@
       </c>
     </row>
     <row r="178" spans="1:150">
-      <c r="A178" s="1">
-        <v>41640</v>
+      <c r="A178" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="CZ178">
         <v>113.4</v>
@@ -65070,8 +65750,8 @@
       </c>
     </row>
     <row r="179" spans="1:150">
-      <c r="A179" s="1">
-        <v>41730</v>
+      <c r="A179" s="2" t="s">
+        <v>177</v>
       </c>
       <c r="DA179">
         <v>105.5</v>
@@ -65213,8 +65893,8 @@
       </c>
     </row>
     <row r="180" spans="1:150">
-      <c r="A180" s="1">
-        <v>41821</v>
+      <c r="A180" s="2" t="s">
+        <v>178</v>
       </c>
       <c r="DB180">
         <v>105.75</v>
@@ -65353,8 +66033,8 @@
       </c>
     </row>
     <row r="181" spans="1:150">
-      <c r="A181" s="1">
-        <v>41913</v>
+      <c r="A181" s="2" t="s">
+        <v>179</v>
       </c>
       <c r="DC181">
         <v>106.5</v>
@@ -65490,8 +66170,8 @@
       </c>
     </row>
     <row r="182" spans="1:150">
-      <c r="A182" s="1">
-        <v>42005</v>
+      <c r="A182" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="DD182">
         <v>106.79</v>
@@ -65624,8 +66304,8 @@
       </c>
     </row>
     <row r="183" spans="1:150">
-      <c r="A183" s="1">
-        <v>42095</v>
+      <c r="A183" s="2" t="s">
+        <v>181</v>
       </c>
       <c r="DE183">
         <v>107.62</v>
@@ -65755,8 +66435,8 @@
       </c>
     </row>
     <row r="184" spans="1:150">
-      <c r="A184" s="1">
-        <v>42186</v>
+      <c r="A184" s="2" t="s">
+        <v>182</v>
       </c>
       <c r="DF184">
         <v>107.96</v>
@@ -65883,8 +66563,8 @@
       </c>
     </row>
     <row r="185" spans="1:150">
-      <c r="A185" s="1">
-        <v>42278</v>
+      <c r="A185" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="DG185">
         <v>108.22</v>
@@ -66008,8 +66688,8 @@
       </c>
     </row>
     <row r="186" spans="1:150">
-      <c r="A186" s="1">
-        <v>42370</v>
+      <c r="A186" s="2" t="s">
+        <v>184</v>
       </c>
       <c r="DH186">
         <v>108.94</v>
@@ -66130,8 +66810,8 @@
       </c>
     </row>
     <row r="187" spans="1:150">
-      <c r="A187" s="1">
-        <v>42461</v>
+      <c r="A187" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="DI187">
         <v>109.87</v>
@@ -66249,8 +66929,8 @@
       </c>
     </row>
     <row r="188" spans="1:150">
-      <c r="A188" s="1">
-        <v>42552</v>
+      <c r="A188" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="DJ188">
         <v>110.08</v>
@@ -66365,8 +67045,8 @@
       </c>
     </row>
     <row r="189" spans="1:150">
-      <c r="A189" s="1">
-        <v>42644</v>
+      <c r="A189" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="DK189">
         <v>110.56</v>
@@ -66478,8 +67158,8 @@
       </c>
     </row>
     <row r="190" spans="1:150">
-      <c r="A190" s="1">
-        <v>42736</v>
+      <c r="A190" s="2" t="s">
+        <v>188</v>
       </c>
       <c r="DL190">
         <v>111.25</v>
@@ -66588,8 +67268,8 @@
       </c>
     </row>
     <row r="191" spans="1:150">
-      <c r="A191" s="1">
-        <v>42826</v>
+      <c r="A191" s="2" t="s">
+        <v>189</v>
       </c>
       <c r="DM191">
         <v>112.62</v>
@@ -66695,8 +67375,8 @@
       </c>
     </row>
     <row r="192" spans="1:150">
-      <c r="A192" s="1">
-        <v>42917</v>
+      <c r="A192" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="DN192">
         <v>113.77</v>
@@ -66799,8 +67479,8 @@
       </c>
     </row>
     <row r="193" spans="1:150">
-      <c r="A193" s="1">
-        <v>43009</v>
+      <c r="A193" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="DO193">
         <v>114.37</v>
@@ -66900,8 +67580,8 @@
       </c>
     </row>
     <row r="194" spans="1:150">
-      <c r="A194" s="1">
-        <v>43101</v>
+      <c r="A194" s="2" t="s">
+        <v>192</v>
       </c>
       <c r="DP194">
         <v>114.71</v>
@@ -66998,8 +67678,8 @@
       </c>
     </row>
     <row r="195" spans="1:150">
-      <c r="A195" s="1">
-        <v>43191</v>
+      <c r="A195" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="DQ195">
         <v>115.67</v>
@@ -67093,8 +67773,8 @@
       </c>
     </row>
     <row r="196" spans="1:150">
-      <c r="A196" s="1">
-        <v>43282</v>
+      <c r="A196" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="DR196">
         <v>115.44</v>
@@ -67185,8 +67865,8 @@
       </c>
     </row>
     <row r="197" spans="1:150">
-      <c r="A197" s="1">
-        <v>43374</v>
+      <c r="A197" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="DS197">
         <v>115.47</v>
@@ -67274,8 +67954,8 @@
       </c>
     </row>
     <row r="198" spans="1:150">
-      <c r="A198" s="1">
-        <v>43466</v>
+      <c r="A198" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="DT198">
         <v>115.96</v>
@@ -67360,8 +68040,8 @@
       </c>
     </row>
     <row r="199" spans="1:150">
-      <c r="A199" s="1">
-        <v>43556</v>
+      <c r="A199" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="DU199">
         <v>107.03</v>
@@ -67443,8 +68123,8 @@
       </c>
     </row>
     <row r="200" spans="1:150">
-      <c r="A200" s="1">
-        <v>43647</v>
+      <c r="A200" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="DV200">
         <v>107.03</v>
@@ -67523,8 +68203,8 @@
       </c>
     </row>
     <row r="201" spans="1:150">
-      <c r="A201" s="1">
-        <v>43739</v>
+      <c r="A201" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="DW201">
         <v>107.19</v>
@@ -67600,8 +68280,8 @@
       </c>
     </row>
     <row r="202" spans="1:150">
-      <c r="A202" s="1">
-        <v>43831</v>
+      <c r="A202" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="DX202">
         <v>104.74</v>
@@ -67674,8 +68354,8 @@
       </c>
     </row>
     <row r="203" spans="1:150">
-      <c r="A203" s="1">
-        <v>43922</v>
+      <c r="A203" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="DY203">
         <v>94.68000000000001</v>
@@ -67745,8 +68425,8 @@
       </c>
     </row>
     <row r="204" spans="1:150">
-      <c r="A204" s="1">
-        <v>44013</v>
+      <c r="A204" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="DZ204">
         <v>102.72</v>
@@ -67813,8 +68493,8 @@
       </c>
     </row>
     <row r="205" spans="1:150">
-      <c r="A205" s="1">
-        <v>44105</v>
+      <c r="A205" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="EA205">
         <v>103.1</v>
@@ -67878,8 +68558,8 @@
       </c>
     </row>
     <row r="206" spans="1:150">
-      <c r="A206" s="1">
-        <v>44197</v>
+      <c r="A206" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="EB206">
         <v>101.62</v>
@@ -67940,8 +68620,8 @@
       </c>
     </row>
     <row r="207" spans="1:150">
-      <c r="A207" s="1">
-        <v>44287</v>
+      <c r="A207" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="EC207">
         <v>103.93</v>
@@ -67999,8 +68679,8 @@
       </c>
     </row>
     <row r="208" spans="1:150">
-      <c r="A208" s="1">
-        <v>44378</v>
+      <c r="A208" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="ED208">
         <v>106.24</v>
@@ -68055,8 +68735,8 @@
       </c>
     </row>
     <row r="209" spans="1:150">
-      <c r="A209" s="1">
-        <v>44470</v>
+      <c r="A209" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="EE209">
         <v>106.2</v>
@@ -68108,8 +68788,8 @@
       </c>
     </row>
     <row r="210" spans="1:150">
-      <c r="A210" s="1">
-        <v>44562</v>
+      <c r="A210" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="EF210">
         <v>106.45</v>
@@ -68158,8 +68838,8 @@
       </c>
     </row>
     <row r="211" spans="1:150">
-      <c r="A211" s="1">
-        <v>44652</v>
+      <c r="A211" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="EG211">
         <v>107.5</v>
@@ -68205,8 +68885,8 @@
       </c>
     </row>
     <row r="212" spans="1:150">
-      <c r="A212" s="1">
-        <v>44743</v>
+      <c r="A212" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="EH212">
         <v>107.89</v>
@@ -68249,8 +68929,8 @@
       </c>
     </row>
     <row r="213" spans="1:150">
-      <c r="A213" s="1">
-        <v>44835</v>
+      <c r="A213" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="EI213">
         <v>107.5</v>
@@ -68290,8 +68970,8 @@
       </c>
     </row>
     <row r="214" spans="1:150">
-      <c r="A214" s="1">
-        <v>44927</v>
+      <c r="A214" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="EJ214">
         <v>107.03</v>
@@ -68328,8 +69008,8 @@
       </c>
     </row>
     <row r="215" spans="1:150">
-      <c r="A215" s="1">
-        <v>45017</v>
+      <c r="A215" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="EK215">
         <v>107.78</v>
@@ -68363,8 +69043,8 @@
       </c>
     </row>
     <row r="216" spans="1:150">
-      <c r="A216" s="1">
-        <v>45108</v>
+      <c r="A216" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="EL216">
         <v>107.87</v>
@@ -68395,8 +69075,8 @@
       </c>
     </row>
     <row r="217" spans="1:150">
-      <c r="A217" s="1">
-        <v>45200</v>
+      <c r="A217" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="EM217">
         <v>107.68</v>
@@ -68424,8 +69104,8 @@
       </c>
     </row>
     <row r="218" spans="1:150">
-      <c r="A218" s="1">
-        <v>45292</v>
+      <c r="A218" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="EN218">
         <v>107.91</v>
@@ -68450,8 +69130,8 @@
       </c>
     </row>
     <row r="219" spans="1:150">
-      <c r="A219" s="1">
-        <v>45383</v>
+      <c r="A219" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="EO219">
         <v>104.78</v>
@@ -68473,8 +69153,8 @@
       </c>
     </row>
     <row r="220" spans="1:150">
-      <c r="A220" s="1">
-        <v>45474</v>
+      <c r="A220" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="EP220">
         <v>104.66</v>
@@ -68493,8 +69173,8 @@
       </c>
     </row>
     <row r="221" spans="1:150">
-      <c r="A221" s="1">
-        <v>45566</v>
+      <c r="A221" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="EQ221">
         <v>104.45</v>
@@ -68510,8 +69190,8 @@
       </c>
     </row>
     <row r="222" spans="1:150">
-      <c r="A222" s="1">
-        <v>45658</v>
+      <c r="A222" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="ER222">
         <v>104.88</v>
@@ -68524,8 +69204,8 @@
       </c>
     </row>
     <row r="223" spans="1:150">
-      <c r="A223" s="1">
-        <v>45748</v>
+      <c r="A223" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="ES223">
         <v>104.52</v>
@@ -68535,16 +69215,16 @@
       </c>
     </row>
     <row r="224" spans="1:150">
-      <c r="A224" s="1">
-        <v>45839</v>
+      <c r="A224" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="ET224">
         <v>104.59</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="1">
-        <v>45931</v>
+      <c r="A225" s="2" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixed evaluation and simulaed rt_data for components
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
@@ -11,683 +11,6 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="224">
-  <si>
-    <t>1970Q1</t>
-  </si>
-  <si>
-    <t>1970Q2</t>
-  </si>
-  <si>
-    <t>1970Q3</t>
-  </si>
-  <si>
-    <t>1970Q4</t>
-  </si>
-  <si>
-    <t>1971Q1</t>
-  </si>
-  <si>
-    <t>1971Q2</t>
-  </si>
-  <si>
-    <t>1971Q3</t>
-  </si>
-  <si>
-    <t>1971Q4</t>
-  </si>
-  <si>
-    <t>1972Q1</t>
-  </si>
-  <si>
-    <t>1972Q2</t>
-  </si>
-  <si>
-    <t>1972Q3</t>
-  </si>
-  <si>
-    <t>1972Q4</t>
-  </si>
-  <si>
-    <t>1973Q1</t>
-  </si>
-  <si>
-    <t>1973Q2</t>
-  </si>
-  <si>
-    <t>1973Q3</t>
-  </si>
-  <si>
-    <t>1973Q4</t>
-  </si>
-  <si>
-    <t>1974Q1</t>
-  </si>
-  <si>
-    <t>1974Q2</t>
-  </si>
-  <si>
-    <t>1974Q3</t>
-  </si>
-  <si>
-    <t>1974Q4</t>
-  </si>
-  <si>
-    <t>1975Q1</t>
-  </si>
-  <si>
-    <t>1975Q2</t>
-  </si>
-  <si>
-    <t>1975Q3</t>
-  </si>
-  <si>
-    <t>1975Q4</t>
-  </si>
-  <si>
-    <t>1976Q1</t>
-  </si>
-  <si>
-    <t>1976Q2</t>
-  </si>
-  <si>
-    <t>1976Q3</t>
-  </si>
-  <si>
-    <t>1976Q4</t>
-  </si>
-  <si>
-    <t>1977Q1</t>
-  </si>
-  <si>
-    <t>1977Q2</t>
-  </si>
-  <si>
-    <t>1977Q3</t>
-  </si>
-  <si>
-    <t>1977Q4</t>
-  </si>
-  <si>
-    <t>1978Q1</t>
-  </si>
-  <si>
-    <t>1978Q2</t>
-  </si>
-  <si>
-    <t>1978Q3</t>
-  </si>
-  <si>
-    <t>1978Q4</t>
-  </si>
-  <si>
-    <t>1979Q1</t>
-  </si>
-  <si>
-    <t>1979Q2</t>
-  </si>
-  <si>
-    <t>1979Q3</t>
-  </si>
-  <si>
-    <t>1979Q4</t>
-  </si>
-  <si>
-    <t>1980Q1</t>
-  </si>
-  <si>
-    <t>1980Q2</t>
-  </si>
-  <si>
-    <t>1980Q3</t>
-  </si>
-  <si>
-    <t>1980Q4</t>
-  </si>
-  <si>
-    <t>1981Q1</t>
-  </si>
-  <si>
-    <t>1981Q2</t>
-  </si>
-  <si>
-    <t>1981Q3</t>
-  </si>
-  <si>
-    <t>1981Q4</t>
-  </si>
-  <si>
-    <t>1982Q1</t>
-  </si>
-  <si>
-    <t>1982Q2</t>
-  </si>
-  <si>
-    <t>1982Q3</t>
-  </si>
-  <si>
-    <t>1982Q4</t>
-  </si>
-  <si>
-    <t>1983Q1</t>
-  </si>
-  <si>
-    <t>1983Q2</t>
-  </si>
-  <si>
-    <t>1983Q3</t>
-  </si>
-  <si>
-    <t>1983Q4</t>
-  </si>
-  <si>
-    <t>1984Q1</t>
-  </si>
-  <si>
-    <t>1984Q2</t>
-  </si>
-  <si>
-    <t>1984Q3</t>
-  </si>
-  <si>
-    <t>1984Q4</t>
-  </si>
-  <si>
-    <t>1985Q1</t>
-  </si>
-  <si>
-    <t>1985Q2</t>
-  </si>
-  <si>
-    <t>1985Q3</t>
-  </si>
-  <si>
-    <t>1985Q4</t>
-  </si>
-  <si>
-    <t>1986Q1</t>
-  </si>
-  <si>
-    <t>1986Q2</t>
-  </si>
-  <si>
-    <t>1986Q3</t>
-  </si>
-  <si>
-    <t>1986Q4</t>
-  </si>
-  <si>
-    <t>1987Q1</t>
-  </si>
-  <si>
-    <t>1987Q2</t>
-  </si>
-  <si>
-    <t>1987Q3</t>
-  </si>
-  <si>
-    <t>1987Q4</t>
-  </si>
-  <si>
-    <t>1988Q1</t>
-  </si>
-  <si>
-    <t>1988Q2</t>
-  </si>
-  <si>
-    <t>1988Q3</t>
-  </si>
-  <si>
-    <t>1988Q4</t>
-  </si>
-  <si>
-    <t>1989Q1</t>
-  </si>
-  <si>
-    <t>1989Q2</t>
-  </si>
-  <si>
-    <t>1989Q3</t>
-  </si>
-  <si>
-    <t>1989Q4</t>
-  </si>
-  <si>
-    <t>1990Q1</t>
-  </si>
-  <si>
-    <t>1990Q2</t>
-  </si>
-  <si>
-    <t>1990Q3</t>
-  </si>
-  <si>
-    <t>1990Q4</t>
-  </si>
-  <si>
-    <t>1991Q1</t>
-  </si>
-  <si>
-    <t>1991Q2</t>
-  </si>
-  <si>
-    <t>1991Q3</t>
-  </si>
-  <si>
-    <t>1991Q4</t>
-  </si>
-  <si>
-    <t>1992Q1</t>
-  </si>
-  <si>
-    <t>1992Q2</t>
-  </si>
-  <si>
-    <t>1992Q3</t>
-  </si>
-  <si>
-    <t>1992Q4</t>
-  </si>
-  <si>
-    <t>1993Q1</t>
-  </si>
-  <si>
-    <t>1993Q2</t>
-  </si>
-  <si>
-    <t>1993Q3</t>
-  </si>
-  <si>
-    <t>1993Q4</t>
-  </si>
-  <si>
-    <t>1994Q1</t>
-  </si>
-  <si>
-    <t>1994Q2</t>
-  </si>
-  <si>
-    <t>1994Q3</t>
-  </si>
-  <si>
-    <t>1994Q4</t>
-  </si>
-  <si>
-    <t>1995Q1</t>
-  </si>
-  <si>
-    <t>1995Q2</t>
-  </si>
-  <si>
-    <t>1995Q3</t>
-  </si>
-  <si>
-    <t>1995Q4</t>
-  </si>
-  <si>
-    <t>1996Q1</t>
-  </si>
-  <si>
-    <t>1996Q2</t>
-  </si>
-  <si>
-    <t>1996Q3</t>
-  </si>
-  <si>
-    <t>1996Q4</t>
-  </si>
-  <si>
-    <t>1997Q1</t>
-  </si>
-  <si>
-    <t>1997Q2</t>
-  </si>
-  <si>
-    <t>1997Q3</t>
-  </si>
-  <si>
-    <t>1997Q4</t>
-  </si>
-  <si>
-    <t>1998Q1</t>
-  </si>
-  <si>
-    <t>1998Q2</t>
-  </si>
-  <si>
-    <t>1998Q3</t>
-  </si>
-  <si>
-    <t>1998Q4</t>
-  </si>
-  <si>
-    <t>1999Q1</t>
-  </si>
-  <si>
-    <t>1999Q2</t>
-  </si>
-  <si>
-    <t>1999Q3</t>
-  </si>
-  <si>
-    <t>1999Q4</t>
-  </si>
-  <si>
-    <t>2000Q1</t>
-  </si>
-  <si>
-    <t>2000Q2</t>
-  </si>
-  <si>
-    <t>2000Q3</t>
-  </si>
-  <si>
-    <t>2000Q4</t>
-  </si>
-  <si>
-    <t>2001Q1</t>
-  </si>
-  <si>
-    <t>2001Q2</t>
-  </si>
-  <si>
-    <t>2001Q3</t>
-  </si>
-  <si>
-    <t>2001Q4</t>
-  </si>
-  <si>
-    <t>2002Q1</t>
-  </si>
-  <si>
-    <t>2002Q2</t>
-  </si>
-  <si>
-    <t>2002Q3</t>
-  </si>
-  <si>
-    <t>2002Q4</t>
-  </si>
-  <si>
-    <t>2003Q1</t>
-  </si>
-  <si>
-    <t>2003Q2</t>
-  </si>
-  <si>
-    <t>2003Q3</t>
-  </si>
-  <si>
-    <t>2003Q4</t>
-  </si>
-  <si>
-    <t>2004Q1</t>
-  </si>
-  <si>
-    <t>2004Q2</t>
-  </si>
-  <si>
-    <t>2004Q3</t>
-  </si>
-  <si>
-    <t>2004Q4</t>
-  </si>
-  <si>
-    <t>2005Q1</t>
-  </si>
-  <si>
-    <t>2005Q2</t>
-  </si>
-  <si>
-    <t>2005Q3</t>
-  </si>
-  <si>
-    <t>2005Q4</t>
-  </si>
-  <si>
-    <t>2006Q1</t>
-  </si>
-  <si>
-    <t>2006Q2</t>
-  </si>
-  <si>
-    <t>2006Q3</t>
-  </si>
-  <si>
-    <t>2006Q4</t>
-  </si>
-  <si>
-    <t>2007Q1</t>
-  </si>
-  <si>
-    <t>2007Q2</t>
-  </si>
-  <si>
-    <t>2007Q3</t>
-  </si>
-  <si>
-    <t>2007Q4</t>
-  </si>
-  <si>
-    <t>2008Q1</t>
-  </si>
-  <si>
-    <t>2008Q2</t>
-  </si>
-  <si>
-    <t>2008Q3</t>
-  </si>
-  <si>
-    <t>2008Q4</t>
-  </si>
-  <si>
-    <t>2009Q1</t>
-  </si>
-  <si>
-    <t>2009Q2</t>
-  </si>
-  <si>
-    <t>2009Q3</t>
-  </si>
-  <si>
-    <t>2009Q4</t>
-  </si>
-  <si>
-    <t>2010Q1</t>
-  </si>
-  <si>
-    <t>2010Q2</t>
-  </si>
-  <si>
-    <t>2010Q3</t>
-  </si>
-  <si>
-    <t>2010Q4</t>
-  </si>
-  <si>
-    <t>2011Q1</t>
-  </si>
-  <si>
-    <t>2011Q2</t>
-  </si>
-  <si>
-    <t>2011Q3</t>
-  </si>
-  <si>
-    <t>2011Q4</t>
-  </si>
-  <si>
-    <t>2012Q1</t>
-  </si>
-  <si>
-    <t>2012Q2</t>
-  </si>
-  <si>
-    <t>2012Q3</t>
-  </si>
-  <si>
-    <t>2012Q4</t>
-  </si>
-  <si>
-    <t>2013Q1</t>
-  </si>
-  <si>
-    <t>2013Q2</t>
-  </si>
-  <si>
-    <t>2013Q3</t>
-  </si>
-  <si>
-    <t>2013Q4</t>
-  </si>
-  <si>
-    <t>2014Q1</t>
-  </si>
-  <si>
-    <t>2014Q2</t>
-  </si>
-  <si>
-    <t>2014Q3</t>
-  </si>
-  <si>
-    <t>2014Q4</t>
-  </si>
-  <si>
-    <t>2015Q1</t>
-  </si>
-  <si>
-    <t>2015Q2</t>
-  </si>
-  <si>
-    <t>2015Q3</t>
-  </si>
-  <si>
-    <t>2015Q4</t>
-  </si>
-  <si>
-    <t>2016Q1</t>
-  </si>
-  <si>
-    <t>2016Q2</t>
-  </si>
-  <si>
-    <t>2016Q3</t>
-  </si>
-  <si>
-    <t>2016Q4</t>
-  </si>
-  <si>
-    <t>2017Q1</t>
-  </si>
-  <si>
-    <t>2017Q2</t>
-  </si>
-  <si>
-    <t>2017Q3</t>
-  </si>
-  <si>
-    <t>2017Q4</t>
-  </si>
-  <si>
-    <t>2018Q1</t>
-  </si>
-  <si>
-    <t>2018Q2</t>
-  </si>
-  <si>
-    <t>2018Q3</t>
-  </si>
-  <si>
-    <t>2018Q4</t>
-  </si>
-  <si>
-    <t>2019Q1</t>
-  </si>
-  <si>
-    <t>2019Q2</t>
-  </si>
-  <si>
-    <t>2019Q3</t>
-  </si>
-  <si>
-    <t>2019Q4</t>
-  </si>
-  <si>
-    <t>2020Q1</t>
-  </si>
-  <si>
-    <t>2020Q2</t>
-  </si>
-  <si>
-    <t>2020Q3</t>
-  </si>
-  <si>
-    <t>2020Q4</t>
-  </si>
-  <si>
-    <t>2021Q1</t>
-  </si>
-  <si>
-    <t>2021Q2</t>
-  </si>
-  <si>
-    <t>2021Q3</t>
-  </si>
-  <si>
-    <t>2021Q4</t>
-  </si>
-  <si>
-    <t>2022Q1</t>
-  </si>
-  <si>
-    <t>2022Q2</t>
-  </si>
-  <si>
-    <t>2022Q3</t>
-  </si>
-  <si>
-    <t>2022Q4</t>
-  </si>
-  <si>
-    <t>2023Q1</t>
-  </si>
-  <si>
-    <t>2023Q2</t>
-  </si>
-  <si>
-    <t>2023Q3</t>
-  </si>
-  <si>
-    <t>2023Q4</t>
-  </si>
-  <si>
-    <t>2024Q1</t>
-  </si>
-  <si>
-    <t>2024Q2</t>
-  </si>
-  <si>
-    <t>2024Q3</t>
-  </si>
-  <si>
-    <t>2024Q4</t>
-  </si>
-  <si>
-    <t>2025Q1</t>
-  </si>
-  <si>
-    <t>2025Q2</t>
-  </si>
-  <si>
-    <t>2025Q3</t>
-  </si>
-  <si>
-    <t>2025Q4</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -747,12 +70,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1505,8 +825,8 @@
       </c>
     </row>
     <row r="2" spans="1:150">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="1">
+        <v>25569</v>
       </c>
       <c r="B2">
         <v>78.38903449704861</v>
@@ -1957,8 +1277,8 @@
       </c>
     </row>
     <row r="3" spans="1:150">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
+      <c r="A3" s="1">
+        <v>25659</v>
       </c>
       <c r="B3">
         <v>81.48467836391049</v>
@@ -2409,8 +1729,8 @@
       </c>
     </row>
     <row r="4" spans="1:150">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
+      <c r="A4" s="1">
+        <v>25750</v>
       </c>
       <c r="B4">
         <v>83.01213421926997</v>
@@ -2861,8 +2181,8 @@
       </c>
     </row>
     <row r="5" spans="1:150">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
+      <c r="A5" s="1">
+        <v>25842</v>
       </c>
       <c r="B5">
         <v>83.72494695177107</v>
@@ -3313,8 +2633,8 @@
       </c>
     </row>
     <row r="6" spans="1:150">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
+      <c r="A6" s="1">
+        <v>25934</v>
       </c>
       <c r="B6">
         <v>82.09566070605429</v>
@@ -3765,8 +3085,8 @@
       </c>
     </row>
     <row r="7" spans="1:150">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
+      <c r="A7" s="1">
+        <v>26024</v>
       </c>
       <c r="B7">
         <v>83.84714342019983</v>
@@ -4217,8 +3537,8 @@
       </c>
     </row>
     <row r="8" spans="1:150">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
+      <c r="A8" s="1">
+        <v>26115</v>
       </c>
       <c r="B8">
         <v>85.27276888520201</v>
@@ -4669,8 +3989,8 @@
       </c>
     </row>
     <row r="9" spans="1:150">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
+      <c r="A9" s="1">
+        <v>26207</v>
       </c>
       <c r="B9">
         <v>85.19130457291617</v>
@@ -5121,8 +4441,8 @@
       </c>
     </row>
     <row r="10" spans="1:150">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
+      <c r="A10" s="1">
+        <v>26299</v>
       </c>
       <c r="B10">
         <v>85.27276888520201</v>
@@ -5573,8 +4893,8 @@
       </c>
     </row>
     <row r="11" spans="1:150">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
+      <c r="A11" s="1">
+        <v>26390</v>
       </c>
       <c r="B11">
         <v>86.67802827213274</v>
@@ -6025,8 +5345,8 @@
       </c>
     </row>
     <row r="12" spans="1:150">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
+      <c r="A12" s="1">
+        <v>26481</v>
       </c>
       <c r="B12">
         <v>88.69427000120724</v>
@@ -6477,8 +5797,8 @@
       </c>
     </row>
     <row r="13" spans="1:150">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
+      <c r="A13" s="1">
+        <v>26573</v>
       </c>
       <c r="B13">
         <v>90.05879723199506</v>
@@ -6929,8 +6249,8 @@
       </c>
     </row>
     <row r="14" spans="1:150">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
+      <c r="A14" s="1">
+        <v>26665</v>
       </c>
       <c r="B14">
         <v>91.36222622856847</v>
@@ -7381,8 +6701,8 @@
       </c>
     </row>
     <row r="15" spans="1:150">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
+      <c r="A15" s="1">
+        <v>26755</v>
       </c>
       <c r="B15">
         <v>91.99357464878373</v>
@@ -7833,8 +7153,8 @@
       </c>
     </row>
     <row r="16" spans="1:150">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
+      <c r="A16" s="1">
+        <v>26846</v>
       </c>
       <c r="B16">
         <v>92.31943189792709</v>
@@ -8285,8 +7605,8 @@
       </c>
     </row>
     <row r="17" spans="1:150">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
+      <c r="A17" s="1">
+        <v>26938</v>
       </c>
       <c r="B17">
         <v>92.52309267864169</v>
@@ -8737,8 +8057,8 @@
       </c>
     </row>
     <row r="18" spans="1:150">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
+      <c r="A18" s="1">
+        <v>27030</v>
       </c>
       <c r="B18">
         <v>93.29700364535717</v>
@@ -9189,8 +8509,8 @@
       </c>
     </row>
     <row r="19" spans="1:150">
-      <c r="A19" s="2" t="s">
-        <v>17</v>
+      <c r="A19" s="1">
+        <v>27120</v>
       </c>
       <c r="B19">
         <v>93.21553933307132</v>
@@ -9641,8 +8961,8 @@
       </c>
     </row>
     <row r="20" spans="1:150">
-      <c r="A20" s="2" t="s">
-        <v>18</v>
+      <c r="A20" s="1">
+        <v>27211</v>
       </c>
       <c r="B20">
         <v>93.23590541114278</v>
@@ -10093,8 +9413,8 @@
       </c>
     </row>
     <row r="21" spans="1:150">
-      <c r="A21" s="2" t="s">
-        <v>19</v>
+      <c r="A21" s="1">
+        <v>27303</v>
       </c>
       <c r="B21">
         <v>92.07503896106957</v>
@@ -10545,8 +9865,8 @@
       </c>
     </row>
     <row r="22" spans="1:150">
-      <c r="A22" s="2" t="s">
-        <v>20</v>
+      <c r="A22" s="1">
+        <v>27395</v>
       </c>
       <c r="B22">
         <v>91.54552093121163</v>
@@ -10997,8 +10317,8 @@
       </c>
     </row>
     <row r="23" spans="1:150">
-      <c r="A23" s="2" t="s">
-        <v>21</v>
+      <c r="A23" s="1">
+        <v>27485</v>
       </c>
       <c r="B23">
         <v>91.07710113556804</v>
@@ -11449,8 +10769,8 @@
       </c>
     </row>
     <row r="24" spans="1:150">
-      <c r="A24" s="2" t="s">
-        <v>22</v>
+      <c r="A24" s="1">
+        <v>27576</v>
       </c>
       <c r="B24">
         <v>92.07503896106957</v>
@@ -11901,8 +11221,8 @@
       </c>
     </row>
     <row r="25" spans="1:150">
-      <c r="A25" s="2" t="s">
-        <v>23</v>
+      <c r="A25" s="1">
+        <v>27668</v>
       </c>
       <c r="B25">
         <v>93.88761990942949</v>
@@ -12353,8 +11673,8 @@
       </c>
     </row>
     <row r="26" spans="1:150">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
+      <c r="A26" s="1">
+        <v>27760</v>
       </c>
       <c r="B26">
         <v>94.70226303228787</v>
@@ -12805,8 +12125,8 @@
       </c>
     </row>
     <row r="27" spans="1:150">
-      <c r="A27" s="2" t="s">
-        <v>25</v>
+      <c r="A27" s="1">
+        <v>27851</v>
       </c>
       <c r="B27">
         <v>96.12788849729007</v>
@@ -13257,8 +12577,8 @@
       </c>
     </row>
     <row r="28" spans="1:150">
-      <c r="A28" s="2" t="s">
-        <v>26</v>
+      <c r="A28" s="1">
+        <v>27942</v>
       </c>
       <c r="B28">
         <v>96.14825457536152</v>
@@ -13709,8 +13029,8 @@
       </c>
     </row>
     <row r="29" spans="1:150">
-      <c r="A29" s="2" t="s">
-        <v>27</v>
+      <c r="A29" s="1">
+        <v>28034</v>
       </c>
       <c r="B29">
         <v>97.94046944564998</v>
@@ -14161,8 +13481,8 @@
       </c>
     </row>
     <row r="30" spans="1:150">
-      <c r="A30" s="2" t="s">
-        <v>28</v>
+      <c r="A30" s="1">
+        <v>28126</v>
       </c>
       <c r="B30">
         <v>98.79584472465129</v>
@@ -14613,8 +13933,8 @@
       </c>
     </row>
     <row r="31" spans="1:150">
-      <c r="A31" s="2" t="s">
-        <v>29</v>
+      <c r="A31" s="1">
+        <v>28216</v>
       </c>
       <c r="B31">
         <v>99.3457288325807</v>
@@ -15065,8 +14385,8 @@
       </c>
     </row>
     <row r="32" spans="1:150">
-      <c r="A32" s="2" t="s">
-        <v>30</v>
+      <c r="A32" s="1">
+        <v>28307</v>
       </c>
       <c r="B32">
         <v>99.30499667643778</v>
@@ -15517,8 +14837,8 @@
       </c>
     </row>
     <row r="33" spans="1:150">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
+      <c r="A33" s="1">
+        <v>28399</v>
       </c>
       <c r="B33">
         <v>101.0157472344404</v>
@@ -15969,8 +15289,8 @@
       </c>
     </row>
     <row r="34" spans="1:150">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
+      <c r="A34" s="1">
+        <v>28491</v>
       </c>
       <c r="B34">
         <v>101.4230687958696</v>
@@ -16421,8 +15741,8 @@
       </c>
     </row>
     <row r="35" spans="1:150">
-      <c r="A35" s="2" t="s">
-        <v>33</v>
+      <c r="A35" s="1">
+        <v>28581</v>
       </c>
       <c r="B35">
         <v>101.8507564353702</v>
@@ -16873,8 +16193,8 @@
       </c>
     </row>
     <row r="36" spans="1:150">
-      <c r="A36" s="2" t="s">
-        <v>34</v>
+      <c r="A36" s="1">
+        <v>28672</v>
       </c>
       <c r="B36">
         <v>103.1745515100151</v>
@@ -17325,8 +16645,8 @@
       </c>
     </row>
     <row r="37" spans="1:150">
-      <c r="A37" s="2" t="s">
-        <v>35</v>
+      <c r="A37" s="1">
+        <v>28764</v>
       </c>
       <c r="B37">
         <v>104.3761501162313</v>
@@ -17777,8 +17097,8 @@
       </c>
     </row>
     <row r="38" spans="1:150">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
+      <c r="A38" s="1">
+        <v>28856</v>
       </c>
       <c r="B38">
         <v>104.5187126627315</v>
@@ -18229,8 +17549,8 @@
       </c>
     </row>
     <row r="39" spans="1:150">
-      <c r="A39" s="2" t="s">
-        <v>37</v>
+      <c r="A39" s="1">
+        <v>28946</v>
       </c>
       <c r="B39">
         <v>107.7569190760936</v>
@@ -18681,8 +18001,8 @@
       </c>
     </row>
     <row r="40" spans="1:150">
-      <c r="A40" s="2" t="s">
-        <v>38</v>
+      <c r="A40" s="1">
+        <v>29037</v>
       </c>
       <c r="B40">
         <v>107.7569190760936</v>
@@ -19133,8 +18453,8 @@
       </c>
     </row>
     <row r="41" spans="1:150">
-      <c r="A41" s="2" t="s">
-        <v>39</v>
+      <c r="A41" s="1">
+        <v>29129</v>
       </c>
       <c r="B41">
         <v>108.4289996524518</v>
@@ -19585,8 +18905,8 @@
       </c>
     </row>
     <row r="42" spans="1:150">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
+      <c r="A42" s="1">
+        <v>29221</v>
       </c>
       <c r="B42">
         <v>109.2843749314531</v>
@@ -20037,8 +19357,8 @@
       </c>
     </row>
     <row r="43" spans="1:150">
-      <c r="A43" s="2" t="s">
-        <v>41</v>
+      <c r="A43" s="1">
+        <v>29312</v>
       </c>
       <c r="B43">
         <v>108.571562198952</v>
@@ -20489,8 +19809,8 @@
       </c>
     </row>
     <row r="44" spans="1:150">
-      <c r="A44" s="2" t="s">
-        <v>42</v>
+      <c r="A44" s="1">
+        <v>29403</v>
       </c>
       <c r="B44">
         <v>108.1235084813799</v>
@@ -20941,8 +20261,8 @@
       </c>
     </row>
     <row r="45" spans="1:150">
-      <c r="A45" s="2" t="s">
-        <v>43</v>
+      <c r="A45" s="1">
+        <v>29495</v>
       </c>
       <c r="B45">
         <v>107.9809459348796</v>
@@ -21393,8 +20713,8 @@
       </c>
     </row>
     <row r="46" spans="1:150">
-      <c r="A46" s="2" t="s">
-        <v>44</v>
+      <c r="A46" s="1">
+        <v>29587</v>
       </c>
       <c r="B46">
         <v>109.2843749314531</v>
@@ -21845,8 +21165,8 @@
       </c>
     </row>
     <row r="47" spans="1:150">
-      <c r="A47" s="2" t="s">
-        <v>45</v>
+      <c r="A47" s="1">
+        <v>29677</v>
       </c>
       <c r="B47">
         <v>108.9992498384526</v>
@@ -22297,8 +21617,8 @@
       </c>
     </row>
     <row r="48" spans="1:150">
-      <c r="A48" s="2" t="s">
-        <v>46</v>
+      <c r="A48" s="1">
+        <v>29768</v>
       </c>
       <c r="B48">
         <v>109.3047410095245</v>
@@ -22749,8 +22069,8 @@
       </c>
     </row>
     <row r="49" spans="1:150">
-      <c r="A49" s="2" t="s">
-        <v>47</v>
+      <c r="A49" s="1">
+        <v>29860</v>
       </c>
       <c r="B49">
         <v>109.1825445410958</v>
@@ -23201,8 +22521,8 @@
       </c>
     </row>
     <row r="50" spans="1:150">
-      <c r="A50" s="2" t="s">
-        <v>48</v>
+      <c r="A50" s="1">
+        <v>29952</v>
       </c>
       <c r="B50">
         <v>109.6305982586679</v>
@@ -23653,8 +22973,8 @@
       </c>
     </row>
     <row r="51" spans="1:150">
-      <c r="A51" s="2" t="s">
-        <v>49</v>
+      <c r="A51" s="1">
+        <v>30042</v>
       </c>
       <c r="B51">
         <v>108.9381516042383</v>
@@ -24105,8 +23425,8 @@
       </c>
     </row>
     <row r="52" spans="1:150">
-      <c r="A52" s="2" t="s">
-        <v>50</v>
+      <c r="A52" s="1">
+        <v>30133</v>
       </c>
       <c r="B52">
         <v>107.8994816225938</v>
@@ -24557,8 +23877,8 @@
       </c>
     </row>
     <row r="53" spans="1:150">
-      <c r="A53" s="2" t="s">
-        <v>51</v>
+      <c r="A53" s="1">
+        <v>30225</v>
       </c>
       <c r="B53">
         <v>108.1235084813799</v>
@@ -25009,8 +24329,8 @@
       </c>
     </row>
     <row r="54" spans="1:150">
-      <c r="A54" s="2" t="s">
-        <v>52</v>
+      <c r="A54" s="1">
+        <v>30317</v>
       </c>
       <c r="B54">
         <v>109.1214463068814</v>
@@ -25461,8 +24781,8 @@
       </c>
     </row>
     <row r="55" spans="1:150">
-      <c r="A55" s="2" t="s">
-        <v>53</v>
+      <c r="A55" s="1">
+        <v>30407</v>
       </c>
       <c r="B55">
         <v>110.2823127569546</v>
@@ -25913,8 +25233,8 @@
       </c>
     </row>
     <row r="56" spans="1:150">
-      <c r="A56" s="2" t="s">
-        <v>54</v>
+      <c r="A56" s="1">
+        <v>30498</v>
       </c>
       <c r="B56">
         <v>110.0175537420256</v>
@@ -26365,8 +25685,8 @@
       </c>
     </row>
     <row r="57" spans="1:150">
-      <c r="A57" s="2" t="s">
-        <v>55</v>
+      <c r="A57" s="1">
+        <v>30590</v>
       </c>
       <c r="B57">
         <v>111.5450095973851</v>
@@ -26817,8 +26137,8 @@
       </c>
     </row>
     <row r="58" spans="1:150">
-      <c r="A58" s="2" t="s">
-        <v>56</v>
+      <c r="A58" s="1">
+        <v>30682</v>
       </c>
       <c r="B58">
         <v>113.0113672185302</v>
@@ -27269,8 +26589,8 @@
       </c>
     </row>
     <row r="59" spans="1:150">
-      <c r="A59" s="2" t="s">
-        <v>57</v>
+      <c r="A59" s="1">
+        <v>30773</v>
       </c>
       <c r="B59">
         <v>111.2395184263132</v>
@@ -27721,8 +27041,8 @@
       </c>
     </row>
     <row r="60" spans="1:150">
-      <c r="A60" s="2" t="s">
-        <v>58</v>
+      <c r="A60" s="1">
+        <v>30864</v>
       </c>
       <c r="B60">
         <v>114.2740640589607</v>
@@ -28173,8 +27493,8 @@
       </c>
     </row>
     <row r="61" spans="1:150">
-      <c r="A61" s="2" t="s">
-        <v>59</v>
+      <c r="A61" s="1">
+        <v>30956</v>
       </c>
       <c r="B61">
         <v>115.2312697283193</v>
@@ -28625,8 +27945,8 @@
       </c>
     </row>
     <row r="62" spans="1:150">
-      <c r="A62" s="2" t="s">
-        <v>60</v>
+      <c r="A62" s="1">
+        <v>31048</v>
       </c>
       <c r="B62">
         <v>114.6202873861755</v>
@@ -29077,8 +28397,8 @@
       </c>
     </row>
     <row r="63" spans="1:150">
-      <c r="A63" s="2" t="s">
-        <v>61</v>
+      <c r="A63" s="1">
+        <v>31138</v>
       </c>
       <c r="B63">
         <v>115.7404216801058</v>
@@ -29529,8 +28849,8 @@
       </c>
     </row>
     <row r="64" spans="1:150">
-      <c r="A64" s="2" t="s">
-        <v>62</v>
+      <c r="A64" s="1">
+        <v>31229</v>
       </c>
       <c r="B64">
         <v>117.2475114573938</v>
@@ -29981,8 +29301,8 @@
       </c>
     </row>
     <row r="65" spans="1:150">
-      <c r="A65" s="2" t="s">
-        <v>63</v>
+      <c r="A65" s="1">
+        <v>31321</v>
       </c>
       <c r="B65">
         <v>117.9603241898949</v>
@@ -30433,8 +29753,8 @@
       </c>
     </row>
     <row r="66" spans="1:150">
-      <c r="A66" s="2" t="s">
-        <v>64</v>
+      <c r="A66" s="1">
+        <v>31413</v>
       </c>
       <c r="B66">
         <v>117.2882436135368</v>
@@ -30885,8 +30205,8 @@
       </c>
     </row>
     <row r="67" spans="1:150">
-      <c r="A67" s="2" t="s">
-        <v>65</v>
+      <c r="A67" s="1">
+        <v>31503</v>
       </c>
       <c r="B67">
         <v>118.6527708443246</v>
@@ -31337,8 +30657,8 @@
       </c>
     </row>
     <row r="68" spans="1:150">
-      <c r="A68" s="2" t="s">
-        <v>66</v>
+      <c r="A68" s="1">
+        <v>31594</v>
       </c>
       <c r="B68">
         <v>119.5285122013973</v>
@@ -31789,8 +31109,8 @@
       </c>
     </row>
     <row r="69" spans="1:150">
-      <c r="A69" s="2" t="s">
-        <v>67</v>
+      <c r="A69" s="1">
+        <v>31686</v>
       </c>
       <c r="B69">
         <v>120.709744729542</v>
@@ -32241,8 +31561,8 @@
       </c>
     </row>
     <row r="70" spans="1:150">
-      <c r="A70" s="2" t="s">
-        <v>68</v>
+      <c r="A70" s="1">
+        <v>31778</v>
       </c>
       <c r="B70">
         <v>117.6751990968945</v>
@@ -32693,8 +32013,8 @@
       </c>
     </row>
     <row r="71" spans="1:150">
-      <c r="A71" s="2" t="s">
-        <v>69</v>
+      <c r="A71" s="1">
+        <v>31868</v>
       </c>
       <c r="B71">
         <v>120.3227892461843</v>
@@ -33145,8 +32465,8 @@
       </c>
     </row>
     <row r="72" spans="1:150">
-      <c r="A72" s="2" t="s">
-        <v>70</v>
+      <c r="A72" s="1">
+        <v>31959</v>
       </c>
       <c r="B72">
         <v>121.1781645251856</v>
@@ -33597,8 +32917,8 @@
       </c>
     </row>
     <row r="73" spans="1:150">
-      <c r="A73" s="2" t="s">
-        <v>71</v>
+      <c r="A73" s="1">
+        <v>32051</v>
       </c>
       <c r="B73">
         <v>123.0925758639028</v>
@@ -34049,8 +33369,8 @@
       </c>
     </row>
     <row r="74" spans="1:150">
-      <c r="A74" s="2" t="s">
-        <v>72</v>
+      <c r="A74" s="1">
+        <v>32143</v>
       </c>
       <c r="B74">
         <v>121.992807648044</v>
@@ -34501,8 +33821,8 @@
       </c>
     </row>
     <row r="75" spans="1:150">
-      <c r="A75" s="2" t="s">
-        <v>73</v>
+      <c r="A75" s="1">
+        <v>32234</v>
       </c>
       <c r="B75">
         <v>124.2127101578331</v>
@@ -34953,8 +34273,8 @@
       </c>
     </row>
     <row r="76" spans="1:150">
-      <c r="A76" s="2" t="s">
-        <v>74</v>
+      <c r="A76" s="1">
+        <v>32325</v>
       </c>
       <c r="B76">
         <v>125.5772373886209</v>
@@ -35405,8 +34725,8 @@
       </c>
     </row>
     <row r="77" spans="1:150">
-      <c r="A77" s="2" t="s">
-        <v>75</v>
+      <c r="A77" s="1">
+        <v>32417</v>
       </c>
       <c r="C77">
         <v>127.0843271659089</v>
@@ -35854,8 +35174,8 @@
       </c>
     </row>
     <row r="78" spans="1:150">
-      <c r="A78" s="2" t="s">
-        <v>76</v>
+      <c r="A78" s="1">
+        <v>32509</v>
       </c>
       <c r="D78">
         <v>128.3877561624823</v>
@@ -36300,8 +35620,8 @@
       </c>
     </row>
     <row r="79" spans="1:150">
-      <c r="A79" s="2" t="s">
-        <v>77</v>
+      <c r="A79" s="1">
+        <v>32599</v>
       </c>
       <c r="E79">
         <v>128.9172741923403</v>
@@ -36743,8 +36063,8 @@
       </c>
     </row>
     <row r="80" spans="1:150">
-      <c r="A80" s="2" t="s">
-        <v>78</v>
+      <c r="A80" s="1">
+        <v>32690</v>
       </c>
       <c r="F80">
         <v>130.0781406424135</v>
@@ -37183,8 +36503,8 @@
       </c>
     </row>
     <row r="81" spans="1:150">
-      <c r="A81" s="2" t="s">
-        <v>79</v>
+      <c r="A81" s="1">
+        <v>32782</v>
       </c>
       <c r="G81">
         <v>131.605596497773</v>
@@ -37620,8 +36940,8 @@
       </c>
     </row>
     <row r="82" spans="1:150">
-      <c r="A82" s="2" t="s">
-        <v>80</v>
+      <c r="A82" s="1">
+        <v>32874</v>
       </c>
       <c r="H82">
         <v>134.3346509593486</v>
@@ -38054,8 +37374,8 @@
       </c>
     </row>
     <row r="83" spans="1:150">
-      <c r="A83" s="2" t="s">
-        <v>81</v>
+      <c r="A83" s="1">
+        <v>32964</v>
       </c>
       <c r="I83">
         <v>134.9863654576353</v>
@@ -38485,8 +37805,8 @@
       </c>
     </row>
     <row r="84" spans="1:150">
-      <c r="A84" s="2" t="s">
-        <v>82</v>
+      <c r="A84" s="1">
+        <v>33055</v>
       </c>
       <c r="J84">
         <v>137.8376163876397</v>
@@ -38913,8 +38233,8 @@
       </c>
     </row>
     <row r="85" spans="1:150">
-      <c r="A85" s="2" t="s">
-        <v>83</v>
+      <c r="A85" s="1">
+        <v>33147</v>
       </c>
       <c r="K85">
         <v>140.2815457562148</v>
@@ -39338,8 +38658,8 @@
       </c>
     </row>
     <row r="86" spans="1:150">
-      <c r="A86" s="2" t="s">
-        <v>84</v>
+      <c r="A86" s="1">
+        <v>33239</v>
       </c>
       <c r="L86">
         <v>144.1511005897922</v>
@@ -39760,8 +39080,8 @@
       </c>
     </row>
     <row r="87" spans="1:150">
-      <c r="A87" s="2" t="s">
-        <v>85</v>
+      <c r="A87" s="1">
+        <v>33329</v>
       </c>
       <c r="M87">
         <v>145.7563919552551</v>
@@ -40179,8 +39499,8 @@
       </c>
     </row>
     <row r="88" spans="1:150">
-      <c r="A88" s="2" t="s">
-        <v>86</v>
+      <c r="A88" s="1">
+        <v>33420</v>
       </c>
       <c r="N88">
         <v>144.8826257689904</v>
@@ -40595,8 +39915,8 @@
       </c>
     </row>
     <row r="89" spans="1:150">
-      <c r="A89" s="2" t="s">
-        <v>87</v>
+      <c r="A89" s="1">
+        <v>33512</v>
       </c>
       <c r="O89">
         <v>146.1424746887208</v>
@@ -41008,8 +40328,8 @@
       </c>
     </row>
     <row r="90" spans="1:150">
-      <c r="A90" s="2" t="s">
-        <v>88</v>
+      <c r="A90" s="1">
+        <v>33604</v>
       </c>
       <c r="P90">
         <v>148.1135286437828</v>
@@ -41418,8 +40738,8 @@
       </c>
     </row>
     <row r="91" spans="1:150">
-      <c r="A91" s="2" t="s">
-        <v>89</v>
+      <c r="A91" s="1">
+        <v>33695</v>
       </c>
       <c r="Q91">
         <v>148.0525682121829</v>
@@ -41825,8 +41145,8 @@
       </c>
     </row>
     <row r="92" spans="1:150">
-      <c r="A92" s="2" t="s">
-        <v>90</v>
+      <c r="A92" s="1">
+        <v>33786</v>
       </c>
       <c r="R92">
         <v>147.8290466296502</v>
@@ -42229,8 +41549,8 @@
       </c>
     </row>
     <row r="93" spans="1:150">
-      <c r="A93" s="2" t="s">
-        <v>91</v>
+      <c r="A93" s="1">
+        <v>33878</v>
       </c>
       <c r="S93">
         <v>147.6258451909839</v>
@@ -42630,8 +41950,8 @@
       </c>
     </row>
     <row r="94" spans="1:150">
-      <c r="A94" s="2" t="s">
-        <v>92</v>
+      <c r="A94" s="1">
+        <v>33970</v>
       </c>
       <c r="T94">
         <v>144.9842264883235</v>
@@ -43028,8 +42348,8 @@
       </c>
     </row>
     <row r="95" spans="1:150">
-      <c r="A95" s="2" t="s">
-        <v>93</v>
+      <c r="A95" s="1">
+        <v>34060</v>
       </c>
       <c r="U95">
         <v>145.8986329623214</v>
@@ -43423,8 +42743,8 @@
       </c>
     </row>
     <row r="96" spans="1:150">
-      <c r="A96" s="2" t="s">
-        <v>94</v>
+      <c r="A96" s="1">
+        <v>34151</v>
       </c>
       <c r="V96">
         <v>146.9552804433855</v>
@@ -43815,8 +43135,8 @@
       </c>
     </row>
     <row r="97" spans="1:150">
-      <c r="A97" s="2" t="s">
-        <v>95</v>
+      <c r="A97" s="1">
+        <v>34243</v>
       </c>
       <c r="W97">
         <v>146.6707984292529</v>
@@ -44204,8 +43524,8 @@
       </c>
     </row>
     <row r="98" spans="1:150">
-      <c r="A98" s="2" t="s">
-        <v>96</v>
+      <c r="A98" s="1">
+        <v>34335</v>
       </c>
       <c r="X98">
         <v>148.3980106579154</v>
@@ -44590,8 +43910,8 @@
       </c>
     </row>
     <row r="99" spans="1:150">
-      <c r="A99" s="2" t="s">
-        <v>97</v>
+      <c r="A99" s="1">
+        <v>34425</v>
       </c>
       <c r="Y99">
         <v>150.2268236059111</v>
@@ -44973,8 +44293,8 @@
       </c>
     </row>
     <row r="100" spans="1:150">
-      <c r="A100" s="2" t="s">
-        <v>98</v>
+      <c r="A100" s="1">
+        <v>34516</v>
       </c>
       <c r="Z100">
         <v>151.1615502237756</v>
@@ -45353,8 +44673,8 @@
       </c>
     </row>
     <row r="101" spans="1:150">
-      <c r="A101" s="2" t="s">
-        <v>99</v>
+      <c r="A101" s="1">
+        <v>34608</v>
       </c>
       <c r="AA101">
         <v>152.09627684164</v>
@@ -45730,8 +45050,8 @@
       </c>
     </row>
     <row r="102" spans="1:150">
-      <c r="A102" s="2" t="s">
-        <v>100</v>
+      <c r="A102" s="1">
+        <v>34700</v>
       </c>
       <c r="AB102">
         <v>152.4213991435059</v>
@@ -46104,8 +45424,8 @@
       </c>
     </row>
     <row r="103" spans="1:150">
-      <c r="A103" s="2" t="s">
-        <v>101</v>
+      <c r="A103" s="1">
+        <v>34790</v>
       </c>
       <c r="AC103">
         <v>154.0470106528354</v>
@@ -46475,8 +45795,8 @@
       </c>
     </row>
     <row r="104" spans="1:150">
-      <c r="A104" s="2" t="s">
-        <v>102</v>
+      <c r="A104" s="1">
+        <v>34881</v>
       </c>
       <c r="AD104">
         <v>154.0266905089688</v>
@@ -46843,8 +46163,8 @@
       </c>
     </row>
     <row r="105" spans="1:150">
-      <c r="A105" s="2" t="s">
-        <v>103</v>
+      <c r="A105" s="1">
+        <v>34973</v>
       </c>
       <c r="AE105">
         <v>153.6609279193697</v>
@@ -47208,8 +46528,8 @@
       </c>
     </row>
     <row r="106" spans="1:150">
-      <c r="A106" s="2" t="s">
-        <v>104</v>
+      <c r="A106" s="1">
+        <v>35065</v>
       </c>
       <c r="AF106">
         <v>153.2545250420373</v>
@@ -47570,8 +46890,8 @@
       </c>
     </row>
     <row r="107" spans="1:150">
-      <c r="A107" s="2" t="s">
-        <v>105</v>
+      <c r="A107" s="1">
+        <v>35156</v>
       </c>
       <c r="AG107">
         <v>155.5710214428318</v>
@@ -47929,8 +47249,8 @@
       </c>
     </row>
     <row r="108" spans="1:150">
-      <c r="A108" s="2" t="s">
-        <v>106</v>
+      <c r="A108" s="1">
+        <v>35247</v>
       </c>
       <c r="AH108">
         <v>156.8715106502954</v>
@@ -48285,8 +47605,8 @@
       </c>
     </row>
     <row r="109" spans="1:150">
-      <c r="A109" s="2" t="s">
-        <v>107</v>
+      <c r="A109" s="1">
+        <v>35339</v>
       </c>
       <c r="AI109">
         <v>156.9121509380286</v>
@@ -48638,8 +47958,8 @@
       </c>
     </row>
     <row r="110" spans="1:150">
-      <c r="A110" s="2" t="s">
-        <v>108</v>
+      <c r="A110" s="1">
+        <v>35431</v>
       </c>
       <c r="AJ110">
         <v>157.6030358294937</v>
@@ -48988,8 +48308,8 @@
       </c>
     </row>
     <row r="111" spans="1:150">
-      <c r="A111" s="2" t="s">
-        <v>109</v>
+      <c r="A111" s="1">
+        <v>35521</v>
       </c>
       <c r="AK111">
         <v>158.436161728025</v>
@@ -49335,8 +48655,8 @@
       </c>
     </row>
     <row r="112" spans="1:150">
-      <c r="A112" s="2" t="s">
-        <v>110</v>
+      <c r="A112" s="1">
+        <v>35612</v>
       </c>
       <c r="AL112">
         <v>159.6960106477554</v>
@@ -49679,8 +48999,8 @@
       </c>
     </row>
     <row r="113" spans="1:150">
-      <c r="A113" s="2" t="s">
-        <v>111</v>
+      <c r="A113" s="1">
+        <v>35704</v>
       </c>
       <c r="AM113">
         <v>160.0008128057547</v>
@@ -50020,8 +49340,8 @@
       </c>
     </row>
     <row r="114" spans="1:150">
-      <c r="A114" s="2" t="s">
-        <v>112</v>
+      <c r="A114" s="1">
+        <v>35796</v>
       </c>
       <c r="AN114">
         <v>161.5654638834843</v>
@@ -50358,8 +49678,8 @@
       </c>
     </row>
     <row r="115" spans="1:150">
-      <c r="A115" s="2" t="s">
-        <v>113</v>
+      <c r="A115" s="1">
+        <v>35886</v>
       </c>
       <c r="AO115">
         <v>161.4029027325514</v>
@@ -50693,8 +50013,8 @@
       </c>
     </row>
     <row r="116" spans="1:150">
-      <c r="A116" s="2" t="s">
-        <v>114</v>
+      <c r="A116" s="1">
+        <v>35977</v>
       </c>
       <c r="AP116">
         <v>162.7033919400149</v>
@@ -51025,8 +50345,8 @@
       </c>
     </row>
     <row r="117" spans="1:150">
-      <c r="A117" s="2" t="s">
-        <v>115</v>
+      <c r="A117" s="1">
+        <v>36069</v>
       </c>
       <c r="AQ117">
         <v>161.9921869046833</v>
@@ -51354,8 +50674,8 @@
       </c>
     </row>
     <row r="118" spans="1:150">
-      <c r="A118" s="2" t="s">
-        <v>116</v>
+      <c r="A118" s="1">
+        <v>36161</v>
       </c>
       <c r="AR118">
         <v>96.39876250323853</v>
@@ -51680,8 +51000,8 @@
       </c>
     </row>
     <row r="119" spans="1:150">
-      <c r="A119" s="2" t="s">
-        <v>117</v>
+      <c r="A119" s="1">
+        <v>36251</v>
       </c>
       <c r="AS119">
         <v>95.93139919430629</v>
@@ -52003,8 +51323,8 @@
       </c>
     </row>
     <row r="120" spans="1:150">
-      <c r="A120" s="2" t="s">
-        <v>118</v>
+      <c r="A120" s="1">
+        <v>36342</v>
       </c>
       <c r="AT120">
         <v>96.86612581217075</v>
@@ -52323,8 +51643,8 @@
       </c>
     </row>
     <row r="121" spans="1:150">
-      <c r="A121" s="2" t="s">
-        <v>119</v>
+      <c r="A121" s="1">
+        <v>36434</v>
       </c>
       <c r="AU121">
         <v>97.69925171070211</v>
@@ -52640,8 +51960,8 @@
       </c>
     </row>
     <row r="122" spans="1:150">
-      <c r="A122" s="2" t="s">
-        <v>120</v>
+      <c r="A122" s="1">
+        <v>36526</v>
       </c>
       <c r="AV122">
         <v>98.29869595476735</v>
@@ -52954,8 +52274,8 @@
       </c>
     </row>
     <row r="123" spans="1:150">
-      <c r="A123" s="2" t="s">
-        <v>121</v>
+      <c r="A123" s="1">
+        <v>36617</v>
       </c>
       <c r="AW123">
         <v>99.51993660115113</v>
@@ -53265,8 +52585,8 @@
       </c>
     </row>
     <row r="124" spans="1:150">
-      <c r="A124" s="2" t="s">
-        <v>122</v>
+      <c r="A124" s="1">
+        <v>36708</v>
       </c>
       <c r="AX124">
         <v>100.2108214926162</v>
@@ -53573,8 +52893,8 @@
       </c>
     </row>
     <row r="125" spans="1:150">
-      <c r="A125" s="2" t="s">
-        <v>123</v>
+      <c r="A125" s="1">
+        <v>36800</v>
       </c>
       <c r="AY125">
         <v>100.302262140016</v>
@@ -53878,8 +53198,8 @@
       </c>
     </row>
     <row r="126" spans="1:150">
-      <c r="A126" s="2" t="s">
-        <v>124</v>
+      <c r="A126" s="1">
+        <v>36892</v>
       </c>
       <c r="AZ126">
         <v>100.6741207727751</v>
@@ -54180,8 +53500,8 @@
       </c>
     </row>
     <row r="127" spans="1:150">
-      <c r="A127" s="2" t="s">
-        <v>125</v>
+      <c r="A127" s="1">
+        <v>36982</v>
       </c>
       <c r="BA127">
         <v>100.8082337222948</v>
@@ -54479,8 +53799,8 @@
       </c>
     </row>
     <row r="128" spans="1:150">
-      <c r="A128" s="2" t="s">
-        <v>126</v>
+      <c r="A128" s="1">
+        <v>37073</v>
       </c>
       <c r="BB128">
         <v>100.6659927152284</v>
@@ -54775,8 +54095,8 @@
       </c>
     </row>
     <row r="129" spans="1:150">
-      <c r="A129" s="2" t="s">
-        <v>127</v>
+      <c r="A129" s="1">
+        <v>37165</v>
       </c>
       <c r="BC129">
         <v>100.4505991902423</v>
@@ -55068,8 +54388,8 @@
       </c>
     </row>
     <row r="130" spans="1:150">
-      <c r="A130" s="2" t="s">
-        <v>128</v>
+      <c r="A130" s="1">
+        <v>37257</v>
       </c>
       <c r="BD130">
         <v>100.6212883987219</v>
@@ -55358,8 +54678,8 @@
       </c>
     </row>
     <row r="131" spans="1:150">
-      <c r="A131" s="2" t="s">
-        <v>129</v>
+      <c r="A131" s="1">
+        <v>37347</v>
       </c>
       <c r="BE131">
         <v>100.9850189739343</v>
@@ -55645,8 +54965,8 @@
       </c>
     </row>
     <row r="132" spans="1:150">
-      <c r="A132" s="2" t="s">
-        <v>130</v>
+      <c r="A132" s="1">
+        <v>37438</v>
       </c>
       <c r="BF132">
         <v>101.1333560241606</v>
@@ -55929,8 +55249,8 @@
       </c>
     </row>
     <row r="133" spans="1:150">
-      <c r="A133" s="2" t="s">
-        <v>131</v>
+      <c r="A133" s="1">
+        <v>37530</v>
       </c>
       <c r="BG133">
         <v>101.1516441536406</v>
@@ -56210,8 +55530,8 @@
       </c>
     </row>
     <row r="134" spans="1:150">
-      <c r="A134" s="2" t="s">
-        <v>132</v>
+      <c r="A134" s="1">
+        <v>37622</v>
       </c>
       <c r="BH134">
         <v>100.9220265279478</v>
@@ -56488,8 +55808,8 @@
       </c>
     </row>
     <row r="135" spans="1:150">
-      <c r="A135" s="2" t="s">
-        <v>133</v>
+      <c r="A135" s="1">
+        <v>37712</v>
       </c>
       <c r="BI135">
         <v>101.0195632185076</v>
@@ -56763,8 +56083,8 @@
       </c>
     </row>
     <row r="136" spans="1:150">
-      <c r="A136" s="2" t="s">
-        <v>134</v>
+      <c r="A136" s="1">
+        <v>37803</v>
       </c>
       <c r="BJ136">
         <v>101.1394520673206</v>
@@ -57035,8 +56355,8 @@
       </c>
     </row>
     <row r="137" spans="1:150">
-      <c r="A137" s="2" t="s">
-        <v>135</v>
+      <c r="A137" s="1">
+        <v>37895</v>
       </c>
       <c r="BK137">
         <v>101.3365574628268</v>
@@ -57304,8 +56624,8 @@
       </c>
     </row>
     <row r="138" spans="1:150">
-      <c r="A138" s="2" t="s">
-        <v>136</v>
+      <c r="A138" s="1">
+        <v>37987</v>
       </c>
       <c r="BL138">
         <v>101.8140808436924</v>
@@ -57570,8 +56890,8 @@
       </c>
     </row>
     <row r="139" spans="1:150">
-      <c r="A139" s="2" t="s">
-        <v>137</v>
+      <c r="A139" s="1">
+        <v>38078</v>
       </c>
       <c r="BM139">
         <v>102.2021955915448</v>
@@ -57833,8 +57153,8 @@
       </c>
     </row>
     <row r="140" spans="1:150">
-      <c r="A140" s="2" t="s">
-        <v>138</v>
+      <c r="A140" s="1">
+        <v>38169</v>
       </c>
       <c r="BN140">
         <v>102.2408038648914</v>
@@ -58093,8 +57413,8 @@
       </c>
     </row>
     <row r="141" spans="1:150">
-      <c r="A141" s="2" t="s">
-        <v>139</v>
+      <c r="A141" s="1">
+        <v>38261</v>
       </c>
       <c r="BO141">
         <v>101.9258416349588</v>
@@ -58350,8 +57670,8 @@
       </c>
     </row>
     <row r="142" spans="1:150">
-      <c r="A142" s="2" t="s">
-        <v>140</v>
+      <c r="A142" s="1">
+        <v>38353</v>
       </c>
       <c r="BP142">
         <v>103.55</v>
@@ -58604,8 +57924,8 @@
       </c>
     </row>
     <row r="143" spans="1:150">
-      <c r="A143" s="2" t="s">
-        <v>141</v>
+      <c r="A143" s="1">
+        <v>38443</v>
       </c>
       <c r="BQ143">
         <v>103.09</v>
@@ -58855,8 +58175,8 @@
       </c>
     </row>
     <row r="144" spans="1:150">
-      <c r="A144" s="2" t="s">
-        <v>142</v>
+      <c r="A144" s="1">
+        <v>38534</v>
       </c>
       <c r="BR144">
         <v>103.79</v>
@@ -59103,8 +58423,8 @@
       </c>
     </row>
     <row r="145" spans="1:150">
-      <c r="A145" s="2" t="s">
-        <v>143</v>
+      <c r="A145" s="1">
+        <v>38626</v>
       </c>
       <c r="BS145">
         <v>103.9</v>
@@ -59348,8 +58668,8 @@
       </c>
     </row>
     <row r="146" spans="1:150">
-      <c r="A146" s="2" t="s">
-        <v>144</v>
+      <c r="A146" s="1">
+        <v>38718</v>
       </c>
       <c r="BT146">
         <v>104.39</v>
@@ -59590,8 +58910,8 @@
       </c>
     </row>
     <row r="147" spans="1:150">
-      <c r="A147" s="2" t="s">
-        <v>145</v>
+      <c r="A147" s="1">
+        <v>38808</v>
       </c>
       <c r="BU147">
         <v>105.26</v>
@@ -59829,8 +59149,8 @@
       </c>
     </row>
     <row r="148" spans="1:150">
-      <c r="A148" s="2" t="s">
-        <v>146</v>
+      <c r="A148" s="1">
+        <v>38899</v>
       </c>
       <c r="BV148">
         <v>106.24</v>
@@ -60065,8 +59385,8 @@
       </c>
     </row>
     <row r="149" spans="1:150">
-      <c r="A149" s="2" t="s">
-        <v>147</v>
+      <c r="A149" s="1">
+        <v>38991</v>
       </c>
       <c r="BW149">
         <v>107.48</v>
@@ -60298,8 +59618,8 @@
       </c>
     </row>
     <row r="150" spans="1:150">
-      <c r="A150" s="2" t="s">
-        <v>148</v>
+      <c r="A150" s="1">
+        <v>39083</v>
       </c>
       <c r="BX150">
         <v>108.25</v>
@@ -60528,8 +59848,8 @@
       </c>
     </row>
     <row r="151" spans="1:150">
-      <c r="A151" s="2" t="s">
-        <v>149</v>
+      <c r="A151" s="1">
+        <v>39173</v>
       </c>
       <c r="BY151">
         <v>108.27</v>
@@ -60755,8 +60075,8 @@
       </c>
     </row>
     <row r="152" spans="1:150">
-      <c r="A152" s="2" t="s">
-        <v>150</v>
+      <c r="A152" s="1">
+        <v>39264</v>
       </c>
       <c r="BZ152">
         <v>109.01</v>
@@ -60979,8 +60299,8 @@
       </c>
     </row>
     <row r="153" spans="1:150">
-      <c r="A153" s="2" t="s">
-        <v>151</v>
+      <c r="A153" s="1">
+        <v>39356</v>
       </c>
       <c r="CA153">
         <v>109.29</v>
@@ -61200,8 +60520,8 @@
       </c>
     </row>
     <row r="154" spans="1:150">
-      <c r="A154" s="2" t="s">
-        <v>152</v>
+      <c r="A154" s="1">
+        <v>39448</v>
       </c>
       <c r="CB154">
         <v>110.96</v>
@@ -61418,8 +60738,8 @@
       </c>
     </row>
     <row r="155" spans="1:150">
-      <c r="A155" s="2" t="s">
-        <v>153</v>
+      <c r="A155" s="1">
+        <v>39539</v>
       </c>
       <c r="CC155">
         <v>110.39</v>
@@ -61633,8 +60953,8 @@
       </c>
     </row>
     <row r="156" spans="1:150">
-      <c r="A156" s="2" t="s">
-        <v>154</v>
+      <c r="A156" s="1">
+        <v>39630</v>
       </c>
       <c r="CD156">
         <v>110.02</v>
@@ -61845,8 +61165,8 @@
       </c>
     </row>
     <row r="157" spans="1:150">
-      <c r="A157" s="2" t="s">
-        <v>155</v>
+      <c r="A157" s="1">
+        <v>39722</v>
       </c>
       <c r="CE157">
         <v>107.74</v>
@@ -62054,8 +61374,8 @@
       </c>
     </row>
     <row r="158" spans="1:150">
-      <c r="A158" s="2" t="s">
-        <v>156</v>
+      <c r="A158" s="1">
+        <v>39814</v>
       </c>
       <c r="CF158">
         <v>103.52</v>
@@ -62260,8 +61580,8 @@
       </c>
     </row>
     <row r="159" spans="1:150">
-      <c r="A159" s="2" t="s">
-        <v>157</v>
+      <c r="A159" s="1">
+        <v>39904</v>
       </c>
       <c r="CG159">
         <v>104.26</v>
@@ -62463,8 +61783,8 @@
       </c>
     </row>
     <row r="160" spans="1:150">
-      <c r="A160" s="2" t="s">
-        <v>158</v>
+      <c r="A160" s="1">
+        <v>39995</v>
       </c>
       <c r="CH160">
         <v>105.15</v>
@@ -62663,8 +61983,8 @@
       </c>
     </row>
     <row r="161" spans="1:150">
-      <c r="A161" s="2" t="s">
-        <v>159</v>
+      <c r="A161" s="1">
+        <v>40087</v>
       </c>
       <c r="CI161">
         <v>105.18</v>
@@ -62860,8 +62180,8 @@
       </c>
     </row>
     <row r="162" spans="1:150">
-      <c r="A162" s="2" t="s">
-        <v>160</v>
+      <c r="A162" s="1">
+        <v>40179</v>
       </c>
       <c r="CJ162">
         <v>105.53</v>
@@ -63054,8 +62374,8 @@
       </c>
     </row>
     <row r="163" spans="1:150">
-      <c r="A163" s="2" t="s">
-        <v>161</v>
+      <c r="A163" s="1">
+        <v>40269</v>
       </c>
       <c r="CK163">
         <v>108.64</v>
@@ -63245,8 +62565,8 @@
       </c>
     </row>
     <row r="164" spans="1:150">
-      <c r="A164" s="2" t="s">
-        <v>162</v>
+      <c r="A164" s="1">
+        <v>40360</v>
       </c>
       <c r="CL164">
         <v>109.64</v>
@@ -63433,8 +62753,8 @@
       </c>
     </row>
     <row r="165" spans="1:150">
-      <c r="A165" s="2" t="s">
-        <v>163</v>
+      <c r="A165" s="1">
+        <v>40452</v>
       </c>
       <c r="CM165">
         <v>110.05</v>
@@ -63618,8 +62938,8 @@
       </c>
     </row>
     <row r="166" spans="1:150">
-      <c r="A166" s="2" t="s">
-        <v>164</v>
+      <c r="A166" s="1">
+        <v>40544</v>
       </c>
       <c r="CN166">
         <v>111.71</v>
@@ -63800,8 +63120,8 @@
       </c>
     </row>
     <row r="167" spans="1:150">
-      <c r="A167" s="2" t="s">
-        <v>165</v>
+      <c r="A167" s="1">
+        <v>40634</v>
       </c>
       <c r="CO167">
         <v>109.17</v>
@@ -63979,8 +63299,8 @@
       </c>
     </row>
     <row r="168" spans="1:150">
-      <c r="A168" s="2" t="s">
-        <v>166</v>
+      <c r="A168" s="1">
+        <v>40725</v>
       </c>
       <c r="CP168">
         <v>109.89</v>
@@ -64155,8 +63475,8 @@
       </c>
     </row>
     <row r="169" spans="1:150">
-      <c r="A169" s="2" t="s">
-        <v>167</v>
+      <c r="A169" s="1">
+        <v>40817</v>
       </c>
       <c r="CQ169">
         <v>109.77</v>
@@ -64328,8 +63648,8 @@
       </c>
     </row>
     <row r="170" spans="1:150">
-      <c r="A170" s="2" t="s">
-        <v>168</v>
+      <c r="A170" s="1">
+        <v>40909</v>
       </c>
       <c r="CR170">
         <v>110.33</v>
@@ -64498,8 +63818,8 @@
       </c>
     </row>
     <row r="171" spans="1:150">
-      <c r="A171" s="2" t="s">
-        <v>169</v>
+      <c r="A171" s="1">
+        <v>41000</v>
       </c>
       <c r="CS171">
         <v>111.12</v>
@@ -64665,8 +63985,8 @@
       </c>
     </row>
     <row r="172" spans="1:150">
-      <c r="A172" s="2" t="s">
-        <v>170</v>
+      <c r="A172" s="1">
+        <v>41091</v>
       </c>
       <c r="CT172">
         <v>111.38</v>
@@ -64829,8 +64149,8 @@
       </c>
     </row>
     <row r="173" spans="1:150">
-      <c r="A173" s="2" t="s">
-        <v>171</v>
+      <c r="A173" s="1">
+        <v>41183</v>
       </c>
       <c r="CU173">
         <v>110.73</v>
@@ -64990,8 +64310,8 @@
       </c>
     </row>
     <row r="174" spans="1:150">
-      <c r="A174" s="2" t="s">
-        <v>172</v>
+      <c r="A174" s="1">
+        <v>41275</v>
       </c>
       <c r="CV174">
         <v>110.68</v>
@@ -65148,8 +64468,8 @@
       </c>
     </row>
     <row r="175" spans="1:150">
-      <c r="A175" s="2" t="s">
-        <v>173</v>
+      <c r="A175" s="1">
+        <v>41365</v>
       </c>
       <c r="CW175">
         <v>111.69</v>
@@ -65303,8 +64623,8 @@
       </c>
     </row>
     <row r="176" spans="1:150">
-      <c r="A176" s="2" t="s">
-        <v>174</v>
+      <c r="A176" s="1">
+        <v>41456</v>
       </c>
       <c r="CX176">
         <v>112.05</v>
@@ -65455,8 +64775,8 @@
       </c>
     </row>
     <row r="177" spans="1:150">
-      <c r="A177" s="2" t="s">
-        <v>175</v>
+      <c r="A177" s="1">
+        <v>41548</v>
       </c>
       <c r="CY177">
         <v>112.48</v>
@@ -65604,8 +64924,8 @@
       </c>
     </row>
     <row r="178" spans="1:150">
-      <c r="A178" s="2" t="s">
-        <v>176</v>
+      <c r="A178" s="1">
+        <v>41640</v>
       </c>
       <c r="CZ178">
         <v>113.4</v>
@@ -65750,8 +65070,8 @@
       </c>
     </row>
     <row r="179" spans="1:150">
-      <c r="A179" s="2" t="s">
-        <v>177</v>
+      <c r="A179" s="1">
+        <v>41730</v>
       </c>
       <c r="DA179">
         <v>105.5</v>
@@ -65893,8 +65213,8 @@
       </c>
     </row>
     <row r="180" spans="1:150">
-      <c r="A180" s="2" t="s">
-        <v>178</v>
+      <c r="A180" s="1">
+        <v>41821</v>
       </c>
       <c r="DB180">
         <v>105.75</v>
@@ -66033,8 +65353,8 @@
       </c>
     </row>
     <row r="181" spans="1:150">
-      <c r="A181" s="2" t="s">
-        <v>179</v>
+      <c r="A181" s="1">
+        <v>41913</v>
       </c>
       <c r="DC181">
         <v>106.5</v>
@@ -66170,8 +65490,8 @@
       </c>
     </row>
     <row r="182" spans="1:150">
-      <c r="A182" s="2" t="s">
-        <v>180</v>
+      <c r="A182" s="1">
+        <v>42005</v>
       </c>
       <c r="DD182">
         <v>106.79</v>
@@ -66304,8 +65624,8 @@
       </c>
     </row>
     <row r="183" spans="1:150">
-      <c r="A183" s="2" t="s">
-        <v>181</v>
+      <c r="A183" s="1">
+        <v>42095</v>
       </c>
       <c r="DE183">
         <v>107.62</v>
@@ -66435,8 +65755,8 @@
       </c>
     </row>
     <row r="184" spans="1:150">
-      <c r="A184" s="2" t="s">
-        <v>182</v>
+      <c r="A184" s="1">
+        <v>42186</v>
       </c>
       <c r="DF184">
         <v>107.96</v>
@@ -66563,8 +65883,8 @@
       </c>
     </row>
     <row r="185" spans="1:150">
-      <c r="A185" s="2" t="s">
-        <v>183</v>
+      <c r="A185" s="1">
+        <v>42278</v>
       </c>
       <c r="DG185">
         <v>108.22</v>
@@ -66688,8 +66008,8 @@
       </c>
     </row>
     <row r="186" spans="1:150">
-      <c r="A186" s="2" t="s">
-        <v>184</v>
+      <c r="A186" s="1">
+        <v>42370</v>
       </c>
       <c r="DH186">
         <v>108.94</v>
@@ -66810,8 +66130,8 @@
       </c>
     </row>
     <row r="187" spans="1:150">
-      <c r="A187" s="2" t="s">
-        <v>185</v>
+      <c r="A187" s="1">
+        <v>42461</v>
       </c>
       <c r="DI187">
         <v>109.87</v>
@@ -66929,8 +66249,8 @@
       </c>
     </row>
     <row r="188" spans="1:150">
-      <c r="A188" s="2" t="s">
-        <v>186</v>
+      <c r="A188" s="1">
+        <v>42552</v>
       </c>
       <c r="DJ188">
         <v>110.08</v>
@@ -67045,8 +66365,8 @@
       </c>
     </row>
     <row r="189" spans="1:150">
-      <c r="A189" s="2" t="s">
-        <v>187</v>
+      <c r="A189" s="1">
+        <v>42644</v>
       </c>
       <c r="DK189">
         <v>110.56</v>
@@ -67158,8 +66478,8 @@
       </c>
     </row>
     <row r="190" spans="1:150">
-      <c r="A190" s="2" t="s">
-        <v>188</v>
+      <c r="A190" s="1">
+        <v>42736</v>
       </c>
       <c r="DL190">
         <v>111.25</v>
@@ -67268,8 +66588,8 @@
       </c>
     </row>
     <row r="191" spans="1:150">
-      <c r="A191" s="2" t="s">
-        <v>189</v>
+      <c r="A191" s="1">
+        <v>42826</v>
       </c>
       <c r="DM191">
         <v>112.62</v>
@@ -67375,8 +66695,8 @@
       </c>
     </row>
     <row r="192" spans="1:150">
-      <c r="A192" s="2" t="s">
-        <v>190</v>
+      <c r="A192" s="1">
+        <v>42917</v>
       </c>
       <c r="DN192">
         <v>113.77</v>
@@ -67479,8 +66799,8 @@
       </c>
     </row>
     <row r="193" spans="1:150">
-      <c r="A193" s="2" t="s">
-        <v>191</v>
+      <c r="A193" s="1">
+        <v>43009</v>
       </c>
       <c r="DO193">
         <v>114.37</v>
@@ -67580,8 +66900,8 @@
       </c>
     </row>
     <row r="194" spans="1:150">
-      <c r="A194" s="2" t="s">
-        <v>192</v>
+      <c r="A194" s="1">
+        <v>43101</v>
       </c>
       <c r="DP194">
         <v>114.71</v>
@@ -67678,8 +66998,8 @@
       </c>
     </row>
     <row r="195" spans="1:150">
-      <c r="A195" s="2" t="s">
-        <v>193</v>
+      <c r="A195" s="1">
+        <v>43191</v>
       </c>
       <c r="DQ195">
         <v>115.67</v>
@@ -67773,8 +67093,8 @@
       </c>
     </row>
     <row r="196" spans="1:150">
-      <c r="A196" s="2" t="s">
-        <v>194</v>
+      <c r="A196" s="1">
+        <v>43282</v>
       </c>
       <c r="DR196">
         <v>115.44</v>
@@ -67865,8 +67185,8 @@
       </c>
     </row>
     <row r="197" spans="1:150">
-      <c r="A197" s="2" t="s">
-        <v>195</v>
+      <c r="A197" s="1">
+        <v>43374</v>
       </c>
       <c r="DS197">
         <v>115.47</v>
@@ -67954,8 +67274,8 @@
       </c>
     </row>
     <row r="198" spans="1:150">
-      <c r="A198" s="2" t="s">
-        <v>196</v>
+      <c r="A198" s="1">
+        <v>43466</v>
       </c>
       <c r="DT198">
         <v>115.96</v>
@@ -68040,8 +67360,8 @@
       </c>
     </row>
     <row r="199" spans="1:150">
-      <c r="A199" s="2" t="s">
-        <v>197</v>
+      <c r="A199" s="1">
+        <v>43556</v>
       </c>
       <c r="DU199">
         <v>107.03</v>
@@ -68123,8 +67443,8 @@
       </c>
     </row>
     <row r="200" spans="1:150">
-      <c r="A200" s="2" t="s">
-        <v>198</v>
+      <c r="A200" s="1">
+        <v>43647</v>
       </c>
       <c r="DV200">
         <v>107.03</v>
@@ -68203,8 +67523,8 @@
       </c>
     </row>
     <row r="201" spans="1:150">
-      <c r="A201" s="2" t="s">
-        <v>199</v>
+      <c r="A201" s="1">
+        <v>43739</v>
       </c>
       <c r="DW201">
         <v>107.19</v>
@@ -68280,8 +67600,8 @@
       </c>
     </row>
     <row r="202" spans="1:150">
-      <c r="A202" s="2" t="s">
-        <v>200</v>
+      <c r="A202" s="1">
+        <v>43831</v>
       </c>
       <c r="DX202">
         <v>104.74</v>
@@ -68354,8 +67674,8 @@
       </c>
     </row>
     <row r="203" spans="1:150">
-      <c r="A203" s="2" t="s">
-        <v>201</v>
+      <c r="A203" s="1">
+        <v>43922</v>
       </c>
       <c r="DY203">
         <v>94.68000000000001</v>
@@ -68425,8 +67745,8 @@
       </c>
     </row>
     <row r="204" spans="1:150">
-      <c r="A204" s="2" t="s">
-        <v>202</v>
+      <c r="A204" s="1">
+        <v>44013</v>
       </c>
       <c r="DZ204">
         <v>102.72</v>
@@ -68493,8 +67813,8 @@
       </c>
     </row>
     <row r="205" spans="1:150">
-      <c r="A205" s="2" t="s">
-        <v>203</v>
+      <c r="A205" s="1">
+        <v>44105</v>
       </c>
       <c r="EA205">
         <v>103.1</v>
@@ -68558,8 +67878,8 @@
       </c>
     </row>
     <row r="206" spans="1:150">
-      <c r="A206" s="2" t="s">
-        <v>204</v>
+      <c r="A206" s="1">
+        <v>44197</v>
       </c>
       <c r="EB206">
         <v>101.62</v>
@@ -68620,8 +67940,8 @@
       </c>
     </row>
     <row r="207" spans="1:150">
-      <c r="A207" s="2" t="s">
-        <v>205</v>
+      <c r="A207" s="1">
+        <v>44287</v>
       </c>
       <c r="EC207">
         <v>103.93</v>
@@ -68679,8 +67999,8 @@
       </c>
     </row>
     <row r="208" spans="1:150">
-      <c r="A208" s="2" t="s">
-        <v>206</v>
+      <c r="A208" s="1">
+        <v>44378</v>
       </c>
       <c r="ED208">
         <v>106.24</v>
@@ -68735,8 +68055,8 @@
       </c>
     </row>
     <row r="209" spans="1:150">
-      <c r="A209" s="2" t="s">
-        <v>207</v>
+      <c r="A209" s="1">
+        <v>44470</v>
       </c>
       <c r="EE209">
         <v>106.2</v>
@@ -68788,8 +68108,8 @@
       </c>
     </row>
     <row r="210" spans="1:150">
-      <c r="A210" s="2" t="s">
-        <v>208</v>
+      <c r="A210" s="1">
+        <v>44562</v>
       </c>
       <c r="EF210">
         <v>106.45</v>
@@ -68838,8 +68158,8 @@
       </c>
     </row>
     <row r="211" spans="1:150">
-      <c r="A211" s="2" t="s">
-        <v>209</v>
+      <c r="A211" s="1">
+        <v>44652</v>
       </c>
       <c r="EG211">
         <v>107.5</v>
@@ -68885,8 +68205,8 @@
       </c>
     </row>
     <row r="212" spans="1:150">
-      <c r="A212" s="2" t="s">
-        <v>210</v>
+      <c r="A212" s="1">
+        <v>44743</v>
       </c>
       <c r="EH212">
         <v>107.89</v>
@@ -68929,8 +68249,8 @@
       </c>
     </row>
     <row r="213" spans="1:150">
-      <c r="A213" s="2" t="s">
-        <v>211</v>
+      <c r="A213" s="1">
+        <v>44835</v>
       </c>
       <c r="EI213">
         <v>107.5</v>
@@ -68970,8 +68290,8 @@
       </c>
     </row>
     <row r="214" spans="1:150">
-      <c r="A214" s="2" t="s">
-        <v>212</v>
+      <c r="A214" s="1">
+        <v>44927</v>
       </c>
       <c r="EJ214">
         <v>107.03</v>
@@ -69008,8 +68328,8 @@
       </c>
     </row>
     <row r="215" spans="1:150">
-      <c r="A215" s="2" t="s">
-        <v>213</v>
+      <c r="A215" s="1">
+        <v>45017</v>
       </c>
       <c r="EK215">
         <v>107.78</v>
@@ -69043,8 +68363,8 @@
       </c>
     </row>
     <row r="216" spans="1:150">
-      <c r="A216" s="2" t="s">
-        <v>214</v>
+      <c r="A216" s="1">
+        <v>45108</v>
       </c>
       <c r="EL216">
         <v>107.87</v>
@@ -69075,8 +68395,8 @@
       </c>
     </row>
     <row r="217" spans="1:150">
-      <c r="A217" s="2" t="s">
-        <v>215</v>
+      <c r="A217" s="1">
+        <v>45200</v>
       </c>
       <c r="EM217">
         <v>107.68</v>
@@ -69104,8 +68424,8 @@
       </c>
     </row>
     <row r="218" spans="1:150">
-      <c r="A218" s="2" t="s">
-        <v>216</v>
+      <c r="A218" s="1">
+        <v>45292</v>
       </c>
       <c r="EN218">
         <v>107.91</v>
@@ -69130,8 +68450,8 @@
       </c>
     </row>
     <row r="219" spans="1:150">
-      <c r="A219" s="2" t="s">
-        <v>217</v>
+      <c r="A219" s="1">
+        <v>45383</v>
       </c>
       <c r="EO219">
         <v>104.78</v>
@@ -69153,8 +68473,8 @@
       </c>
     </row>
     <row r="220" spans="1:150">
-      <c r="A220" s="2" t="s">
-        <v>218</v>
+      <c r="A220" s="1">
+        <v>45474</v>
       </c>
       <c r="EP220">
         <v>104.66</v>
@@ -69173,8 +68493,8 @@
       </c>
     </row>
     <row r="221" spans="1:150">
-      <c r="A221" s="2" t="s">
-        <v>219</v>
+      <c r="A221" s="1">
+        <v>45566</v>
       </c>
       <c r="EQ221">
         <v>104.45</v>
@@ -69190,8 +68510,8 @@
       </c>
     </row>
     <row r="222" spans="1:150">
-      <c r="A222" s="2" t="s">
-        <v>220</v>
+      <c r="A222" s="1">
+        <v>45658</v>
       </c>
       <c r="ER222">
         <v>104.88</v>
@@ -69204,8 +68524,8 @@
       </c>
     </row>
     <row r="223" spans="1:150">
-      <c r="A223" s="2" t="s">
-        <v>221</v>
+      <c r="A223" s="1">
+        <v>45748</v>
       </c>
       <c r="ES223">
         <v>104.52</v>
@@ -69215,16 +68535,16 @@
       </c>
     </row>
     <row r="224" spans="1:150">
-      <c r="A224" s="2" t="s">
-        <v>222</v>
+      <c r="A224" s="1">
+        <v>45839</v>
       </c>
       <c r="ET224">
         <v>104.59</v>
       </c>
     </row>
     <row r="225" spans="1:1">
-      <c r="A225" s="2" t="s">
-        <v>223</v>
+      <c r="A225" s="1">
+        <v>45931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Quarterly indexing esoteric bug-fix operation
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/1_combined_GDP_series/absolute_combined_GDP.xlsx
@@ -826,7 +826,7 @@
     </row>
     <row r="2" spans="1:150">
       <c r="A2" s="1">
-        <v>25569</v>
+        <v>25614</v>
       </c>
       <c r="B2">
         <v>78.38903449704861</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="3" spans="1:150">
       <c r="A3" s="1">
-        <v>25659</v>
+        <v>25703</v>
       </c>
       <c r="B3">
         <v>81.48467836391049</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="4" spans="1:150">
       <c r="A4" s="1">
-        <v>25750</v>
+        <v>25795</v>
       </c>
       <c r="B4">
         <v>83.01213421926997</v>
@@ -2182,7 +2182,7 @@
     </row>
     <row r="5" spans="1:150">
       <c r="A5" s="1">
-        <v>25842</v>
+        <v>25887</v>
       </c>
       <c r="B5">
         <v>83.72494695177107</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="6" spans="1:150">
       <c r="A6" s="1">
-        <v>25934</v>
+        <v>25979</v>
       </c>
       <c r="B6">
         <v>82.09566070605429</v>
@@ -3086,7 +3086,7 @@
     </row>
     <row r="7" spans="1:150">
       <c r="A7" s="1">
-        <v>26024</v>
+        <v>26068</v>
       </c>
       <c r="B7">
         <v>83.84714342019983</v>
@@ -3538,7 +3538,7 @@
     </row>
     <row r="8" spans="1:150">
       <c r="A8" s="1">
-        <v>26115</v>
+        <v>26160</v>
       </c>
       <c r="B8">
         <v>85.27276888520201</v>
@@ -3990,7 +3990,7 @@
     </row>
     <row r="9" spans="1:150">
       <c r="A9" s="1">
-        <v>26207</v>
+        <v>26252</v>
       </c>
       <c r="B9">
         <v>85.19130457291617</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="10" spans="1:150">
       <c r="A10" s="1">
-        <v>26299</v>
+        <v>26344</v>
       </c>
       <c r="B10">
         <v>85.27276888520201</v>
@@ -4894,7 +4894,7 @@
     </row>
     <row r="11" spans="1:150">
       <c r="A11" s="1">
-        <v>26390</v>
+        <v>26434</v>
       </c>
       <c r="B11">
         <v>86.67802827213274</v>
@@ -5346,7 +5346,7 @@
     </row>
     <row r="12" spans="1:150">
       <c r="A12" s="1">
-        <v>26481</v>
+        <v>26526</v>
       </c>
       <c r="B12">
         <v>88.69427000120724</v>
@@ -5798,7 +5798,7 @@
     </row>
     <row r="13" spans="1:150">
       <c r="A13" s="1">
-        <v>26573</v>
+        <v>26618</v>
       </c>
       <c r="B13">
         <v>90.05879723199506</v>
@@ -6250,7 +6250,7 @@
     </row>
     <row r="14" spans="1:150">
       <c r="A14" s="1">
-        <v>26665</v>
+        <v>26710</v>
       </c>
       <c r="B14">
         <v>91.36222622856847</v>
@@ -6702,7 +6702,7 @@
     </row>
     <row r="15" spans="1:150">
       <c r="A15" s="1">
-        <v>26755</v>
+        <v>26799</v>
       </c>
       <c r="B15">
         <v>91.99357464878373</v>
@@ -7154,7 +7154,7 @@
     </row>
     <row r="16" spans="1:150">
       <c r="A16" s="1">
-        <v>26846</v>
+        <v>26891</v>
       </c>
       <c r="B16">
         <v>92.31943189792709</v>
@@ -7606,7 +7606,7 @@
     </row>
     <row r="17" spans="1:150">
       <c r="A17" s="1">
-        <v>26938</v>
+        <v>26983</v>
       </c>
       <c r="B17">
         <v>92.52309267864169</v>
@@ -8058,7 +8058,7 @@
     </row>
     <row r="18" spans="1:150">
       <c r="A18" s="1">
-        <v>27030</v>
+        <v>27075</v>
       </c>
       <c r="B18">
         <v>93.29700364535717</v>
@@ -8510,7 +8510,7 @@
     </row>
     <row r="19" spans="1:150">
       <c r="A19" s="1">
-        <v>27120</v>
+        <v>27164</v>
       </c>
       <c r="B19">
         <v>93.21553933307132</v>
@@ -8962,7 +8962,7 @@
     </row>
     <row r="20" spans="1:150">
       <c r="A20" s="1">
-        <v>27211</v>
+        <v>27256</v>
       </c>
       <c r="B20">
         <v>93.23590541114278</v>
@@ -9414,7 +9414,7 @@
     </row>
     <row r="21" spans="1:150">
       <c r="A21" s="1">
-        <v>27303</v>
+        <v>27348</v>
       </c>
       <c r="B21">
         <v>92.07503896106957</v>
@@ -9866,7 +9866,7 @@
     </row>
     <row r="22" spans="1:150">
       <c r="A22" s="1">
-        <v>27395</v>
+        <v>27440</v>
       </c>
       <c r="B22">
         <v>91.54552093121163</v>
@@ -10318,7 +10318,7 @@
     </row>
     <row r="23" spans="1:150">
       <c r="A23" s="1">
-        <v>27485</v>
+        <v>27529</v>
       </c>
       <c r="B23">
         <v>91.07710113556804</v>
@@ -10770,7 +10770,7 @@
     </row>
     <row r="24" spans="1:150">
       <c r="A24" s="1">
-        <v>27576</v>
+        <v>27621</v>
       </c>
       <c r="B24">
         <v>92.07503896106957</v>
@@ -11222,7 +11222,7 @@
     </row>
     <row r="25" spans="1:150">
       <c r="A25" s="1">
-        <v>27668</v>
+        <v>27713</v>
       </c>
       <c r="B25">
         <v>93.88761990942949</v>
@@ -11674,7 +11674,7 @@
     </row>
     <row r="26" spans="1:150">
       <c r="A26" s="1">
-        <v>27760</v>
+        <v>27805</v>
       </c>
       <c r="B26">
         <v>94.70226303228787</v>
@@ -12126,7 +12126,7 @@
     </row>
     <row r="27" spans="1:150">
       <c r="A27" s="1">
-        <v>27851</v>
+        <v>27895</v>
       </c>
       <c r="B27">
         <v>96.12788849729007</v>
@@ -12578,7 +12578,7 @@
     </row>
     <row r="28" spans="1:150">
       <c r="A28" s="1">
-        <v>27942</v>
+        <v>27987</v>
       </c>
       <c r="B28">
         <v>96.14825457536152</v>
@@ -13030,7 +13030,7 @@
     </row>
     <row r="29" spans="1:150">
       <c r="A29" s="1">
-        <v>28034</v>
+        <v>28079</v>
       </c>
       <c r="B29">
         <v>97.94046944564998</v>
@@ -13482,7 +13482,7 @@
     </row>
     <row r="30" spans="1:150">
       <c r="A30" s="1">
-        <v>28126</v>
+        <v>28171</v>
       </c>
       <c r="B30">
         <v>98.79584472465129</v>
@@ -13934,7 +13934,7 @@
     </row>
     <row r="31" spans="1:150">
       <c r="A31" s="1">
-        <v>28216</v>
+        <v>28260</v>
       </c>
       <c r="B31">
         <v>99.3457288325807</v>
@@ -14386,7 +14386,7 @@
     </row>
     <row r="32" spans="1:150">
       <c r="A32" s="1">
-        <v>28307</v>
+        <v>28352</v>
       </c>
       <c r="B32">
         <v>99.30499667643778</v>
@@ -14838,7 +14838,7 @@
     </row>
     <row r="33" spans="1:150">
       <c r="A33" s="1">
-        <v>28399</v>
+        <v>28444</v>
       </c>
       <c r="B33">
         <v>101.0157472344404</v>
@@ -15290,7 +15290,7 @@
     </row>
     <row r="34" spans="1:150">
       <c r="A34" s="1">
-        <v>28491</v>
+        <v>28536</v>
       </c>
       <c r="B34">
         <v>101.4230687958696</v>
@@ -15742,7 +15742,7 @@
     </row>
     <row r="35" spans="1:150">
       <c r="A35" s="1">
-        <v>28581</v>
+        <v>28625</v>
       </c>
       <c r="B35">
         <v>101.8507564353702</v>
@@ -16194,7 +16194,7 @@
     </row>
     <row r="36" spans="1:150">
       <c r="A36" s="1">
-        <v>28672</v>
+        <v>28717</v>
       </c>
       <c r="B36">
         <v>103.1745515100151</v>
@@ -16646,7 +16646,7 @@
     </row>
     <row r="37" spans="1:150">
       <c r="A37" s="1">
-        <v>28764</v>
+        <v>28809</v>
       </c>
       <c r="B37">
         <v>104.3761501162313</v>
@@ -17098,7 +17098,7 @@
     </row>
     <row r="38" spans="1:150">
       <c r="A38" s="1">
-        <v>28856</v>
+        <v>28901</v>
       </c>
       <c r="B38">
         <v>104.5187126627315</v>
@@ -17550,7 +17550,7 @@
     </row>
     <row r="39" spans="1:150">
       <c r="A39" s="1">
-        <v>28946</v>
+        <v>28990</v>
       </c>
       <c r="B39">
         <v>107.7569190760936</v>
@@ -18002,7 +18002,7 @@
     </row>
     <row r="40" spans="1:150">
       <c r="A40" s="1">
-        <v>29037</v>
+        <v>29082</v>
       </c>
       <c r="B40">
         <v>107.7569190760936</v>
@@ -18454,7 +18454,7 @@
     </row>
     <row r="41" spans="1:150">
       <c r="A41" s="1">
-        <v>29129</v>
+        <v>29174</v>
       </c>
       <c r="B41">
         <v>108.4289996524518</v>
@@ -18906,7 +18906,7 @@
     </row>
     <row r="42" spans="1:150">
       <c r="A42" s="1">
-        <v>29221</v>
+        <v>29266</v>
       </c>
       <c r="B42">
         <v>109.2843749314531</v>
@@ -19358,7 +19358,7 @@
     </row>
     <row r="43" spans="1:150">
       <c r="A43" s="1">
-        <v>29312</v>
+        <v>29356</v>
       </c>
       <c r="B43">
         <v>108.571562198952</v>
@@ -19810,7 +19810,7 @@
     </row>
     <row r="44" spans="1:150">
       <c r="A44" s="1">
-        <v>29403</v>
+        <v>29448</v>
       </c>
       <c r="B44">
         <v>108.1235084813799</v>
@@ -20262,7 +20262,7 @@
     </row>
     <row r="45" spans="1:150">
       <c r="A45" s="1">
-        <v>29495</v>
+        <v>29540</v>
       </c>
       <c r="B45">
         <v>107.9809459348796</v>
@@ -20714,7 +20714,7 @@
     </row>
     <row r="46" spans="1:150">
       <c r="A46" s="1">
-        <v>29587</v>
+        <v>29632</v>
       </c>
       <c r="B46">
         <v>109.2843749314531</v>
@@ -21166,7 +21166,7 @@
     </row>
     <row r="47" spans="1:150">
       <c r="A47" s="1">
-        <v>29677</v>
+        <v>29721</v>
       </c>
       <c r="B47">
         <v>108.9992498384526</v>
@@ -21618,7 +21618,7 @@
     </row>
     <row r="48" spans="1:150">
       <c r="A48" s="1">
-        <v>29768</v>
+        <v>29813</v>
       </c>
       <c r="B48">
         <v>109.3047410095245</v>
@@ -22070,7 +22070,7 @@
     </row>
     <row r="49" spans="1:150">
       <c r="A49" s="1">
-        <v>29860</v>
+        <v>29905</v>
       </c>
       <c r="B49">
         <v>109.1825445410958</v>
@@ -22522,7 +22522,7 @@
     </row>
     <row r="50" spans="1:150">
       <c r="A50" s="1">
-        <v>29952</v>
+        <v>29997</v>
       </c>
       <c r="B50">
         <v>109.6305982586679</v>
@@ -22974,7 +22974,7 @@
     </row>
     <row r="51" spans="1:150">
       <c r="A51" s="1">
-        <v>30042</v>
+        <v>30086</v>
       </c>
       <c r="B51">
         <v>108.9381516042383</v>
@@ -23426,7 +23426,7 @@
     </row>
     <row r="52" spans="1:150">
       <c r="A52" s="1">
-        <v>30133</v>
+        <v>30178</v>
       </c>
       <c r="B52">
         <v>107.8994816225938</v>
@@ -23878,7 +23878,7 @@
     </row>
     <row r="53" spans="1:150">
       <c r="A53" s="1">
-        <v>30225</v>
+        <v>30270</v>
       </c>
       <c r="B53">
         <v>108.1235084813799</v>
@@ -24330,7 +24330,7 @@
     </row>
     <row r="54" spans="1:150">
       <c r="A54" s="1">
-        <v>30317</v>
+        <v>30362</v>
       </c>
       <c r="B54">
         <v>109.1214463068814</v>
@@ -24782,7 +24782,7 @@
     </row>
     <row r="55" spans="1:150">
       <c r="A55" s="1">
-        <v>30407</v>
+        <v>30451</v>
       </c>
       <c r="B55">
         <v>110.2823127569546</v>
@@ -25234,7 +25234,7 @@
     </row>
     <row r="56" spans="1:150">
       <c r="A56" s="1">
-        <v>30498</v>
+        <v>30543</v>
       </c>
       <c r="B56">
         <v>110.0175537420256</v>
@@ -25686,7 +25686,7 @@
     </row>
     <row r="57" spans="1:150">
       <c r="A57" s="1">
-        <v>30590</v>
+        <v>30635</v>
       </c>
       <c r="B57">
         <v>111.5450095973851</v>
@@ -26138,7 +26138,7 @@
     </row>
     <row r="58" spans="1:150">
       <c r="A58" s="1">
-        <v>30682</v>
+        <v>30727</v>
       </c>
       <c r="B58">
         <v>113.0113672185302</v>
@@ -26590,7 +26590,7 @@
     </row>
     <row r="59" spans="1:150">
       <c r="A59" s="1">
-        <v>30773</v>
+        <v>30817</v>
       </c>
       <c r="B59">
         <v>111.2395184263132</v>
@@ -27042,7 +27042,7 @@
     </row>
     <row r="60" spans="1:150">
       <c r="A60" s="1">
-        <v>30864</v>
+        <v>30909</v>
       </c>
       <c r="B60">
         <v>114.2740640589607</v>
@@ -27494,7 +27494,7 @@
     </row>
     <row r="61" spans="1:150">
       <c r="A61" s="1">
-        <v>30956</v>
+        <v>31001</v>
       </c>
       <c r="B61">
         <v>115.2312697283193</v>
@@ -27946,7 +27946,7 @@
     </row>
     <row r="62" spans="1:150">
       <c r="A62" s="1">
-        <v>31048</v>
+        <v>31093</v>
       </c>
       <c r="B62">
         <v>114.6202873861755</v>
@@ -28398,7 +28398,7 @@
     </row>
     <row r="63" spans="1:150">
       <c r="A63" s="1">
-        <v>31138</v>
+        <v>31182</v>
       </c>
       <c r="B63">
         <v>115.7404216801058</v>
@@ -28850,7 +28850,7 @@
     </row>
     <row r="64" spans="1:150">
       <c r="A64" s="1">
-        <v>31229</v>
+        <v>31274</v>
       </c>
       <c r="B64">
         <v>117.2475114573938</v>
@@ -29302,7 +29302,7 @@
     </row>
     <row r="65" spans="1:150">
       <c r="A65" s="1">
-        <v>31321</v>
+        <v>31366</v>
       </c>
       <c r="B65">
         <v>117.9603241898949</v>
@@ -29754,7 +29754,7 @@
     </row>
     <row r="66" spans="1:150">
       <c r="A66" s="1">
-        <v>31413</v>
+        <v>31458</v>
       </c>
       <c r="B66">
         <v>117.2882436135368</v>
@@ -30206,7 +30206,7 @@
     </row>
     <row r="67" spans="1:150">
       <c r="A67" s="1">
-        <v>31503</v>
+        <v>31547</v>
       </c>
       <c r="B67">
         <v>118.6527708443246</v>
@@ -30658,7 +30658,7 @@
     </row>
     <row r="68" spans="1:150">
       <c r="A68" s="1">
-        <v>31594</v>
+        <v>31639</v>
       </c>
       <c r="B68">
         <v>119.5285122013973</v>
@@ -31110,7 +31110,7 @@
     </row>
     <row r="69" spans="1:150">
       <c r="A69" s="1">
-        <v>31686</v>
+        <v>31731</v>
       </c>
       <c r="B69">
         <v>120.709744729542</v>
@@ -31562,7 +31562,7 @@
     </row>
     <row r="70" spans="1:150">
       <c r="A70" s="1">
-        <v>31778</v>
+        <v>31823</v>
       </c>
       <c r="B70">
         <v>117.6751990968945</v>
@@ -32014,7 +32014,7 @@
     </row>
     <row r="71" spans="1:150">
       <c r="A71" s="1">
-        <v>31868</v>
+        <v>31912</v>
       </c>
       <c r="B71">
         <v>120.3227892461843</v>
@@ -32466,7 +32466,7 @@
     </row>
     <row r="72" spans="1:150">
       <c r="A72" s="1">
-        <v>31959</v>
+        <v>32004</v>
       </c>
       <c r="B72">
         <v>121.1781645251856</v>
@@ -32918,7 +32918,7 @@
     </row>
     <row r="73" spans="1:150">
       <c r="A73" s="1">
-        <v>32051</v>
+        <v>32096</v>
       </c>
       <c r="B73">
         <v>123.0925758639028</v>
@@ -33370,7 +33370,7 @@
     </row>
     <row r="74" spans="1:150">
       <c r="A74" s="1">
-        <v>32143</v>
+        <v>32188</v>
       </c>
       <c r="B74">
         <v>121.992807648044</v>
@@ -33822,7 +33822,7 @@
     </row>
     <row r="75" spans="1:150">
       <c r="A75" s="1">
-        <v>32234</v>
+        <v>32278</v>
       </c>
       <c r="B75">
         <v>124.2127101578331</v>
@@ -34274,7 +34274,7 @@
     </row>
     <row r="76" spans="1:150">
       <c r="A76" s="1">
-        <v>32325</v>
+        <v>32370</v>
       </c>
       <c r="B76">
         <v>125.5772373886209</v>
@@ -34726,7 +34726,7 @@
     </row>
     <row r="77" spans="1:150">
       <c r="A77" s="1">
-        <v>32417</v>
+        <v>32462</v>
       </c>
       <c r="C77">
         <v>127.0843271659089</v>
@@ -35175,7 +35175,7 @@
     </row>
     <row r="78" spans="1:150">
       <c r="A78" s="1">
-        <v>32509</v>
+        <v>32554</v>
       </c>
       <c r="D78">
         <v>128.3877561624823</v>
@@ -35621,7 +35621,7 @@
     </row>
     <row r="79" spans="1:150">
       <c r="A79" s="1">
-        <v>32599</v>
+        <v>32643</v>
       </c>
       <c r="E79">
         <v>128.9172741923403</v>
@@ -36064,7 +36064,7 @@
     </row>
     <row r="80" spans="1:150">
       <c r="A80" s="1">
-        <v>32690</v>
+        <v>32735</v>
       </c>
       <c r="F80">
         <v>130.0781406424135</v>
@@ -36504,7 +36504,7 @@
     </row>
     <row r="81" spans="1:150">
       <c r="A81" s="1">
-        <v>32782</v>
+        <v>32827</v>
       </c>
       <c r="G81">
         <v>131.605596497773</v>
@@ -36941,7 +36941,7 @@
     </row>
     <row r="82" spans="1:150">
       <c r="A82" s="1">
-        <v>32874</v>
+        <v>32919</v>
       </c>
       <c r="H82">
         <v>134.3346509593486</v>
@@ -37375,7 +37375,7 @@
     </row>
     <row r="83" spans="1:150">
       <c r="A83" s="1">
-        <v>32964</v>
+        <v>33008</v>
       </c>
       <c r="I83">
         <v>134.9863654576353</v>
@@ -37806,7 +37806,7 @@
     </row>
     <row r="84" spans="1:150">
       <c r="A84" s="1">
-        <v>33055</v>
+        <v>33100</v>
       </c>
       <c r="J84">
         <v>137.8376163876397</v>
@@ -38234,7 +38234,7 @@
     </row>
     <row r="85" spans="1:150">
       <c r="A85" s="1">
-        <v>33147</v>
+        <v>33192</v>
       </c>
       <c r="K85">
         <v>140.2815457562148</v>
@@ -38659,7 +38659,7 @@
     </row>
     <row r="86" spans="1:150">
       <c r="A86" s="1">
-        <v>33239</v>
+        <v>33284</v>
       </c>
       <c r="L86">
         <v>144.1511005897922</v>
@@ -39081,7 +39081,7 @@
     </row>
     <row r="87" spans="1:150">
       <c r="A87" s="1">
-        <v>33329</v>
+        <v>33373</v>
       </c>
       <c r="M87">
         <v>145.7563919552551</v>
@@ -39500,7 +39500,7 @@
     </row>
     <row r="88" spans="1:150">
       <c r="A88" s="1">
-        <v>33420</v>
+        <v>33465</v>
       </c>
       <c r="N88">
         <v>144.8826257689904</v>
@@ -39916,7 +39916,7 @@
     </row>
     <row r="89" spans="1:150">
       <c r="A89" s="1">
-        <v>33512</v>
+        <v>33557</v>
       </c>
       <c r="O89">
         <v>146.1424746887208</v>
@@ -40329,7 +40329,7 @@
     </row>
     <row r="90" spans="1:150">
       <c r="A90" s="1">
-        <v>33604</v>
+        <v>33649</v>
       </c>
       <c r="P90">
         <v>148.1135286437828</v>
@@ -40739,7 +40739,7 @@
     </row>
     <row r="91" spans="1:150">
       <c r="A91" s="1">
-        <v>33695</v>
+        <v>33739</v>
       </c>
       <c r="Q91">
         <v>148.0525682121829</v>
@@ -41146,7 +41146,7 @@
     </row>
     <row r="92" spans="1:150">
       <c r="A92" s="1">
-        <v>33786</v>
+        <v>33831</v>
       </c>
       <c r="R92">
         <v>147.8290466296502</v>
@@ -41550,7 +41550,7 @@
     </row>
     <row r="93" spans="1:150">
       <c r="A93" s="1">
-        <v>33878</v>
+        <v>33923</v>
       </c>
       <c r="S93">
         <v>147.6258451909839</v>
@@ -41951,7 +41951,7 @@
     </row>
     <row r="94" spans="1:150">
       <c r="A94" s="1">
-        <v>33970</v>
+        <v>34015</v>
       </c>
       <c r="T94">
         <v>144.9842264883235</v>
@@ -42349,7 +42349,7 @@
     </row>
     <row r="95" spans="1:150">
       <c r="A95" s="1">
-        <v>34060</v>
+        <v>34104</v>
       </c>
       <c r="U95">
         <v>145.8986329623214</v>
@@ -42744,7 +42744,7 @@
     </row>
     <row r="96" spans="1:150">
       <c r="A96" s="1">
-        <v>34151</v>
+        <v>34196</v>
       </c>
       <c r="V96">
         <v>146.9552804433855</v>
@@ -43136,7 +43136,7 @@
     </row>
     <row r="97" spans="1:150">
       <c r="A97" s="1">
-        <v>34243</v>
+        <v>34288</v>
       </c>
       <c r="W97">
         <v>146.6707984292529</v>
@@ -43525,7 +43525,7 @@
     </row>
     <row r="98" spans="1:150">
       <c r="A98" s="1">
-        <v>34335</v>
+        <v>34380</v>
       </c>
       <c r="X98">
         <v>148.3980106579154</v>
@@ -43911,7 +43911,7 @@
     </row>
     <row r="99" spans="1:150">
       <c r="A99" s="1">
-        <v>34425</v>
+        <v>34469</v>
       </c>
       <c r="Y99">
         <v>150.2268236059111</v>
@@ -44294,7 +44294,7 @@
     </row>
     <row r="100" spans="1:150">
       <c r="A100" s="1">
-        <v>34516</v>
+        <v>34561</v>
       </c>
       <c r="Z100">
         <v>151.1615502237756</v>
@@ -44674,7 +44674,7 @@
     </row>
     <row r="101" spans="1:150">
       <c r="A101" s="1">
-        <v>34608</v>
+        <v>34653</v>
       </c>
       <c r="AA101">
         <v>152.09627684164</v>
@@ -45051,7 +45051,7 @@
     </row>
     <row r="102" spans="1:150">
       <c r="A102" s="1">
-        <v>34700</v>
+        <v>34745</v>
       </c>
       <c r="AB102">
         <v>152.4213991435059</v>
@@ -45425,7 +45425,7 @@
     </row>
     <row r="103" spans="1:150">
       <c r="A103" s="1">
-        <v>34790</v>
+        <v>34834</v>
       </c>
       <c r="AC103">
         <v>154.0470106528354</v>
@@ -45796,7 +45796,7 @@
     </row>
     <row r="104" spans="1:150">
       <c r="A104" s="1">
-        <v>34881</v>
+        <v>34926</v>
       </c>
       <c r="AD104">
         <v>154.0266905089688</v>
@@ -46164,7 +46164,7 @@
     </row>
     <row r="105" spans="1:150">
       <c r="A105" s="1">
-        <v>34973</v>
+        <v>35018</v>
       </c>
       <c r="AE105">
         <v>153.6609279193697</v>
@@ -46529,7 +46529,7 @@
     </row>
     <row r="106" spans="1:150">
       <c r="A106" s="1">
-        <v>35065</v>
+        <v>35110</v>
       </c>
       <c r="AF106">
         <v>153.2545250420373</v>
@@ -46891,7 +46891,7 @@
     </row>
     <row r="107" spans="1:150">
       <c r="A107" s="1">
-        <v>35156</v>
+        <v>35200</v>
       </c>
       <c r="AG107">
         <v>155.5710214428318</v>
@@ -47250,7 +47250,7 @@
     </row>
     <row r="108" spans="1:150">
       <c r="A108" s="1">
-        <v>35247</v>
+        <v>35292</v>
       </c>
       <c r="AH108">
         <v>156.8715106502954</v>
@@ -47606,7 +47606,7 @@
     </row>
     <row r="109" spans="1:150">
       <c r="A109" s="1">
-        <v>35339</v>
+        <v>35384</v>
       </c>
       <c r="AI109">
         <v>156.9121509380286</v>
@@ -47959,7 +47959,7 @@
     </row>
     <row r="110" spans="1:150">
       <c r="A110" s="1">
-        <v>35431</v>
+        <v>35476</v>
       </c>
       <c r="AJ110">
         <v>157.6030358294937</v>
@@ -48309,7 +48309,7 @@
     </row>
     <row r="111" spans="1:150">
       <c r="A111" s="1">
-        <v>35521</v>
+        <v>35565</v>
       </c>
       <c r="AK111">
         <v>158.436161728025</v>
@@ -48656,7 +48656,7 @@
     </row>
     <row r="112" spans="1:150">
       <c r="A112" s="1">
-        <v>35612</v>
+        <v>35657</v>
       </c>
       <c r="AL112">
         <v>159.6960106477554</v>
@@ -49000,7 +49000,7 @@
     </row>
     <row r="113" spans="1:150">
       <c r="A113" s="1">
-        <v>35704</v>
+        <v>35749</v>
       </c>
       <c r="AM113">
         <v>160.0008128057547</v>
@@ -49341,7 +49341,7 @@
     </row>
     <row r="114" spans="1:150">
       <c r="A114" s="1">
-        <v>35796</v>
+        <v>35841</v>
       </c>
       <c r="AN114">
         <v>161.5654638834843</v>
@@ -49679,7 +49679,7 @@
     </row>
     <row r="115" spans="1:150">
       <c r="A115" s="1">
-        <v>35886</v>
+        <v>35930</v>
       </c>
       <c r="AO115">
         <v>161.4029027325514</v>
@@ -50014,7 +50014,7 @@
     </row>
     <row r="116" spans="1:150">
       <c r="A116" s="1">
-        <v>35977</v>
+        <v>36022</v>
       </c>
       <c r="AP116">
         <v>162.7033919400149</v>
@@ -50346,7 +50346,7 @@
     </row>
     <row r="117" spans="1:150">
       <c r="A117" s="1">
-        <v>36069</v>
+        <v>36114</v>
       </c>
       <c r="AQ117">
         <v>161.9921869046833</v>
@@ -50675,7 +50675,7 @@
     </row>
     <row r="118" spans="1:150">
       <c r="A118" s="1">
-        <v>36161</v>
+        <v>36206</v>
       </c>
       <c r="AR118">
         <v>96.39876250323853</v>
@@ -51001,7 +51001,7 @@
     </row>
     <row r="119" spans="1:150">
       <c r="A119" s="1">
-        <v>36251</v>
+        <v>36295</v>
       </c>
       <c r="AS119">
         <v>95.93139919430629</v>
@@ -51324,7 +51324,7 @@
     </row>
     <row r="120" spans="1:150">
       <c r="A120" s="1">
-        <v>36342</v>
+        <v>36387</v>
       </c>
       <c r="AT120">
         <v>96.86612581217075</v>
@@ -51644,7 +51644,7 @@
     </row>
     <row r="121" spans="1:150">
       <c r="A121" s="1">
-        <v>36434</v>
+        <v>36479</v>
       </c>
       <c r="AU121">
         <v>97.69925171070211</v>
@@ -51961,7 +51961,7 @@
     </row>
     <row r="122" spans="1:150">
       <c r="A122" s="1">
-        <v>36526</v>
+        <v>36571</v>
       </c>
       <c r="AV122">
         <v>98.29869595476735</v>
@@ -52275,7 +52275,7 @@
     </row>
     <row r="123" spans="1:150">
       <c r="A123" s="1">
-        <v>36617</v>
+        <v>36661</v>
       </c>
       <c r="AW123">
         <v>99.51993660115113</v>
@@ -52586,7 +52586,7 @@
     </row>
     <row r="124" spans="1:150">
       <c r="A124" s="1">
-        <v>36708</v>
+        <v>36753</v>
       </c>
       <c r="AX124">
         <v>100.2108214926162</v>
@@ -52894,7 +52894,7 @@
     </row>
     <row r="125" spans="1:150">
       <c r="A125" s="1">
-        <v>36800</v>
+        <v>36845</v>
       </c>
       <c r="AY125">
         <v>100.302262140016</v>
@@ -53199,7 +53199,7 @@
     </row>
     <row r="126" spans="1:150">
       <c r="A126" s="1">
-        <v>36892</v>
+        <v>36937</v>
       </c>
       <c r="AZ126">
         <v>100.6741207727751</v>
@@ -53501,7 +53501,7 @@
     </row>
     <row r="127" spans="1:150">
       <c r="A127" s="1">
-        <v>36982</v>
+        <v>37026</v>
       </c>
       <c r="BA127">
         <v>100.8082337222948</v>
@@ -53800,7 +53800,7 @@
     </row>
     <row r="128" spans="1:150">
       <c r="A128" s="1">
-        <v>37073</v>
+        <v>37118</v>
       </c>
       <c r="BB128">
         <v>100.6659927152284</v>
@@ -54096,7 +54096,7 @@
     </row>
     <row r="129" spans="1:150">
       <c r="A129" s="1">
-        <v>37165</v>
+        <v>37210</v>
       </c>
       <c r="BC129">
         <v>100.4505991902423</v>
@@ -54389,7 +54389,7 @@
     </row>
     <row r="130" spans="1:150">
       <c r="A130" s="1">
-        <v>37257</v>
+        <v>37302</v>
       </c>
       <c r="BD130">
         <v>100.6212883987219</v>
@@ -54679,7 +54679,7 @@
     </row>
     <row r="131" spans="1:150">
       <c r="A131" s="1">
-        <v>37347</v>
+        <v>37391</v>
       </c>
       <c r="BE131">
         <v>100.9850189739343</v>
@@ -54966,7 +54966,7 @@
     </row>
     <row r="132" spans="1:150">
       <c r="A132" s="1">
-        <v>37438</v>
+        <v>37483</v>
       </c>
       <c r="BF132">
         <v>101.1333560241606</v>
@@ -55250,7 +55250,7 @@
     </row>
     <row r="133" spans="1:150">
       <c r="A133" s="1">
-        <v>37530</v>
+        <v>37575</v>
       </c>
       <c r="BG133">
         <v>101.1516441536406</v>
@@ -55531,7 +55531,7 @@
     </row>
     <row r="134" spans="1:150">
       <c r="A134" s="1">
-        <v>37622</v>
+        <v>37667</v>
       </c>
       <c r="BH134">
         <v>100.9220265279478</v>
@@ -55809,7 +55809,7 @@
     </row>
     <row r="135" spans="1:150">
       <c r="A135" s="1">
-        <v>37712</v>
+        <v>37756</v>
       </c>
       <c r="BI135">
         <v>101.0195632185076</v>
@@ -56084,7 +56084,7 @@
     </row>
     <row r="136" spans="1:150">
       <c r="A136" s="1">
-        <v>37803</v>
+        <v>37848</v>
       </c>
       <c r="BJ136">
         <v>101.1394520673206</v>
@@ -56356,7 +56356,7 @@
     </row>
     <row r="137" spans="1:150">
       <c r="A137" s="1">
-        <v>37895</v>
+        <v>37940</v>
       </c>
       <c r="BK137">
         <v>101.3365574628268</v>
@@ -56625,7 +56625,7 @@
     </row>
     <row r="138" spans="1:150">
       <c r="A138" s="1">
-        <v>37987</v>
+        <v>38032</v>
       </c>
       <c r="BL138">
         <v>101.8140808436924</v>
@@ -56891,7 +56891,7 @@
     </row>
     <row r="139" spans="1:150">
       <c r="A139" s="1">
-        <v>38078</v>
+        <v>38122</v>
       </c>
       <c r="BM139">
         <v>102.2021955915448</v>
@@ -57154,7 +57154,7 @@
     </row>
     <row r="140" spans="1:150">
       <c r="A140" s="1">
-        <v>38169</v>
+        <v>38214</v>
       </c>
       <c r="BN140">
         <v>102.2408038648914</v>
@@ -57414,7 +57414,7 @@
     </row>
     <row r="141" spans="1:150">
       <c r="A141" s="1">
-        <v>38261</v>
+        <v>38306</v>
       </c>
       <c r="BO141">
         <v>101.9258416349588</v>
@@ -57671,7 +57671,7 @@
     </row>
     <row r="142" spans="1:150">
       <c r="A142" s="1">
-        <v>38353</v>
+        <v>38398</v>
       </c>
       <c r="BP142">
         <v>103.55</v>
@@ -57925,7 +57925,7 @@
     </row>
     <row r="143" spans="1:150">
       <c r="A143" s="1">
-        <v>38443</v>
+        <v>38487</v>
       </c>
       <c r="BQ143">
         <v>103.09</v>
@@ -58176,7 +58176,7 @@
     </row>
     <row r="144" spans="1:150">
       <c r="A144" s="1">
-        <v>38534</v>
+        <v>38579</v>
       </c>
       <c r="BR144">
         <v>103.79</v>
@@ -58424,7 +58424,7 @@
     </row>
     <row r="145" spans="1:150">
       <c r="A145" s="1">
-        <v>38626</v>
+        <v>38671</v>
       </c>
       <c r="BS145">
         <v>103.9</v>
@@ -58669,7 +58669,7 @@
     </row>
     <row r="146" spans="1:150">
       <c r="A146" s="1">
-        <v>38718</v>
+        <v>38763</v>
       </c>
       <c r="BT146">
         <v>104.39</v>
@@ -58911,7 +58911,7 @@
     </row>
     <row r="147" spans="1:150">
       <c r="A147" s="1">
-        <v>38808</v>
+        <v>38852</v>
       </c>
       <c r="BU147">
         <v>105.26</v>
@@ -59150,7 +59150,7 @@
     </row>
     <row r="148" spans="1:150">
       <c r="A148" s="1">
-        <v>38899</v>
+        <v>38944</v>
       </c>
       <c r="BV148">
         <v>106.24</v>
@@ -59386,7 +59386,7 @@
     </row>
     <row r="149" spans="1:150">
       <c r="A149" s="1">
-        <v>38991</v>
+        <v>39036</v>
       </c>
       <c r="BW149">
         <v>107.48</v>
@@ -59619,7 +59619,7 @@
     </row>
     <row r="150" spans="1:150">
       <c r="A150" s="1">
-        <v>39083</v>
+        <v>39128</v>
       </c>
       <c r="BX150">
         <v>108.25</v>
@@ -59849,7 +59849,7 @@
     </row>
     <row r="151" spans="1:150">
       <c r="A151" s="1">
-        <v>39173</v>
+        <v>39217</v>
       </c>
       <c r="BY151">
         <v>108.27</v>
@@ -60076,7 +60076,7 @@
     </row>
     <row r="152" spans="1:150">
       <c r="A152" s="1">
-        <v>39264</v>
+        <v>39309</v>
       </c>
       <c r="BZ152">
         <v>109.01</v>
@@ -60300,7 +60300,7 @@
     </row>
     <row r="153" spans="1:150">
       <c r="A153" s="1">
-        <v>39356</v>
+        <v>39401</v>
       </c>
       <c r="CA153">
         <v>109.29</v>
@@ -60521,7 +60521,7 @@
     </row>
     <row r="154" spans="1:150">
       <c r="A154" s="1">
-        <v>39448</v>
+        <v>39493</v>
       </c>
       <c r="CB154">
         <v>110.96</v>
@@ -60739,7 +60739,7 @@
     </row>
     <row r="155" spans="1:150">
       <c r="A155" s="1">
-        <v>39539</v>
+        <v>39583</v>
       </c>
       <c r="CC155">
         <v>110.39</v>
@@ -60954,7 +60954,7 @@
     </row>
     <row r="156" spans="1:150">
       <c r="A156" s="1">
-        <v>39630</v>
+        <v>39675</v>
       </c>
       <c r="CD156">
         <v>110.02</v>
@@ -61166,7 +61166,7 @@
     </row>
     <row r="157" spans="1:150">
       <c r="A157" s="1">
-        <v>39722</v>
+        <v>39767</v>
       </c>
       <c r="CE157">
         <v>107.74</v>
@@ -61375,7 +61375,7 @@
     </row>
     <row r="158" spans="1:150">
       <c r="A158" s="1">
-        <v>39814</v>
+        <v>39859</v>
       </c>
       <c r="CF158">
         <v>103.52</v>
@@ -61581,7 +61581,7 @@
     </row>
     <row r="159" spans="1:150">
       <c r="A159" s="1">
-        <v>39904</v>
+        <v>39948</v>
       </c>
       <c r="CG159">
         <v>104.26</v>
@@ -61784,7 +61784,7 @@
     </row>
     <row r="160" spans="1:150">
       <c r="A160" s="1">
-        <v>39995</v>
+        <v>40040</v>
       </c>
       <c r="CH160">
         <v>105.15</v>
@@ -61984,7 +61984,7 @@
     </row>
     <row r="161" spans="1:150">
       <c r="A161" s="1">
-        <v>40087</v>
+        <v>40132</v>
       </c>
       <c r="CI161">
         <v>105.18</v>
@@ -62181,7 +62181,7 @@
     </row>
     <row r="162" spans="1:150">
       <c r="A162" s="1">
-        <v>40179</v>
+        <v>40224</v>
       </c>
       <c r="CJ162">
         <v>105.53</v>
@@ -62375,7 +62375,7 @@
     </row>
     <row r="163" spans="1:150">
       <c r="A163" s="1">
-        <v>40269</v>
+        <v>40313</v>
       </c>
       <c r="CK163">
         <v>108.64</v>
@@ -62566,7 +62566,7 @@
     </row>
     <row r="164" spans="1:150">
       <c r="A164" s="1">
-        <v>40360</v>
+        <v>40405</v>
       </c>
       <c r="CL164">
         <v>109.64</v>
@@ -62754,7 +62754,7 @@
     </row>
     <row r="165" spans="1:150">
       <c r="A165" s="1">
-        <v>40452</v>
+        <v>40497</v>
       </c>
       <c r="CM165">
         <v>110.05</v>
@@ -62939,7 +62939,7 @@
     </row>
     <row r="166" spans="1:150">
       <c r="A166" s="1">
-        <v>40544</v>
+        <v>40589</v>
       </c>
       <c r="CN166">
         <v>111.71</v>
@@ -63121,7 +63121,7 @@
     </row>
     <row r="167" spans="1:150">
       <c r="A167" s="1">
-        <v>40634</v>
+        <v>40678</v>
       </c>
       <c r="CO167">
         <v>109.17</v>
@@ -63300,7 +63300,7 @@
     </row>
     <row r="168" spans="1:150">
       <c r="A168" s="1">
-        <v>40725</v>
+        <v>40770</v>
       </c>
       <c r="CP168">
         <v>109.89</v>
@@ -63476,7 +63476,7 @@
     </row>
     <row r="169" spans="1:150">
       <c r="A169" s="1">
-        <v>40817</v>
+        <v>40862</v>
       </c>
       <c r="CQ169">
         <v>109.77</v>
@@ -63649,7 +63649,7 @@
     </row>
     <row r="170" spans="1:150">
       <c r="A170" s="1">
-        <v>40909</v>
+        <v>40954</v>
       </c>
       <c r="CR170">
         <v>110.33</v>
@@ -63819,7 +63819,7 @@
     </row>
     <row r="171" spans="1:150">
       <c r="A171" s="1">
-        <v>41000</v>
+        <v>41044</v>
       </c>
       <c r="CS171">
         <v>111.12</v>
@@ -63986,7 +63986,7 @@
     </row>
     <row r="172" spans="1:150">
       <c r="A172" s="1">
-        <v>41091</v>
+        <v>41136</v>
       </c>
       <c r="CT172">
         <v>111.38</v>
@@ -64150,7 +64150,7 @@
     </row>
     <row r="173" spans="1:150">
       <c r="A173" s="1">
-        <v>41183</v>
+        <v>41228</v>
       </c>
       <c r="CU173">
         <v>110.73</v>
@@ -64311,7 +64311,7 @@
     </row>
     <row r="174" spans="1:150">
       <c r="A174" s="1">
-        <v>41275</v>
+        <v>41320</v>
       </c>
       <c r="CV174">
         <v>110.68</v>
@@ -64469,7 +64469,7 @@
     </row>
     <row r="175" spans="1:150">
       <c r="A175" s="1">
-        <v>41365</v>
+        <v>41409</v>
       </c>
       <c r="CW175">
         <v>111.69</v>
@@ -64624,7 +64624,7 @@
     </row>
     <row r="176" spans="1:150">
       <c r="A176" s="1">
-        <v>41456</v>
+        <v>41501</v>
       </c>
       <c r="CX176">
         <v>112.05</v>
@@ -64776,7 +64776,7 @@
     </row>
     <row r="177" spans="1:150">
       <c r="A177" s="1">
-        <v>41548</v>
+        <v>41593</v>
       </c>
       <c r="CY177">
         <v>112.48</v>
@@ -64925,7 +64925,7 @@
     </row>
     <row r="178" spans="1:150">
       <c r="A178" s="1">
-        <v>41640</v>
+        <v>41685</v>
       </c>
       <c r="CZ178">
         <v>113.4</v>
@@ -65071,7 +65071,7 @@
     </row>
     <row r="179" spans="1:150">
       <c r="A179" s="1">
-        <v>41730</v>
+        <v>41774</v>
       </c>
       <c r="DA179">
         <v>105.5</v>
@@ -65214,7 +65214,7 @@
     </row>
     <row r="180" spans="1:150">
       <c r="A180" s="1">
-        <v>41821</v>
+        <v>41866</v>
       </c>
       <c r="DB180">
         <v>105.75</v>
@@ -65354,7 +65354,7 @@
     </row>
     <row r="181" spans="1:150">
       <c r="A181" s="1">
-        <v>41913</v>
+        <v>41958</v>
       </c>
       <c r="DC181">
         <v>106.5</v>
@@ -65491,7 +65491,7 @@
     </row>
     <row r="182" spans="1:150">
       <c r="A182" s="1">
-        <v>42005</v>
+        <v>42050</v>
       </c>
       <c r="DD182">
         <v>106.79</v>
@@ -65625,7 +65625,7 @@
     </row>
     <row r="183" spans="1:150">
       <c r="A183" s="1">
-        <v>42095</v>
+        <v>42139</v>
       </c>
       <c r="DE183">
         <v>107.62</v>
@@ -65756,7 +65756,7 @@
     </row>
     <row r="184" spans="1:150">
       <c r="A184" s="1">
-        <v>42186</v>
+        <v>42231</v>
       </c>
       <c r="DF184">
         <v>107.96</v>
@@ -65884,7 +65884,7 @@
     </row>
     <row r="185" spans="1:150">
       <c r="A185" s="1">
-        <v>42278</v>
+        <v>42323</v>
       </c>
       <c r="DG185">
         <v>108.22</v>
@@ -66009,7 +66009,7 @@
     </row>
     <row r="186" spans="1:150">
       <c r="A186" s="1">
-        <v>42370</v>
+        <v>42415</v>
       </c>
       <c r="DH186">
         <v>108.94</v>
@@ -66131,7 +66131,7 @@
     </row>
     <row r="187" spans="1:150">
       <c r="A187" s="1">
-        <v>42461</v>
+        <v>42505</v>
       </c>
       <c r="DI187">
         <v>109.87</v>
@@ -66250,7 +66250,7 @@
     </row>
     <row r="188" spans="1:150">
       <c r="A188" s="1">
-        <v>42552</v>
+        <v>42597</v>
       </c>
       <c r="DJ188">
         <v>110.08</v>
@@ -66366,7 +66366,7 @@
     </row>
     <row r="189" spans="1:150">
       <c r="A189" s="1">
-        <v>42644</v>
+        <v>42689</v>
       </c>
       <c r="DK189">
         <v>110.56</v>
@@ -66479,7 +66479,7 @@
     </row>
     <row r="190" spans="1:150">
       <c r="A190" s="1">
-        <v>42736</v>
+        <v>42781</v>
       </c>
       <c r="DL190">
         <v>111.25</v>
@@ -66589,7 +66589,7 @@
     </row>
     <row r="191" spans="1:150">
       <c r="A191" s="1">
-        <v>42826</v>
+        <v>42870</v>
       </c>
       <c r="DM191">
         <v>112.62</v>
@@ -66696,7 +66696,7 @@
     </row>
     <row r="192" spans="1:150">
       <c r="A192" s="1">
-        <v>42917</v>
+        <v>42962</v>
       </c>
       <c r="DN192">
         <v>113.77</v>
@@ -66800,7 +66800,7 @@
     </row>
     <row r="193" spans="1:150">
       <c r="A193" s="1">
-        <v>43009</v>
+        <v>43054</v>
       </c>
       <c r="DO193">
         <v>114.37</v>
@@ -66901,7 +66901,7 @@
     </row>
     <row r="194" spans="1:150">
       <c r="A194" s="1">
-        <v>43101</v>
+        <v>43146</v>
       </c>
       <c r="DP194">
         <v>114.71</v>
@@ -66999,7 +66999,7 @@
     </row>
     <row r="195" spans="1:150">
       <c r="A195" s="1">
-        <v>43191</v>
+        <v>43235</v>
       </c>
       <c r="DQ195">
         <v>115.67</v>
@@ -67094,7 +67094,7 @@
     </row>
     <row r="196" spans="1:150">
       <c r="A196" s="1">
-        <v>43282</v>
+        <v>43327</v>
       </c>
       <c r="DR196">
         <v>115.44</v>
@@ -67186,7 +67186,7 @@
     </row>
     <row r="197" spans="1:150">
       <c r="A197" s="1">
-        <v>43374</v>
+        <v>43419</v>
       </c>
       <c r="DS197">
         <v>115.47</v>
@@ -67275,7 +67275,7 @@
     </row>
     <row r="198" spans="1:150">
       <c r="A198" s="1">
-        <v>43466</v>
+        <v>43511</v>
       </c>
       <c r="DT198">
         <v>115.96</v>
@@ -67361,7 +67361,7 @@
     </row>
     <row r="199" spans="1:150">
       <c r="A199" s="1">
-        <v>43556</v>
+        <v>43600</v>
       </c>
       <c r="DU199">
         <v>107.03</v>
@@ -67444,7 +67444,7 @@
     </row>
     <row r="200" spans="1:150">
       <c r="A200" s="1">
-        <v>43647</v>
+        <v>43692</v>
       </c>
       <c r="DV200">
         <v>107.03</v>
@@ -67524,7 +67524,7 @@
     </row>
     <row r="201" spans="1:150">
       <c r="A201" s="1">
-        <v>43739</v>
+        <v>43784</v>
       </c>
       <c r="DW201">
         <v>107.19</v>
@@ -67601,7 +67601,7 @@
     </row>
     <row r="202" spans="1:150">
       <c r="A202" s="1">
-        <v>43831</v>
+        <v>43876</v>
       </c>
       <c r="DX202">
         <v>104.74</v>
@@ -67675,7 +67675,7 @@
     </row>
     <row r="203" spans="1:150">
       <c r="A203" s="1">
-        <v>43922</v>
+        <v>43966</v>
       </c>
       <c r="DY203">
         <v>94.68000000000001</v>
@@ -67746,7 +67746,7 @@
     </row>
     <row r="204" spans="1:150">
       <c r="A204" s="1">
-        <v>44013</v>
+        <v>44058</v>
       </c>
       <c r="DZ204">
         <v>102.72</v>
@@ -67814,7 +67814,7 @@
     </row>
     <row r="205" spans="1:150">
       <c r="A205" s="1">
-        <v>44105</v>
+        <v>44150</v>
       </c>
       <c r="EA205">
         <v>103.1</v>
@@ -67879,7 +67879,7 @@
     </row>
     <row r="206" spans="1:150">
       <c r="A206" s="1">
-        <v>44197</v>
+        <v>44242</v>
       </c>
       <c r="EB206">
         <v>101.62</v>
@@ -67941,7 +67941,7 @@
     </row>
     <row r="207" spans="1:150">
       <c r="A207" s="1">
-        <v>44287</v>
+        <v>44331</v>
       </c>
       <c r="EC207">
         <v>103.93</v>
@@ -68000,7 +68000,7 @@
     </row>
     <row r="208" spans="1:150">
       <c r="A208" s="1">
-        <v>44378</v>
+        <v>44423</v>
       </c>
       <c r="ED208">
         <v>106.24</v>
@@ -68056,7 +68056,7 @@
     </row>
     <row r="209" spans="1:150">
       <c r="A209" s="1">
-        <v>44470</v>
+        <v>44515</v>
       </c>
       <c r="EE209">
         <v>106.2</v>
@@ -68109,7 +68109,7 @@
     </row>
     <row r="210" spans="1:150">
       <c r="A210" s="1">
-        <v>44562</v>
+        <v>44607</v>
       </c>
       <c r="EF210">
         <v>106.45</v>
@@ -68159,7 +68159,7 @@
     </row>
     <row r="211" spans="1:150">
       <c r="A211" s="1">
-        <v>44652</v>
+        <v>44696</v>
       </c>
       <c r="EG211">
         <v>107.5</v>
@@ -68206,7 +68206,7 @@
     </row>
     <row r="212" spans="1:150">
       <c r="A212" s="1">
-        <v>44743</v>
+        <v>44788</v>
       </c>
       <c r="EH212">
         <v>107.89</v>
@@ -68250,7 +68250,7 @@
     </row>
     <row r="213" spans="1:150">
       <c r="A213" s="1">
-        <v>44835</v>
+        <v>44880</v>
       </c>
       <c r="EI213">
         <v>107.5</v>
@@ -68291,7 +68291,7 @@
     </row>
     <row r="214" spans="1:150">
       <c r="A214" s="1">
-        <v>44927</v>
+        <v>44972</v>
       </c>
       <c r="EJ214">
         <v>107.03</v>
@@ -68329,7 +68329,7 @@
     </row>
     <row r="215" spans="1:150">
       <c r="A215" s="1">
-        <v>45017</v>
+        <v>45061</v>
       </c>
       <c r="EK215">
         <v>107.78</v>
@@ -68364,7 +68364,7 @@
     </row>
     <row r="216" spans="1:150">
       <c r="A216" s="1">
-        <v>45108</v>
+        <v>45153</v>
       </c>
       <c r="EL216">
         <v>107.87</v>
@@ -68396,7 +68396,7 @@
     </row>
     <row r="217" spans="1:150">
       <c r="A217" s="1">
-        <v>45200</v>
+        <v>45245</v>
       </c>
       <c r="EM217">
         <v>107.68</v>
@@ -68425,7 +68425,7 @@
     </row>
     <row r="218" spans="1:150">
       <c r="A218" s="1">
-        <v>45292</v>
+        <v>45337</v>
       </c>
       <c r="EN218">
         <v>107.91</v>
@@ -68451,7 +68451,7 @@
     </row>
     <row r="219" spans="1:150">
       <c r="A219" s="1">
-        <v>45383</v>
+        <v>45427</v>
       </c>
       <c r="EO219">
         <v>104.78</v>
@@ -68474,7 +68474,7 @@
     </row>
     <row r="220" spans="1:150">
       <c r="A220" s="1">
-        <v>45474</v>
+        <v>45519</v>
       </c>
       <c r="EP220">
         <v>104.66</v>
@@ -68494,7 +68494,7 @@
     </row>
     <row r="221" spans="1:150">
       <c r="A221" s="1">
-        <v>45566</v>
+        <v>45611</v>
       </c>
       <c r="EQ221">
         <v>104.45</v>
@@ -68511,7 +68511,7 @@
     </row>
     <row r="222" spans="1:150">
       <c r="A222" s="1">
-        <v>45658</v>
+        <v>45703</v>
       </c>
       <c r="ER222">
         <v>104.88</v>
@@ -68525,7 +68525,7 @@
     </row>
     <row r="223" spans="1:150">
       <c r="A223" s="1">
-        <v>45748</v>
+        <v>45792</v>
       </c>
       <c r="ES223">
         <v>104.52</v>
@@ -68536,7 +68536,7 @@
     </row>
     <row r="224" spans="1:150">
       <c r="A224" s="1">
-        <v>45839</v>
+        <v>45884</v>
       </c>
       <c r="ET224">
         <v>104.59</v>
@@ -68544,7 +68544,7 @@
     </row>
     <row r="225" spans="1:1">
       <c r="A225" s="1">
-        <v>45931</v>
+        <v>45976</v>
       </c>
     </row>
   </sheetData>

</xml_diff>